<commit_message>
fix typo in excel file for blending reservoir and rerun automation script
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F522AED-EDCD-44EF-8D5A-B95E7ECCD121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34F3EBB-410F-41B4-9902-8823C6DBDBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>blending resevoir</t>
   </si>
   <si>
-    <t>blending_resevoir_zo</t>
-  </si>
-  <si>
     <t>PT</t>
   </si>
   <si>
@@ -1166,6 +1163,9 @@
   </si>
   <si>
     <t>ozone_aop_zo</t>
+  </si>
+  <si>
+    <t>blending_reservoir_zo</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1577,7 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1825,13 +1825,13 @@
         <v>29</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>377</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>12</v>
@@ -1851,22 +1851,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1879,16 +1879,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>12</v>
@@ -1908,22 +1908,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1936,10 +1936,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -1965,22 +1965,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1993,13 +1993,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>28</v>
@@ -2008,7 +2008,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
@@ -2050,16 +2050,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>12</v>
@@ -2079,22 +2079,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2107,16 +2107,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>12</v>
@@ -2136,19 +2136,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="3" t="b">
         <f t="shared" si="0"/>
@@ -2165,10 +2165,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>
@@ -2194,16 +2194,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>12</v>
@@ -2223,13 +2223,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>11</v>
@@ -2238,7 +2238,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G23" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2251,10 +2251,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
@@ -2280,22 +2280,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
@@ -2337,13 +2337,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>20</v>
@@ -2352,7 +2352,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G27" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2365,10 +2365,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>10</v>
@@ -2394,10 +2394,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -2406,10 +2406,10 @@
         <v>20</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2422,22 +2422,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2450,16 +2450,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>12</v>
@@ -2479,13 +2479,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>11</v>
@@ -2494,7 +2494,7 @@
         <v>12</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2507,16 +2507,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>12</v>
@@ -2536,49 +2536,49 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="3" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="H34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G35" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2591,13 +2591,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>28</v>
@@ -2606,7 +2606,7 @@
         <v>12</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2619,22 +2619,22 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="C37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G37" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2647,16 +2647,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>23</v>
@@ -2666,24 +2666,24 @@
         <v>0</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>12</v>
@@ -2703,16 +2703,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>12</v>
@@ -2732,13 +2732,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>11</v>
@@ -2747,7 +2747,7 @@
         <v>23</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G41" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2760,22 +2760,22 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="C42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G42" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2788,22 +2788,22 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G43" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2816,10 +2816,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>19</v>
@@ -2831,7 +2831,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>10</v>
@@ -2873,10 +2873,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>10</v>
@@ -2902,10 +2902,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>19</v>
@@ -2914,10 +2914,10 @@
         <v>20</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>10</v>
@@ -2959,10 +2959,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>10</v>
@@ -2988,22 +2988,22 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="C50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3016,16 +3016,16 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>12</v>
@@ -3045,22 +3045,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="C52" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3073,22 +3073,22 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3101,22 +3101,22 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="C54" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G54" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3129,10 +3129,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>19</v>
@@ -3141,10 +3141,10 @@
         <v>11</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G55" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3157,10 +3157,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>10</v>
@@ -3186,22 +3186,22 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="G57" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3214,16 +3214,16 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>12</v>
@@ -3243,10 +3243,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>10</v>
@@ -3272,13 +3272,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="C60" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>11</v>
@@ -3287,7 +3287,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G60" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3300,13 +3300,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="C61" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>11</v>
@@ -3315,7 +3315,7 @@
         <v>12</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G61" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3328,10 +3328,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>10</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>10</v>
@@ -3386,16 +3386,16 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>12</v>
@@ -3415,16 +3415,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>12</v>
@@ -3444,22 +3444,22 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="C66" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G66" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3472,22 +3472,22 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="C67" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G67" s="3" t="str">
         <f t="shared" ref="G67:G78" si="3">IF(D67="SIDO","single-input, double-output",IF(D67="SISO","single-input, single-output",IF(D67="PT","pass-through",IF(D67="DISO","double-input, single-output",IF(D67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3500,16 +3500,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>23</v>
@@ -3529,16 +3529,16 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>12</v>
@@ -3558,10 +3558,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>10</v>
@@ -3587,10 +3587,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>10</v>
@@ -3616,13 +3616,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="C72" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>28</v>
@@ -3631,7 +3631,7 @@
         <v>12</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G72" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3644,13 +3644,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="C73" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>28</v>
@@ -3659,7 +3659,7 @@
         <v>12</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G73" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3672,13 +3672,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="C74" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>11</v>
@@ -3701,10 +3701,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>10</v>
@@ -3730,10 +3730,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>10</v>
@@ -3759,22 +3759,22 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="C77" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="F77" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G77" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3787,22 +3787,22 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C78" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="G78" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3836,17 +3836,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE(A1,"_zo")</f>
         <v>aeration_basin_zo</v>
       </c>
       <c r="C1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
         <v>207</v>
-      </c>
-      <c r="D1" t="s">
-        <v>208</v>
       </c>
       <c r="G1" t="str">
         <f>CONCATENATE(C1," ",D1)</f>
@@ -3855,17 +3855,17 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B65" si="0">CONCATENATE(A2,"_zo")</f>
         <v>air_flotation_zo</v>
       </c>
       <c r="C2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" t="s">
         <v>210</v>
-      </c>
-      <c r="D2" t="s">
-        <v>211</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" si="1">CONCATENATE(C2," ",D2)</f>
@@ -3874,20 +3874,20 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_digestion_oxidation_zo</v>
+      </c>
+      <c r="C3" t="s">
         <v>212</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_digestion_oxidation_zo</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>213</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>214</v>
-      </c>
-      <c r="E3" t="s">
-        <v>215</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="1"/>
@@ -3896,20 +3896,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_mbr_mec_zo</v>
+      </c>
+      <c r="C4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" t="s">
         <v>216</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_mbr_mec_zo</v>
-      </c>
-      <c r="C4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>217</v>
-      </c>
-      <c r="E4" t="s">
-        <v>218</v>
       </c>
       <c r="G4" t="str">
         <f>CONCATENATE(C4," ",D4," ",E4)</f>
@@ -3918,20 +3918,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>backwash_solids_handling_zo</v>
+      </c>
+      <c r="C5" t="s">
         <v>219</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>backwash_solids_handling_zo</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>220</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>221</v>
-      </c>
-      <c r="E5" t="s">
-        <v>222</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ref="G5:G6" si="2">CONCATENATE(C5," ",D5," ",E5)</f>
@@ -3940,20 +3940,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>bio_active_filtration_zo</v>
+      </c>
+      <c r="C6" t="s">
         <v>223</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>bio_active_filtration_zo</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>224</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>225</v>
-      </c>
-      <c r="E6" t="s">
-        <v>226</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
@@ -3962,14 +3962,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>bioreactor_zo</v>
       </c>
       <c r="C7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -3978,17 +3978,17 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>blending_resevoir_zo</v>
+      </c>
+      <c r="C8" t="s">
         <v>228</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>blending_resevoir_zo</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>229</v>
-      </c>
-      <c r="D8" t="s">
-        <v>230</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
@@ -3997,17 +3997,17 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>brine_concentrator_zo</v>
+      </c>
+      <c r="C9" t="s">
         <v>231</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>brine_concentrator_zo</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>232</v>
-      </c>
-      <c r="D9" t="s">
-        <v>233</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -4016,17 +4016,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>buffer_tank_zo</v>
+      </c>
+      <c r="C10" t="s">
         <v>234</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>buffer_tank_zo</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>235</v>
-      </c>
-      <c r="D10" t="s">
-        <v>236</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -4035,14 +4035,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>CANDOP_zo</v>
       </c>
       <c r="C11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -4051,17 +4051,17 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>cartridge_filtration_zo</v>
+      </c>
+      <c r="C12" t="s">
         <v>238</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>cartridge_filtration_zo</v>
-      </c>
-      <c r="C12" t="s">
-        <v>239</v>
-      </c>
       <c r="D12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -4070,17 +4070,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>chemical_addition_zo</v>
+      </c>
+      <c r="C13" t="s">
         <v>240</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>chemical_addition_zo</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>241</v>
-      </c>
-      <c r="D13" t="s">
-        <v>242</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -4089,14 +4089,14 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>chlorination_zo</v>
       </c>
       <c r="C14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -4105,14 +4105,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>clarifier_zo</v>
       </c>
       <c r="C15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -4121,17 +4121,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>co2_addition_zo</v>
+      </c>
+      <c r="C16" t="s">
         <v>245</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>co2_addition_zo</v>
-      </c>
-      <c r="C16" t="s">
-        <v>246</v>
-      </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -4140,20 +4140,20 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>coag_and_floc_zo</v>
+      </c>
+      <c r="C17" t="s">
         <v>247</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>coag_and_floc_zo</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>248</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>249</v>
-      </c>
-      <c r="E17" t="s">
-        <v>250</v>
       </c>
       <c r="G17" t="str">
         <f>CONCATENATE(C17," ",D17," ",E17)</f>
@@ -4162,14 +4162,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>cofermentation_zo</v>
       </c>
       <c r="C18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ref="G18:G19" si="3">CONCATENATE(C18," ",D18," ",E18)</f>
@@ -4178,17 +4178,17 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>constructed_wetlands_zo</v>
+      </c>
+      <c r="C19" t="s">
         <v>252</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>constructed_wetlands_zo</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>253</v>
-      </c>
-      <c r="D19" t="s">
-        <v>254</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="3"/>
@@ -4197,20 +4197,20 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>conventional_activated_sludge_zo</v>
+      </c>
+      <c r="C20" t="s">
         <v>255</v>
       </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>conventional_activated_sludge_zo</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>256</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>257</v>
-      </c>
-      <c r="E20" t="s">
-        <v>258</v>
       </c>
       <c r="G20" t="str">
         <f>CONCATENATE(C20," ",D20," ",E20)</f>
@@ -4219,17 +4219,17 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>cooling_supply_zo</v>
+      </c>
+      <c r="C21" t="s">
         <v>259</v>
       </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>cooling_supply_zo</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>260</v>
-      </c>
-      <c r="D21" t="s">
-        <v>261</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ref="G21:G22" si="4">CONCATENATE(C21," ",D21," ",E21)</f>
@@ -4238,17 +4238,17 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>cooling_tower_zo</v>
+      </c>
+      <c r="C22" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" t="s">
         <v>262</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>cooling_tower_zo</v>
-      </c>
-      <c r="C22" t="s">
-        <v>260</v>
-      </c>
-      <c r="D22" t="s">
-        <v>263</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="4"/>
@@ -4257,14 +4257,14 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>decarbonator_zo</v>
       </c>
       <c r="C23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -4273,20 +4273,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>deep_well_injection_zo</v>
+      </c>
+      <c r="C24" t="s">
         <v>265</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>deep_well_injection_zo</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>266</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>267</v>
-      </c>
-      <c r="E24" t="s">
-        <v>268</v>
       </c>
       <c r="G24" t="str">
         <f>CONCATENATE(C24," ",D24," ",E24)</f>
@@ -4295,20 +4295,20 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>dissolved_air_flotation_zo</v>
+      </c>
+      <c r="C25" t="s">
         <v>269</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>dissolved_air_flotation_zo</v>
-      </c>
-      <c r="C25" t="s">
-        <v>270</v>
-      </c>
       <c r="D25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E25" t="s">
         <v>210</v>
-      </c>
-      <c r="E25" t="s">
-        <v>211</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ref="G25" si="5">CONCATENATE(C25," ",D25," ",E25)</f>
@@ -4317,14 +4317,14 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>dmbr_zo</v>
       </c>
       <c r="C26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G26" t="str">
         <f>CONCATENATE(C26," ",D26)</f>
@@ -4333,20 +4333,20 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>dual_media_filtration_zo</v>
+      </c>
+      <c r="C27" t="s">
         <v>272</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>dual_media_filtration_zo</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>273</v>
       </c>
-      <c r="D27" t="s">
-        <v>274</v>
-      </c>
       <c r="E27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G27" t="str">
         <f>CONCATENATE(C27," ",D27," ",E27)</f>
@@ -4355,20 +4355,20 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>electrochemical_nutrient_removal_zo</v>
+      </c>
+      <c r="C28" t="s">
         <v>275</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>electrochemical_nutrient_removal_zo</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>276</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>277</v>
-      </c>
-      <c r="E28" t="s">
-        <v>278</v>
       </c>
       <c r="G28" t="str">
         <f>CONCATENATE(C28," ",D28," ",E28)</f>
@@ -4377,17 +4377,17 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>electrodialysis_reversal_zo</v>
+      </c>
+      <c r="C29" t="s">
         <v>279</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>electrodialysis_reversal_zo</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>280</v>
-      </c>
-      <c r="D29" t="s">
-        <v>281</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -4406,7 +4406,7 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -4415,17 +4415,17 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>evaporation_pond_zo</v>
+      </c>
+      <c r="C31" t="s">
         <v>284</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>evaporation_pond_zo</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>285</v>
-      </c>
-      <c r="D31" t="s">
-        <v>286</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -4434,20 +4434,20 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>feed_water_tank_zo</v>
+      </c>
+      <c r="C32" t="s">
         <v>287</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>feed_water_tank_zo</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>288</v>
       </c>
-      <c r="D32" t="s">
-        <v>289</v>
-      </c>
       <c r="E32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G32" t="str">
         <f>CONCATENATE(C32," ",D32," ",E32)</f>
@@ -4456,14 +4456,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>feed_zo</v>
       </c>
       <c r="C33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -4472,17 +4472,17 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>filter_press_zo</v>
+      </c>
+      <c r="C34" t="s">
         <v>290</v>
       </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>filter_press_zo</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>291</v>
-      </c>
-      <c r="D34" t="s">
-        <v>292</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -4491,17 +4491,17 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>fixed_bed_zo</v>
+      </c>
+      <c r="C35" t="s">
         <v>293</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>fixed_bed_zo</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>294</v>
-      </c>
-      <c r="D35" t="s">
-        <v>295</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -4510,14 +4510,14 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>gac_zo</v>
       </c>
       <c r="C36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -4526,20 +4526,20 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>gas_sparged_membrane_zo</v>
+      </c>
+      <c r="C37" t="s">
         <v>297</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>gas_sparged_membrane_zo</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>298</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>299</v>
-      </c>
-      <c r="E37" t="s">
-        <v>300</v>
       </c>
       <c r="G37" t="str">
         <f>CONCATENATE(C37," ",D37," ",E37)</f>
@@ -4548,20 +4548,20 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>injection_well_disposal_zo</v>
+      </c>
+      <c r="C38" t="s">
+        <v>267</v>
+      </c>
+      <c r="D38" t="s">
+        <v>266</v>
+      </c>
+      <c r="E38" t="s">
         <v>301</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>injection_well_disposal_zo</v>
-      </c>
-      <c r="C38" t="s">
-        <v>268</v>
-      </c>
-      <c r="D38" t="s">
-        <v>267</v>
-      </c>
-      <c r="E38" t="s">
-        <v>302</v>
       </c>
       <c r="G38" t="str">
         <f>CONCATENATE(C38," ",D38," ",E38)</f>
@@ -4570,17 +4570,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>intrusion_mitigation_zo</v>
+      </c>
+      <c r="C39" t="s">
         <v>303</v>
       </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>intrusion_mitigation_zo</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>304</v>
-      </c>
-      <c r="D39" t="s">
-        <v>305</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -4589,17 +4589,17 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>ion_exchange_zo</v>
+      </c>
+      <c r="C40" t="s">
         <v>306</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>ion_exchange_zo</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>307</v>
-      </c>
-      <c r="D40" t="s">
-        <v>308</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -4608,23 +4608,23 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>iron_and_manganese_removal_zo</v>
+      </c>
+      <c r="C41" t="s">
         <v>309</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>iron_and_manganese_removal_zo</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" t="s">
         <v>310</v>
       </c>
-      <c r="D41" t="s">
-        <v>249</v>
-      </c>
-      <c r="E41" t="s">
-        <v>311</v>
-      </c>
       <c r="F41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G41" t="str">
         <f>CONCATENATE(C41," ",D41," ",E41," ",F41)</f>
@@ -4633,14 +4633,14 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>landfill_zo</v>
       </c>
       <c r="C42" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -4649,14 +4649,14 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>mabr_zo</v>
       </c>
       <c r="C43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -4665,14 +4665,14 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>mbr_zo</v>
       </c>
       <c r="C44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -4681,17 +4681,17 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>media_filtration_zo</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -4700,14 +4700,14 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>metab_zo</v>
       </c>
       <c r="C46" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -4716,14 +4716,14 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>microfiltration_zo</v>
       </c>
       <c r="C47" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -4732,17 +4732,17 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>microscreen_filtration_zo</v>
+      </c>
+      <c r="C48" t="s">
         <v>317</v>
       </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>microscreen_filtration_zo</v>
-      </c>
-      <c r="C48" t="s">
-        <v>318</v>
-      </c>
       <c r="D48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -4751,17 +4751,17 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>municipal_drinking_zo</v>
+      </c>
+      <c r="C49" t="s">
         <v>319</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>municipal_drinking_zo</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>320</v>
-      </c>
-      <c r="D49" t="s">
-        <v>321</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -4770,17 +4770,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>municipal_wwtp_zo</v>
+      </c>
+      <c r="C50" t="s">
+        <v>319</v>
+      </c>
+      <c r="D50" t="s">
         <v>322</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>municipal_wwtp_zo</v>
-      </c>
-      <c r="C50" t="s">
-        <v>320</v>
-      </c>
-      <c r="D50" t="s">
-        <v>323</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -4789,14 +4789,14 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>nanofiltration_zo</v>
       </c>
       <c r="C51" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -4805,17 +4805,17 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>ozone_aop _zo</v>
+      </c>
+      <c r="C52" t="s">
         <v>325</v>
       </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>ozone_aop _zo</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>326</v>
-      </c>
-      <c r="D52" t="s">
-        <v>327</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -4824,14 +4824,14 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>ozone_zo</v>
       </c>
       <c r="C53" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -4840,17 +4840,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>photothermal_membrane_zo</v>
+      </c>
+      <c r="C54" t="s">
         <v>328</v>
       </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>photothermal_membrane_zo</v>
-      </c>
-      <c r="C54" t="s">
-        <v>329</v>
-      </c>
       <c r="D54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -4859,17 +4859,17 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>primary_separator_zo</v>
+      </c>
+      <c r="C55" t="s">
         <v>330</v>
       </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>primary_separator_zo</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>331</v>
-      </c>
-      <c r="D55" t="s">
-        <v>332</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -4885,10 +4885,10 @@
         <v>pump_electricity_zo</v>
       </c>
       <c r="C56" t="s">
+        <v>332</v>
+      </c>
+      <c r="D56" t="s">
         <v>333</v>
-      </c>
-      <c r="D56" t="s">
-        <v>334</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
@@ -4897,14 +4897,14 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
         <v>pump_zo</v>
       </c>
       <c r="C57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -4913,14 +4913,14 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
         <v>screen_zo</v>
       </c>
       <c r="C58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -4929,20 +4929,20 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>secondary_treatment_wwtp_zo</v>
+      </c>
+      <c r="C59" t="s">
         <v>336</v>
       </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>secondary_treatment_wwtp_zo</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>337</v>
       </c>
-      <c r="D59" t="s">
-        <v>338</v>
-      </c>
       <c r="E59" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G59" t="str">
         <f>CONCATENATE(C59," ",D59," ",E59)</f>
@@ -4951,14 +4951,14 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
         <v>sedimentation_zo</v>
       </c>
       <c r="C60" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -4967,17 +4967,17 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>settling_pond_zo</v>
+      </c>
+      <c r="C61" t="s">
         <v>340</v>
       </c>
-      <c r="B61" t="str">
-        <f t="shared" si="0"/>
-        <v>settling_pond_zo</v>
-      </c>
-      <c r="C61" t="s">
-        <v>341</v>
-      </c>
       <c r="D61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -4986,17 +4986,17 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
         <v>sludge_tank_zo</v>
       </c>
       <c r="C62" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D62" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -5005,14 +5005,14 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
         <v>smp_zo</v>
       </c>
       <c r="C63" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -5021,17 +5021,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>static_mixer_zo</v>
+      </c>
+      <c r="C64" t="s">
         <v>344</v>
       </c>
-      <c r="B64" t="str">
-        <f t="shared" si="0"/>
-        <v>static_mixer_zo</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>345</v>
-      </c>
-      <c r="D64" t="s">
-        <v>346</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -5040,17 +5040,17 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>storage_tank_zo</v>
+      </c>
+      <c r="C65" t="s">
         <v>347</v>
       </c>
-      <c r="B65" t="str">
-        <f t="shared" si="0"/>
-        <v>storage_tank_zo</v>
-      </c>
-      <c r="C65" t="s">
-        <v>348</v>
-      </c>
       <c r="D65" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -5059,17 +5059,17 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" ref="B66:B77" si="6">CONCATENATE(A66,"_zo")</f>
         <v>surface_discharge_zo</v>
       </c>
       <c r="C66" t="s">
+        <v>349</v>
+      </c>
+      <c r="D66" t="s">
         <v>350</v>
-      </c>
-      <c r="D66" t="s">
-        <v>351</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G77" si="7">CONCATENATE(C66," ",D66)</f>
@@ -5078,20 +5078,20 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="6"/>
         <v>sw_onshore_intake_zo</v>
       </c>
       <c r="C67" t="s">
+        <v>352</v>
+      </c>
+      <c r="D67" t="s">
         <v>353</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>354</v>
-      </c>
-      <c r="E67" t="s">
-        <v>355</v>
       </c>
       <c r="G67" t="str">
         <f>CONCATENATE(C67," ",D67," ",E67)</f>
@@ -5100,20 +5100,20 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="6"/>
         <v>tramp_oil_tank_zo</v>
       </c>
       <c r="C68" t="s">
+        <v>356</v>
+      </c>
+      <c r="D68" t="s">
         <v>357</v>
       </c>
-      <c r="D68" t="s">
-        <v>358</v>
-      </c>
       <c r="E68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" ref="G68:G69" si="8">CONCATENATE(C68," ",D68," ",E68)</f>
@@ -5122,20 +5122,20 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="6"/>
         <v>tri_media_filtration_zo</v>
       </c>
       <c r="C69" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D69" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="8"/>
@@ -5144,17 +5144,17 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="6"/>
         <v>ultra_filtration_zo</v>
       </c>
       <c r="C70" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="7"/>
@@ -5163,17 +5163,17 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="6"/>
         <v>uv_aop_zo</v>
       </c>
       <c r="C71" t="s">
+        <v>363</v>
+      </c>
+      <c r="D71" t="s">
         <v>364</v>
-      </c>
-      <c r="D71" t="s">
-        <v>365</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="7"/>
@@ -5182,14 +5182,14 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="6"/>
         <v>uv_zo</v>
       </c>
       <c r="C72" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="7"/>
@@ -5198,17 +5198,17 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="6"/>
         <v>vfa_recovery_zo</v>
       </c>
       <c r="C73" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D73" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="7"/>
@@ -5217,14 +5217,14 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="6"/>
         <v>waiv_zo</v>
       </c>
       <c r="C74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="7"/>
@@ -5233,20 +5233,20 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="6"/>
         <v>walnut_shell_filter_zo</v>
       </c>
       <c r="C75" t="s">
+        <v>369</v>
+      </c>
+      <c r="D75" t="s">
         <v>370</v>
       </c>
-      <c r="D75" t="s">
-        <v>371</v>
-      </c>
       <c r="E75" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ref="G75:G76" si="9">CONCATENATE(C75," ",D75," ",E75)</f>
@@ -5255,20 +5255,20 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="6"/>
         <v>water_pumping_station_zo</v>
       </c>
       <c r="C76" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D76" t="s">
+        <v>372</v>
+      </c>
+      <c r="E76" t="s">
         <v>373</v>
-      </c>
-      <c r="E76" t="s">
-        <v>374</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="9"/>
@@ -5277,17 +5277,17 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="6"/>
         <v>well_field_zo</v>
       </c>
       <c r="C77" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D77" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
correcting the other typo on blending res
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34F3EBB-410F-41B4-9902-8823C6DBDBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AD6B36-2DD8-4668-8E1E-D2B182143B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>SISO</t>
   </si>
   <si>
-    <t>blending resevoir</t>
-  </si>
-  <si>
     <t>PT</t>
   </si>
   <si>
@@ -1166,6 +1163,9 @@
   </si>
   <si>
     <t>blending_reservoir_zo</t>
+  </si>
+  <si>
+    <t>blending reservoir</t>
   </si>
 </sst>
 </file>
@@ -1576,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1822,16 +1822,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>377</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>12</v>
@@ -1851,22 +1851,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1879,16 +1879,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>12</v>
@@ -1908,22 +1908,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1936,10 +1936,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -1965,22 +1965,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1993,13 +1993,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>28</v>
@@ -2008,7 +2008,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
@@ -2050,16 +2050,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>12</v>
@@ -2079,22 +2079,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2107,16 +2107,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>12</v>
@@ -2136,19 +2136,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" s="3" t="b">
         <f t="shared" si="0"/>
@@ -2165,10 +2165,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>
@@ -2194,16 +2194,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>12</v>
@@ -2223,13 +2223,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>11</v>
@@ -2238,7 +2238,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2251,10 +2251,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
@@ -2280,22 +2280,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
@@ -2337,13 +2337,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>20</v>
@@ -2352,7 +2352,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G27" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2365,10 +2365,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>10</v>
@@ -2394,10 +2394,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>19</v>
@@ -2406,10 +2406,10 @@
         <v>20</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G29" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2422,22 +2422,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2450,16 +2450,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>12</v>
@@ -2479,13 +2479,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>11</v>
@@ -2494,7 +2494,7 @@
         <v>12</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2507,16 +2507,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>12</v>
@@ -2536,49 +2536,49 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="3" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="H34" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G35" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2591,13 +2591,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="C36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>28</v>
@@ -2606,7 +2606,7 @@
         <v>12</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2619,22 +2619,22 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="C37" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G37" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2647,16 +2647,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>23</v>
@@ -2666,24 +2666,24 @@
         <v>0</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>12</v>
@@ -2703,16 +2703,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>12</v>
@@ -2732,13 +2732,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>11</v>
@@ -2747,7 +2747,7 @@
         <v>23</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G41" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2760,22 +2760,22 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G42" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2788,22 +2788,22 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G43" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2816,10 +2816,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>19</v>
@@ -2831,7 +2831,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>10</v>
@@ -2873,10 +2873,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>10</v>
@@ -2902,10 +2902,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>19</v>
@@ -2914,10 +2914,10 @@
         <v>20</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>10</v>
@@ -2959,10 +2959,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>10</v>
@@ -2988,22 +2988,22 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="C50" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3016,16 +3016,16 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>12</v>
@@ -3045,22 +3045,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="C52" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3073,22 +3073,22 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3101,22 +3101,22 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="C54" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G54" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3129,10 +3129,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>19</v>
@@ -3141,10 +3141,10 @@
         <v>11</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G55" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3157,10 +3157,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>10</v>
@@ -3186,22 +3186,22 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="G57" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3214,16 +3214,16 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>12</v>
@@ -3243,10 +3243,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>10</v>
@@ -3272,13 +3272,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C60" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>11</v>
@@ -3287,7 +3287,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G60" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3300,13 +3300,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="C61" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>11</v>
@@ -3315,7 +3315,7 @@
         <v>12</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G61" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3328,10 +3328,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>10</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>10</v>
@@ -3386,16 +3386,16 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>12</v>
@@ -3415,16 +3415,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>12</v>
@@ -3444,22 +3444,22 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="C66" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G66" s="3" t="str">
         <f t="shared" si="1"/>
@@ -3472,22 +3472,22 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="C67" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G67" s="3" t="str">
         <f t="shared" ref="G67:G78" si="3">IF(D67="SIDO","single-input, double-output",IF(D67="SISO","single-input, single-output",IF(D67="PT","pass-through",IF(D67="DISO","double-input, single-output",IF(D67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3500,16 +3500,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>23</v>
@@ -3529,16 +3529,16 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>12</v>
@@ -3558,10 +3558,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>10</v>
@@ -3587,10 +3587,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>10</v>
@@ -3616,13 +3616,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="C72" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>28</v>
@@ -3631,7 +3631,7 @@
         <v>12</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G72" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3644,13 +3644,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="C73" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>28</v>
@@ -3659,7 +3659,7 @@
         <v>12</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G73" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3672,13 +3672,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="C74" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>11</v>
@@ -3701,10 +3701,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>10</v>
@@ -3730,10 +3730,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>10</v>
@@ -3759,22 +3759,22 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="C77" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F77" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G77" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3787,22 +3787,22 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C78" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="G78" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3836,17 +3836,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE(A1,"_zo")</f>
         <v>aeration_basin_zo</v>
       </c>
       <c r="C1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" t="s">
         <v>206</v>
-      </c>
-      <c r="D1" t="s">
-        <v>207</v>
       </c>
       <c r="G1" t="str">
         <f>CONCATENATE(C1," ",D1)</f>
@@ -3855,17 +3855,17 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B65" si="0">CONCATENATE(A2,"_zo")</f>
         <v>air_flotation_zo</v>
       </c>
       <c r="C2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" t="s">
         <v>209</v>
-      </c>
-      <c r="D2" t="s">
-        <v>210</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" si="1">CONCATENATE(C2," ",D2)</f>
@@ -3874,20 +3874,20 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_digestion_oxidation_zo</v>
+      </c>
+      <c r="C3" t="s">
         <v>211</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_digestion_oxidation_zo</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>212</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>213</v>
-      </c>
-      <c r="E3" t="s">
-        <v>214</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="1"/>
@@ -3896,20 +3896,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_mbr_mec_zo</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
         <v>215</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_mbr_mec_zo</v>
-      </c>
-      <c r="C4" t="s">
-        <v>212</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>216</v>
-      </c>
-      <c r="E4" t="s">
-        <v>217</v>
       </c>
       <c r="G4" t="str">
         <f>CONCATENATE(C4," ",D4," ",E4)</f>
@@ -3918,20 +3918,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>backwash_solids_handling_zo</v>
+      </c>
+      <c r="C5" t="s">
         <v>218</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>backwash_solids_handling_zo</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>219</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>220</v>
-      </c>
-      <c r="E5" t="s">
-        <v>221</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ref="G5:G6" si="2">CONCATENATE(C5," ",D5," ",E5)</f>
@@ -3940,20 +3940,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>bio_active_filtration_zo</v>
+      </c>
+      <c r="C6" t="s">
         <v>222</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>bio_active_filtration_zo</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>223</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>224</v>
-      </c>
-      <c r="E6" t="s">
-        <v>225</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
@@ -3962,14 +3962,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>bioreactor_zo</v>
       </c>
       <c r="C7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -3978,17 +3978,17 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>blending_resevoir_zo</v>
+      </c>
+      <c r="C8" t="s">
         <v>227</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>blending_resevoir_zo</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>228</v>
-      </c>
-      <c r="D8" t="s">
-        <v>229</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
@@ -3997,17 +3997,17 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>brine_concentrator_zo</v>
+      </c>
+      <c r="C9" t="s">
         <v>230</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>brine_concentrator_zo</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>231</v>
-      </c>
-      <c r="D9" t="s">
-        <v>232</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -4016,17 +4016,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>buffer_tank_zo</v>
+      </c>
+      <c r="C10" t="s">
         <v>233</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>buffer_tank_zo</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>234</v>
-      </c>
-      <c r="D10" t="s">
-        <v>235</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -4035,14 +4035,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>CANDOP_zo</v>
       </c>
       <c r="C11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -4051,17 +4051,17 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>cartridge_filtration_zo</v>
+      </c>
+      <c r="C12" t="s">
         <v>237</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>cartridge_filtration_zo</v>
-      </c>
-      <c r="C12" t="s">
-        <v>238</v>
-      </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -4070,17 +4070,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>chemical_addition_zo</v>
+      </c>
+      <c r="C13" t="s">
         <v>239</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>chemical_addition_zo</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>240</v>
-      </c>
-      <c r="D13" t="s">
-        <v>241</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -4089,14 +4089,14 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>chlorination_zo</v>
       </c>
       <c r="C14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -4105,14 +4105,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>clarifier_zo</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -4121,17 +4121,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>co2_addition_zo</v>
+      </c>
+      <c r="C16" t="s">
         <v>244</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>co2_addition_zo</v>
-      </c>
-      <c r="C16" t="s">
-        <v>245</v>
-      </c>
       <c r="D16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -4140,20 +4140,20 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>coag_and_floc_zo</v>
+      </c>
+      <c r="C17" t="s">
         <v>246</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>coag_and_floc_zo</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>247</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>248</v>
-      </c>
-      <c r="E17" t="s">
-        <v>249</v>
       </c>
       <c r="G17" t="str">
         <f>CONCATENATE(C17," ",D17," ",E17)</f>
@@ -4162,14 +4162,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>cofermentation_zo</v>
       </c>
       <c r="C18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ref="G18:G19" si="3">CONCATENATE(C18," ",D18," ",E18)</f>
@@ -4178,17 +4178,17 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>constructed_wetlands_zo</v>
+      </c>
+      <c r="C19" t="s">
         <v>251</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>constructed_wetlands_zo</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>252</v>
-      </c>
-      <c r="D19" t="s">
-        <v>253</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="3"/>
@@ -4197,20 +4197,20 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>conventional_activated_sludge_zo</v>
+      </c>
+      <c r="C20" t="s">
         <v>254</v>
       </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>conventional_activated_sludge_zo</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>255</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>256</v>
-      </c>
-      <c r="E20" t="s">
-        <v>257</v>
       </c>
       <c r="G20" t="str">
         <f>CONCATENATE(C20," ",D20," ",E20)</f>
@@ -4219,17 +4219,17 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>cooling_supply_zo</v>
+      </c>
+      <c r="C21" t="s">
         <v>258</v>
       </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>cooling_supply_zo</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>259</v>
-      </c>
-      <c r="D21" t="s">
-        <v>260</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ref="G21:G22" si="4">CONCATENATE(C21," ",D21," ",E21)</f>
@@ -4238,17 +4238,17 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>cooling_tower_zo</v>
+      </c>
+      <c r="C22" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" t="s">
         <v>261</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>cooling_tower_zo</v>
-      </c>
-      <c r="C22" t="s">
-        <v>259</v>
-      </c>
-      <c r="D22" t="s">
-        <v>262</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="4"/>
@@ -4257,14 +4257,14 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>decarbonator_zo</v>
       </c>
       <c r="C23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -4273,20 +4273,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>deep_well_injection_zo</v>
+      </c>
+      <c r="C24" t="s">
         <v>264</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>deep_well_injection_zo</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>265</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>266</v>
-      </c>
-      <c r="E24" t="s">
-        <v>267</v>
       </c>
       <c r="G24" t="str">
         <f>CONCATENATE(C24," ",D24," ",E24)</f>
@@ -4295,20 +4295,20 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>dissolved_air_flotation_zo</v>
+      </c>
+      <c r="C25" t="s">
         <v>268</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>dissolved_air_flotation_zo</v>
-      </c>
-      <c r="C25" t="s">
-        <v>269</v>
-      </c>
       <c r="D25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
         <v>209</v>
-      </c>
-      <c r="E25" t="s">
-        <v>210</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ref="G25" si="5">CONCATENATE(C25," ",D25," ",E25)</f>
@@ -4317,14 +4317,14 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>dmbr_zo</v>
       </c>
       <c r="C26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G26" t="str">
         <f>CONCATENATE(C26," ",D26)</f>
@@ -4333,20 +4333,20 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>dual_media_filtration_zo</v>
+      </c>
+      <c r="C27" t="s">
         <v>271</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>dual_media_filtration_zo</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>272</v>
       </c>
-      <c r="D27" t="s">
-        <v>273</v>
-      </c>
       <c r="E27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G27" t="str">
         <f>CONCATENATE(C27," ",D27," ",E27)</f>
@@ -4355,20 +4355,20 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>electrochemical_nutrient_removal_zo</v>
+      </c>
+      <c r="C28" t="s">
         <v>274</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>electrochemical_nutrient_removal_zo</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>275</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>276</v>
-      </c>
-      <c r="E28" t="s">
-        <v>277</v>
       </c>
       <c r="G28" t="str">
         <f>CONCATENATE(C28," ",D28," ",E28)</f>
@@ -4377,17 +4377,17 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>electrodialysis_reversal_zo</v>
+      </c>
+      <c r="C29" t="s">
         <v>278</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>electrodialysis_reversal_zo</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>279</v>
-      </c>
-      <c r="D29" t="s">
-        <v>280</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -4406,7 +4406,7 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -4415,17 +4415,17 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>evaporation_pond_zo</v>
+      </c>
+      <c r="C31" t="s">
         <v>283</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>evaporation_pond_zo</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>284</v>
-      </c>
-      <c r="D31" t="s">
-        <v>285</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -4434,20 +4434,20 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>feed_water_tank_zo</v>
+      </c>
+      <c r="C32" t="s">
         <v>286</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>feed_water_tank_zo</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>287</v>
       </c>
-      <c r="D32" t="s">
-        <v>288</v>
-      </c>
       <c r="E32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G32" t="str">
         <f>CONCATENATE(C32," ",D32," ",E32)</f>
@@ -4456,14 +4456,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>feed_zo</v>
       </c>
       <c r="C33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -4472,17 +4472,17 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>filter_press_zo</v>
+      </c>
+      <c r="C34" t="s">
         <v>289</v>
       </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>filter_press_zo</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>290</v>
-      </c>
-      <c r="D34" t="s">
-        <v>291</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -4491,17 +4491,17 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>fixed_bed_zo</v>
+      </c>
+      <c r="C35" t="s">
         <v>292</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>fixed_bed_zo</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>293</v>
-      </c>
-      <c r="D35" t="s">
-        <v>294</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -4510,14 +4510,14 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>gac_zo</v>
       </c>
       <c r="C36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -4526,20 +4526,20 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>gas_sparged_membrane_zo</v>
+      </c>
+      <c r="C37" t="s">
         <v>296</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>gas_sparged_membrane_zo</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>297</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>298</v>
-      </c>
-      <c r="E37" t="s">
-        <v>299</v>
       </c>
       <c r="G37" t="str">
         <f>CONCATENATE(C37," ",D37," ",E37)</f>
@@ -4548,20 +4548,20 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>injection_well_disposal_zo</v>
+      </c>
+      <c r="C38" t="s">
+        <v>266</v>
+      </c>
+      <c r="D38" t="s">
+        <v>265</v>
+      </c>
+      <c r="E38" t="s">
         <v>300</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>injection_well_disposal_zo</v>
-      </c>
-      <c r="C38" t="s">
-        <v>267</v>
-      </c>
-      <c r="D38" t="s">
-        <v>266</v>
-      </c>
-      <c r="E38" t="s">
-        <v>301</v>
       </c>
       <c r="G38" t="str">
         <f>CONCATENATE(C38," ",D38," ",E38)</f>
@@ -4570,17 +4570,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>intrusion_mitigation_zo</v>
+      </c>
+      <c r="C39" t="s">
         <v>302</v>
       </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>intrusion_mitigation_zo</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>303</v>
-      </c>
-      <c r="D39" t="s">
-        <v>304</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -4589,17 +4589,17 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>ion_exchange_zo</v>
+      </c>
+      <c r="C40" t="s">
         <v>305</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>ion_exchange_zo</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>306</v>
-      </c>
-      <c r="D40" t="s">
-        <v>307</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -4608,23 +4608,23 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>iron_and_manganese_removal_zo</v>
+      </c>
+      <c r="C41" t="s">
         <v>308</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>iron_and_manganese_removal_zo</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>247</v>
+      </c>
+      <c r="E41" t="s">
         <v>309</v>
       </c>
-      <c r="D41" t="s">
-        <v>248</v>
-      </c>
-      <c r="E41" t="s">
-        <v>310</v>
-      </c>
       <c r="F41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G41" t="str">
         <f>CONCATENATE(C41," ",D41," ",E41," ",F41)</f>
@@ -4633,14 +4633,14 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>landfill_zo</v>
       </c>
       <c r="C42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -4649,14 +4649,14 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>mabr_zo</v>
       </c>
       <c r="C43" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -4665,14 +4665,14 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>mbr_zo</v>
       </c>
       <c r="C44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -4681,17 +4681,17 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>media_filtration_zo</v>
       </c>
       <c r="C45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -4700,14 +4700,14 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>metab_zo</v>
       </c>
       <c r="C46" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -4716,14 +4716,14 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>microfiltration_zo</v>
       </c>
       <c r="C47" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -4732,17 +4732,17 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>microscreen_filtration_zo</v>
+      </c>
+      <c r="C48" t="s">
         <v>316</v>
       </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>microscreen_filtration_zo</v>
-      </c>
-      <c r="C48" t="s">
-        <v>317</v>
-      </c>
       <c r="D48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -4751,17 +4751,17 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>municipal_drinking_zo</v>
+      </c>
+      <c r="C49" t="s">
         <v>318</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>municipal_drinking_zo</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>319</v>
-      </c>
-      <c r="D49" t="s">
-        <v>320</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -4770,17 +4770,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>municipal_wwtp_zo</v>
+      </c>
+      <c r="C50" t="s">
+        <v>318</v>
+      </c>
+      <c r="D50" t="s">
         <v>321</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>municipal_wwtp_zo</v>
-      </c>
-      <c r="C50" t="s">
-        <v>319</v>
-      </c>
-      <c r="D50" t="s">
-        <v>322</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -4789,14 +4789,14 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>nanofiltration_zo</v>
       </c>
       <c r="C51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -4805,17 +4805,17 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>ozone_aop _zo</v>
+      </c>
+      <c r="C52" t="s">
         <v>324</v>
       </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>ozone_aop _zo</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>325</v>
-      </c>
-      <c r="D52" t="s">
-        <v>326</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -4824,14 +4824,14 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>ozone_zo</v>
       </c>
       <c r="C53" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -4840,17 +4840,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>photothermal_membrane_zo</v>
+      </c>
+      <c r="C54" t="s">
         <v>327</v>
       </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>photothermal_membrane_zo</v>
-      </c>
-      <c r="C54" t="s">
-        <v>328</v>
-      </c>
       <c r="D54" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -4859,17 +4859,17 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>primary_separator_zo</v>
+      </c>
+      <c r="C55" t="s">
         <v>329</v>
       </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>primary_separator_zo</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>330</v>
-      </c>
-      <c r="D55" t="s">
-        <v>331</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -4885,10 +4885,10 @@
         <v>pump_electricity_zo</v>
       </c>
       <c r="C56" t="s">
+        <v>331</v>
+      </c>
+      <c r="D56" t="s">
         <v>332</v>
-      </c>
-      <c r="D56" t="s">
-        <v>333</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
@@ -4897,14 +4897,14 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
         <v>pump_zo</v>
       </c>
       <c r="C57" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -4913,14 +4913,14 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
         <v>screen_zo</v>
       </c>
       <c r="C58" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -4929,20 +4929,20 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>secondary_treatment_wwtp_zo</v>
+      </c>
+      <c r="C59" t="s">
         <v>335</v>
       </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>secondary_treatment_wwtp_zo</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>336</v>
       </c>
-      <c r="D59" t="s">
-        <v>337</v>
-      </c>
       <c r="E59" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G59" t="str">
         <f>CONCATENATE(C59," ",D59," ",E59)</f>
@@ -4951,14 +4951,14 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
         <v>sedimentation_zo</v>
       </c>
       <c r="C60" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -4967,17 +4967,17 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>settling_pond_zo</v>
+      </c>
+      <c r="C61" t="s">
         <v>339</v>
       </c>
-      <c r="B61" t="str">
-        <f t="shared" si="0"/>
-        <v>settling_pond_zo</v>
-      </c>
-      <c r="C61" t="s">
-        <v>340</v>
-      </c>
       <c r="D61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -4986,17 +4986,17 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
         <v>sludge_tank_zo</v>
       </c>
       <c r="C62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -5005,14 +5005,14 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
         <v>smp_zo</v>
       </c>
       <c r="C63" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -5021,17 +5021,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>static_mixer_zo</v>
+      </c>
+      <c r="C64" t="s">
         <v>343</v>
       </c>
-      <c r="B64" t="str">
-        <f t="shared" si="0"/>
-        <v>static_mixer_zo</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>344</v>
-      </c>
-      <c r="D64" t="s">
-        <v>345</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -5040,17 +5040,17 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>storage_tank_zo</v>
+      </c>
+      <c r="C65" t="s">
         <v>346</v>
       </c>
-      <c r="B65" t="str">
-        <f t="shared" si="0"/>
-        <v>storage_tank_zo</v>
-      </c>
-      <c r="C65" t="s">
-        <v>347</v>
-      </c>
       <c r="D65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -5059,17 +5059,17 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" ref="B66:B77" si="6">CONCATENATE(A66,"_zo")</f>
         <v>surface_discharge_zo</v>
       </c>
       <c r="C66" t="s">
+        <v>348</v>
+      </c>
+      <c r="D66" t="s">
         <v>349</v>
-      </c>
-      <c r="D66" t="s">
-        <v>350</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G77" si="7">CONCATENATE(C66," ",D66)</f>
@@ -5078,20 +5078,20 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="6"/>
         <v>sw_onshore_intake_zo</v>
       </c>
       <c r="C67" t="s">
+        <v>351</v>
+      </c>
+      <c r="D67" t="s">
         <v>352</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>353</v>
-      </c>
-      <c r="E67" t="s">
-        <v>354</v>
       </c>
       <c r="G67" t="str">
         <f>CONCATENATE(C67," ",D67," ",E67)</f>
@@ -5100,20 +5100,20 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="6"/>
         <v>tramp_oil_tank_zo</v>
       </c>
       <c r="C68" t="s">
+        <v>355</v>
+      </c>
+      <c r="D68" t="s">
         <v>356</v>
       </c>
-      <c r="D68" t="s">
-        <v>357</v>
-      </c>
       <c r="E68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" ref="G68:G69" si="8">CONCATENATE(C68," ",D68," ",E68)</f>
@@ -5122,20 +5122,20 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="6"/>
         <v>tri_media_filtration_zo</v>
       </c>
       <c r="C69" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D69" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E69" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="8"/>
@@ -5144,17 +5144,17 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="6"/>
         <v>ultra_filtration_zo</v>
       </c>
       <c r="C70" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="7"/>
@@ -5163,17 +5163,17 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="6"/>
         <v>uv_aop_zo</v>
       </c>
       <c r="C71" t="s">
+        <v>362</v>
+      </c>
+      <c r="D71" t="s">
         <v>363</v>
-      </c>
-      <c r="D71" t="s">
-        <v>364</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="7"/>
@@ -5182,14 +5182,14 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="6"/>
         <v>uv_zo</v>
       </c>
       <c r="C72" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="7"/>
@@ -5198,17 +5198,17 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="6"/>
         <v>vfa_recovery_zo</v>
       </c>
       <c r="C73" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D73" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="7"/>
@@ -5217,14 +5217,14 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="6"/>
         <v>waiv_zo</v>
       </c>
       <c r="C74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="7"/>
@@ -5233,20 +5233,20 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="6"/>
         <v>walnut_shell_filter_zo</v>
       </c>
       <c r="C75" t="s">
+        <v>368</v>
+      </c>
+      <c r="D75" t="s">
         <v>369</v>
       </c>
-      <c r="D75" t="s">
-        <v>370</v>
-      </c>
       <c r="E75" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ref="G75:G76" si="9">CONCATENATE(C75," ",D75," ",E75)</f>
@@ -5255,20 +5255,20 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="6"/>
         <v>water_pumping_station_zo</v>
       </c>
       <c r="C76" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D76" t="s">
+        <v>371</v>
+      </c>
+      <c r="E76" t="s">
         <v>372</v>
-      </c>
-      <c r="E76" t="s">
-        <v>373</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="9"/>
@@ -5277,17 +5277,17 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="6"/>
         <v>well_field_zo</v>
       </c>
       <c r="C77" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D77" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Add dictionaries for unit doc sections that require unique customization; first test with updating titles for those that need the update; add Additional Variables section if unit non-basic
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AD6B36-2DD8-4668-8E1E-D2B182143B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCCF707-F279-4750-BC7A-D4F5B38171A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$78</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="379">
   <si>
     <t>Name</t>
   </si>
@@ -1166,6 +1166,9 @@
   </si>
   <si>
     <t>blending reservoir</t>
+  </si>
+  <si>
+    <t>energy_helper_func</t>
   </si>
 </sst>
 </file>
@@ -1231,11 +1234,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1574,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1585,13 +1589,13 @@
     <col min="1" max="1" width="33.3984375" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.59765625" customWidth="1"/>
-    <col min="5" max="5" width="20.265625" customWidth="1"/>
-    <col min="6" max="6" width="38.59765625" customWidth="1"/>
-    <col min="7" max="7" width="30.265625" customWidth="1"/>
-    <col min="8" max="8" width="25.59765625" customWidth="1"/>
+    <col min="6" max="6" width="20.265625" customWidth="1"/>
+    <col min="7" max="7" width="38.59765625" customWidth="1"/>
+    <col min="8" max="8" width="30.265625" customWidth="1"/>
+    <col min="9" max="9" width="25.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1604,20 +1608,23 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1630,23 +1637,26 @@
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="str">
+      <c r="G2" s="3" t="str">
         <f>IF(C2="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G2" s="3" t="str">
+      <c r="H2" s="3" t="str">
         <f>IF(D2="SIDO","single-input, double-output",IF(D2="SISO","single-input, single-output",IF(D2="PT","pass-through",IF(D2="DISO","double-input, single-output",IF(D2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="H2" s="3" t="str">
+      <c r="I2" s="3" t="str">
         <f>IF(D2="SIDO","sido_methods",IF(D2="SISO","siso_methods",IF(D2="PT","pt_methods",IF(D2="DISO","diso_methods",IF(D2="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -1659,23 +1669,26 @@
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F65" si="0">IF(C3="basic","cost_power_law_flow")</f>
+      <c r="G3" s="3" t="str">
+        <f t="shared" ref="G3:G65" si="0">IF(C3="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G3" s="3" t="str">
-        <f t="shared" ref="G3:G66" si="1">IF(D3="SIDO","single-input, double-output",IF(D3="SISO","single-input, single-output",IF(D3="PT","pass-through",IF(D3="DISO","double-input, single-output",IF(D3="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="H3" s="3" t="str">
+        <f t="shared" ref="H3:H66" si="1">IF(D3="SIDO","single-input, double-output",IF(D3="SISO","single-input, single-output",IF(D3="PT","pass-through",IF(D3="DISO","double-input, single-output",IF(D3="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="H3" s="3" t="str">
-        <f t="shared" ref="H3:H66" si="2">IF(D3="SIDO","sido_methods",IF(D3="SISO","siso_methods",IF(D3="PT","pt_methods",IF(D3="DISO","diso_methods",IF(D3="SIDO reactive","sidor_methods","")))))</f>
+      <c r="I3" s="3" t="str">
+        <f t="shared" ref="I3:I66" si="2">IF(D3="SIDO","sido_methods",IF(D3="SISO","siso_methods",IF(D3="PT","pt_methods",IF(D3="DISO","diso_methods",IF(D3="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1688,23 +1701,26 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="G4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G4" s="3" t="str">
+      <c r="H4" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H4" s="3" t="str">
+      <c r="I4" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1717,23 +1733,26 @@
       <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3" t="b">
+      <c r="G5" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="3" t="str">
+      <c r="H5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H5" s="3" t="str">
+      <c r="I5" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1746,23 +1765,26 @@
       <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="G6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G6" s="3" t="str">
+      <c r="H6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H6" s="3" t="str">
+      <c r="I6" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1775,23 +1797,26 @@
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="H7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="I7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -1804,23 +1829,26 @@
       <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="3" t="str">
+      <c r="G8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G8" s="3" t="str">
+      <c r="H8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H8" s="3" t="str">
+      <c r="I8" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>377</v>
       </c>
@@ -1833,23 +1861,26 @@
       <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="G9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="H9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="I9" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1862,22 +1893,25 @@
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="3" t="str">
+      <c r="H10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H10" s="3" t="str">
+      <c r="I10" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -1890,23 +1924,26 @@
       <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="3" t="str">
+      <c r="G11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G11" s="3" t="str">
+      <c r="H11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H11" s="3" t="str">
+      <c r="I11" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1919,22 +1956,25 @@
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="3" t="str">
+      <c r="H12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H12" s="3" t="str">
+      <c r="I12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -1947,23 +1987,26 @@
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="G13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G13" s="3" t="str">
+      <c r="H13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H13" s="3" t="str">
+      <c r="I13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1976,22 +2019,25 @@
       <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="3" t="str">
+      <c r="H14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H14" s="3" t="str">
+      <c r="I14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -2004,22 +2050,25 @@
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="3" t="str">
+      <c r="H15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H15" s="3" t="str">
+      <c r="I15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -2032,23 +2081,26 @@
       <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3" t="str">
+      <c r="G16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G16" s="3" t="str">
+      <c r="H16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H16" s="3" t="str">
+      <c r="I16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
@@ -2061,23 +2113,26 @@
       <c r="D17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="3" t="str">
+      <c r="G17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G17" s="3" t="str">
+      <c r="H17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H17" s="3" t="str">
+      <c r="I17" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
@@ -2090,22 +2145,25 @@
       <c r="D18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="3" t="str">
+      <c r="H18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H18" s="3" t="str">
+      <c r="I18" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
@@ -2118,23 +2176,26 @@
       <c r="D19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="3" t="b">
+      <c r="G19" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="3" t="str">
+      <c r="H19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>double-input, single-output</v>
       </c>
-      <c r="H19" s="3" t="str">
+      <c r="I19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>diso_methods</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -2147,23 +2208,26 @@
       <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="3" t="b">
+      <c r="G20" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="3" t="str">
+      <c r="H20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H20" s="3" t="str">
+      <c r="I20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
@@ -2176,23 +2240,26 @@
       <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="3" t="str">
+      <c r="G21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G21" s="3" t="str">
+      <c r="H21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H21" s="3" t="str">
+      <c r="I21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
@@ -2205,23 +2272,26 @@
       <c r="D22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="3" t="str">
+      <c r="G22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G22" s="3" t="str">
+      <c r="H22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H22" s="3" t="str">
+      <c r="I22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
@@ -2234,22 +2304,25 @@
       <c r="D23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="3" t="str">
+      <c r="H23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H23" s="3" t="str">
+      <c r="I23" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
@@ -2262,23 +2335,26 @@
       <c r="D24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="3" t="str">
+      <c r="G24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G24" s="3" t="str">
+      <c r="H24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H24" s="3" t="str">
+      <c r="I24" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
@@ -2291,22 +2367,25 @@
       <c r="D25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="3" t="str">
+      <c r="H25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H25" s="3" t="str">
+      <c r="I25" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>74</v>
       </c>
@@ -2319,23 +2398,26 @@
       <c r="D26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="3" t="str">
+      <c r="G26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G26" s="3" t="str">
+      <c r="H26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H26" s="3" t="str">
+      <c r="I26" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -2348,22 +2430,25 @@
       <c r="D27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="3" t="str">
+      <c r="H27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H27" s="3" t="str">
+      <c r="I27" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
@@ -2376,23 +2461,26 @@
       <c r="D28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="3" t="str">
+      <c r="G28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G28" s="3" t="str">
+      <c r="H28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H28" s="3" t="str">
+      <c r="I28" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>81</v>
       </c>
@@ -2405,22 +2493,25 @@
       <c r="D29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="3" t="str">
+      <c r="H29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H29" s="3" t="str">
+      <c r="I29" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
@@ -2433,22 +2524,25 @@
       <c r="D30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G30" s="3" t="str">
+      <c r="H30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H30" s="3" t="str">
+      <c r="I30" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>86</v>
       </c>
@@ -2461,23 +2555,26 @@
       <c r="D31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="3" t="str">
+      <c r="G31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G31" s="3" t="str">
+      <c r="H31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H31" s="3" t="str">
+      <c r="I31" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
@@ -2490,22 +2587,25 @@
       <c r="D32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="3" t="str">
+      <c r="H32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H32" s="3" t="str">
+      <c r="I32" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
@@ -2518,23 +2618,26 @@
       <c r="D33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="3" t="str">
+      <c r="G33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G33" s="3" t="str">
+      <c r="H33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H33" s="3" t="str">
+      <c r="I33" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>93</v>
       </c>
@@ -2547,21 +2650,24 @@
       <c r="D34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F34" s="3" t="b">
+      <c r="G34" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I34" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>97</v>
       </c>
@@ -2574,22 +2680,25 @@
       <c r="D35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G35" s="3" t="str">
+      <c r="H35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H35" s="3" t="str">
+      <c r="I35" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>100</v>
       </c>
@@ -2602,22 +2711,25 @@
       <c r="D36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G36" s="3" t="str">
+      <c r="H36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H36" s="3" t="str">
+      <c r="I36" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>103</v>
       </c>
@@ -2630,22 +2742,25 @@
       <c r="D37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="3" t="str">
+      <c r="H37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H37" s="3" t="str">
+      <c r="I37" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>106</v>
       </c>
@@ -2658,21 +2773,24 @@
       <c r="D38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="3" t="b">
+      <c r="G38" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="I38" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>109</v>
       </c>
@@ -2685,23 +2803,26 @@
       <c r="D39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="3" t="str">
+      <c r="G39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G39" s="3" t="str">
+      <c r="H39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H39" s="3" t="str">
+      <c r="I39" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>111</v>
       </c>
@@ -2714,23 +2835,26 @@
       <c r="D40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="3" t="str">
+      <c r="G40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G40" s="3" t="str">
+      <c r="H40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H40" s="3" t="str">
+      <c r="I40" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>113</v>
       </c>
@@ -2743,22 +2867,25 @@
       <c r="D41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G41" s="3" t="str">
+      <c r="H41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H41" s="3" t="str">
+      <c r="I41" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
@@ -2771,22 +2898,25 @@
       <c r="D42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G42" s="3" t="str">
+      <c r="H42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H42" s="3" t="str">
+      <c r="I42" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
@@ -2799,22 +2929,25 @@
       <c r="D43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="G43" s="3" t="str">
+      <c r="H43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H43" s="3" t="str">
+      <c r="I43" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>122</v>
       </c>
@@ -2827,22 +2960,25 @@
       <c r="D44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G44" s="3" t="str">
+      <c r="H44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H44" s="3" t="str">
+      <c r="I44" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>125</v>
       </c>
@@ -2855,23 +2991,26 @@
       <c r="D45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="3" t="str">
+      <c r="G45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G45" s="3" t="str">
+      <c r="H45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H45" s="3" t="str">
+      <c r="I45" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>127</v>
       </c>
@@ -2884,23 +3023,26 @@
       <c r="D46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="3" t="str">
+      <c r="G46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G46" s="3" t="str">
+      <c r="H46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H46" s="3" t="str">
+      <c r="I46" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>129</v>
       </c>
@@ -2913,22 +3055,25 @@
       <c r="D47" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G47" s="3" t="str">
+      <c r="H47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H47" s="3" t="str">
+      <c r="I47" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>132</v>
       </c>
@@ -2941,23 +3086,26 @@
       <c r="D48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="3" t="str">
+      <c r="G48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G48" s="3" t="str">
+      <c r="H48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H48" s="3" t="str">
+      <c r="I48" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>134</v>
       </c>
@@ -2970,23 +3118,26 @@
       <c r="D49" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="3" t="str">
+      <c r="G49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G49" s="3" t="str">
+      <c r="H49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H49" s="3" t="str">
+      <c r="I49" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>136</v>
       </c>
@@ -2999,22 +3150,25 @@
       <c r="D50" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="3" t="str">
+      <c r="H50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H50" s="3" t="str">
+      <c r="I50" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>138</v>
       </c>
@@ -3027,23 +3181,26 @@
       <c r="D51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F51" s="3" t="str">
+      <c r="G51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G51" s="3" t="str">
+      <c r="H51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H51" s="3" t="str">
+      <c r="I51" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>140</v>
       </c>
@@ -3056,22 +3213,25 @@
       <c r="D52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G52" s="3" t="str">
+      <c r="H52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H52" s="3" t="str">
+      <c r="I52" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>143</v>
       </c>
@@ -3084,22 +3244,25 @@
       <c r="D53" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G53" s="3" t="str">
+      <c r="H53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H53" s="3" t="str">
+      <c r="I53" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>145</v>
       </c>
@@ -3112,22 +3275,25 @@
       <c r="D54" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G54" s="3" t="str">
+      <c r="H54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H54" s="3" t="str">
+      <c r="I54" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>148</v>
       </c>
@@ -3140,22 +3306,25 @@
       <c r="D55" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G55" s="3" t="str">
+      <c r="H55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H55" s="3" t="str">
+      <c r="I55" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>151</v>
       </c>
@@ -3168,23 +3337,26 @@
       <c r="D56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="3" t="str">
+      <c r="G56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G56" s="3" t="str">
+      <c r="H56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H56" s="3" t="str">
+      <c r="I56" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>153</v>
       </c>
@@ -3197,22 +3369,25 @@
       <c r="D57" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G57" s="3" t="str">
+      <c r="H57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H57" s="3" t="str">
+      <c r="I57" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>156</v>
       </c>
@@ -3225,23 +3400,26 @@
       <c r="D58" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="3" t="str">
+      <c r="G58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G58" s="3" t="str">
+      <c r="H58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H58" s="3" t="str">
+      <c r="I58" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>158</v>
       </c>
@@ -3254,23 +3432,26 @@
       <c r="D59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="3" t="str">
+      <c r="G59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G59" s="3" t="str">
+      <c r="H59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H59" s="3" t="str">
+      <c r="I59" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>160</v>
       </c>
@@ -3283,22 +3464,25 @@
       <c r="D60" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G60" s="3" t="str">
+      <c r="H60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H60" s="3" t="str">
+      <c r="I60" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>162</v>
       </c>
@@ -3311,22 +3495,25 @@
       <c r="D61" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G61" s="3" t="str">
+      <c r="H61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H61" s="3" t="str">
+      <c r="I61" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>165</v>
       </c>
@@ -3339,23 +3526,26 @@
       <c r="D62" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="3" t="str">
+      <c r="G62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G62" s="3" t="str">
+      <c r="H62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H62" s="3" t="str">
+      <c r="I62" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>167</v>
       </c>
@@ -3368,23 +3558,26 @@
       <c r="D63" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F63" s="3" t="str">
+      <c r="G63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G63" s="3" t="str">
+      <c r="H63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H63" s="3" t="str">
+      <c r="I63" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>169</v>
       </c>
@@ -3397,23 +3590,26 @@
       <c r="D64" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="3" t="str">
+      <c r="G64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G64" s="3" t="str">
+      <c r="H64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H64" s="3" t="str">
+      <c r="I64" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>171</v>
       </c>
@@ -3426,23 +3622,26 @@
       <c r="D65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="3" t="str">
+      <c r="G65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G65" s="3" t="str">
+      <c r="H65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H65" s="3" t="str">
+      <c r="I65" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>173</v>
       </c>
@@ -3455,22 +3654,25 @@
       <c r="D66" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G66" s="3" t="str">
+      <c r="H66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H66" s="3" t="str">
+      <c r="I66" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>176</v>
       </c>
@@ -3483,22 +3685,25 @@
       <c r="D67" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="G67" s="3" t="str">
-        <f t="shared" ref="G67:G78" si="3">IF(D67="SIDO","single-input, double-output",IF(D67="SISO","single-input, single-output",IF(D67="PT","pass-through",IF(D67="DISO","double-input, single-output",IF(D67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="H67" s="3" t="str">
+        <f t="shared" ref="H67:H78" si="3">IF(D67="SIDO","single-input, double-output",IF(D67="SISO","single-input, single-output",IF(D67="PT","pass-through",IF(D67="DISO","double-input, single-output",IF(D67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="H67" s="3" t="str">
-        <f t="shared" ref="H67:H78" si="4">IF(D67="SIDO","sido_methods",IF(D67="SISO","siso_methods",IF(D67="PT","pt_methods",IF(D67="DISO","diso_methods",IF(D67="SIDO reactive","sidor_methods","")))))</f>
+      <c r="I67" s="3" t="str">
+        <f t="shared" ref="I67:I78" si="4">IF(D67="SIDO","sido_methods",IF(D67="SISO","siso_methods",IF(D67="PT","pt_methods",IF(D67="DISO","diso_methods",IF(D67="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>179</v>
       </c>
@@ -3511,23 +3716,26 @@
       <c r="D68" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="3" t="str">
-        <f t="shared" ref="F68:F76" si="5">IF(C68="basic","cost_power_law_flow")</f>
+      <c r="G68" s="3" t="str">
+        <f t="shared" ref="G68:G76" si="5">IF(C68="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G68" s="3" t="str">
+      <c r="H68" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H68" s="3" t="str">
+      <c r="I68" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>181</v>
       </c>
@@ -3540,23 +3748,26 @@
       <c r="D69" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F69" s="3" t="str">
+      <c r="G69" s="3" t="str">
         <f t="shared" si="5"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G69" s="3" t="str">
+      <c r="H69" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H69" s="3" t="str">
+      <c r="I69" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>183</v>
       </c>
@@ -3569,23 +3780,26 @@
       <c r="D70" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="3" t="str">
+      <c r="G70" s="3" t="str">
         <f t="shared" si="5"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G70" s="3" t="str">
+      <c r="H70" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H70" s="3" t="str">
+      <c r="I70" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>185</v>
       </c>
@@ -3598,23 +3812,26 @@
       <c r="D71" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F71" s="3" t="str">
+      <c r="G71" s="3" t="str">
         <f t="shared" si="5"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G71" s="3" t="str">
+      <c r="H71" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H71" s="3" t="str">
+      <c r="I71" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>187</v>
       </c>
@@ -3627,22 +3844,25 @@
       <c r="D72" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="G72" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G72" s="3" t="str">
+      <c r="H72" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H72" s="3" t="str">
+      <c r="I72" s="3" t="str">
         <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>190</v>
       </c>
@@ -3655,22 +3875,25 @@
       <c r="D73" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="G73" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G73" s="3" t="str">
+      <c r="H73" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H73" s="3" t="str">
+      <c r="I73" s="3" t="str">
         <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>193</v>
       </c>
@@ -3683,23 +3906,26 @@
       <c r="D74" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F74" s="3" t="b">
+      <c r="G74" s="3" t="b">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G74" s="3" t="str">
+      <c r="H74" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H74" s="3" t="str">
+      <c r="I74" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>195</v>
       </c>
@@ -3712,23 +3938,26 @@
       <c r="D75" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F75" s="3" t="str">
+      <c r="G75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G75" s="3" t="str">
+      <c r="H75" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H75" s="3" t="str">
+      <c r="I75" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>197</v>
       </c>
@@ -3741,23 +3970,26 @@
       <c r="D76" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E76" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F76" s="3" t="str">
+      <c r="G76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G76" s="3" t="str">
+      <c r="H76" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H76" s="3" t="str">
+      <c r="I76" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>199</v>
       </c>
@@ -3770,22 +4002,25 @@
       <c r="D77" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="G77" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G77" s="3" t="str">
+      <c r="H77" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H77" s="3" t="str">
+      <c r="I77" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>201</v>
       </c>
@@ -3798,17 +4033,20 @@
       <c r="D78" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F78" s="3" t="s">
+      <c r="G78" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="G78" s="3" t="str">
+      <c r="H78" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H78" s="3" t="str">
+      <c r="I78" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>

</xml_diff>

<commit_message>
Automate  inclusion of additional variables for non-basic units with description from doc strings
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B246C665-906F-4E72-8231-B60DBF79748C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3159F15A-AF51-45D4-9255-499A24D3C4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$78</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="463">
   <si>
     <t>Name</t>
   </si>
@@ -1169,6 +1169,258 @@
   </si>
   <si>
     <t>energy_helper_func</t>
+  </si>
+  <si>
+    <t>class_name</t>
+  </si>
+  <si>
+    <t>BackwashSolidsHandlingZO</t>
+  </si>
+  <si>
+    <t>BioActiveFiltrationZO</t>
+  </si>
+  <si>
+    <t>BlendingReservoirZO</t>
+  </si>
+  <si>
+    <t>CASZO</t>
+  </si>
+  <si>
+    <t>CoolingTowerZO</t>
+  </si>
+  <si>
+    <t>DeepWellInjectionZO</t>
+  </si>
+  <si>
+    <t>DMBRZO</t>
+  </si>
+  <si>
+    <t>ElectrodialysisReversalZO</t>
+  </si>
+  <si>
+    <t>AerationBasinZO</t>
+  </si>
+  <si>
+    <t>AirFlotationZO</t>
+  </si>
+  <si>
+    <t>BioreactorZO</t>
+  </si>
+  <si>
+    <t>MetabZO</t>
+  </si>
+  <si>
+    <t>BufferTankZO</t>
+  </si>
+  <si>
+    <t>ChemicalAdditionZO</t>
+  </si>
+  <si>
+    <t>CartridgeFiltrationZO</t>
+  </si>
+  <si>
+    <t>CoolingSupplyZO</t>
+  </si>
+  <si>
+    <t>DecarbonatorZO</t>
+  </si>
+  <si>
+    <t>DissolvedAirFlotationZO</t>
+  </si>
+  <si>
+    <t>FeedWaterTankZO</t>
+  </si>
+  <si>
+    <t>FeedZO</t>
+  </si>
+  <si>
+    <t>ElectroNPZO</t>
+  </si>
+  <si>
+    <t>EnergyRecoveryZO</t>
+  </si>
+  <si>
+    <t>IronManganeseRemovalZO</t>
+  </si>
+  <si>
+    <t>LandfillZO</t>
+  </si>
+  <si>
+    <t>PumpElectricityZO</t>
+  </si>
+  <si>
+    <t>MABRZO</t>
+  </si>
+  <si>
+    <t>MBRZO</t>
+  </si>
+  <si>
+    <t>MediaFiltrationZO</t>
+  </si>
+  <si>
+    <t>MicroFiltrationZO</t>
+  </si>
+  <si>
+    <t>MicroscreenFiltrationZO</t>
+  </si>
+  <si>
+    <t>MunicipalWWTPZO</t>
+  </si>
+  <si>
+    <t>NanofiltrationZO</t>
+  </si>
+  <si>
+    <t>ClarifierZO</t>
+  </si>
+  <si>
+    <t>PrimarySeparatorZO</t>
+  </si>
+  <si>
+    <t>PumpZO</t>
+  </si>
+  <si>
+    <t>ScreenZO</t>
+  </si>
+  <si>
+    <t>SedimentationZO</t>
+  </si>
+  <si>
+    <t>SettlingPondZO</t>
+  </si>
+  <si>
+    <t>SMPZO</t>
+  </si>
+  <si>
+    <t>TrampOilTankZO</t>
+  </si>
+  <si>
+    <t>TriMediaFiltrationZO</t>
+  </si>
+  <si>
+    <t>CoagulationFlocculationZO</t>
+  </si>
+  <si>
+    <t>UltraFiltrationZO</t>
+  </si>
+  <si>
+    <t>UVZO</t>
+  </si>
+  <si>
+    <t>UVAOPZO</t>
+  </si>
+  <si>
+    <t>WalnutShellFilterZO</t>
+  </si>
+  <si>
+    <t>WAIVZO</t>
+  </si>
+  <si>
+    <t>AnaerobicDigestionOxidationZO</t>
+  </si>
+  <si>
+    <t>FixedBedZO</t>
+  </si>
+  <si>
+    <t>MunicipalDrinkingZO</t>
+  </si>
+  <si>
+    <t>OzoneZO</t>
+  </si>
+  <si>
+    <t>OzoneAOPZO</t>
+  </si>
+  <si>
+    <t>IonExchangeZO</t>
+  </si>
+  <si>
+    <t>BrineConcentratorZO</t>
+  </si>
+  <si>
+    <t>GACZO</t>
+  </si>
+  <si>
+    <t>DualMediaFiltrationZO</t>
+  </si>
+  <si>
+    <t>StorageTankZO</t>
+  </si>
+  <si>
+    <t>SWOnshoreIntakeZO</t>
+  </si>
+  <si>
+    <t>ChlorinationZO</t>
+  </si>
+  <si>
+    <t>StaticMixerZO</t>
+  </si>
+  <si>
+    <t>CO2AdditionZO</t>
+  </si>
+  <si>
+    <t>SludgeTankZO</t>
+  </si>
+  <si>
+    <t>EvaporationPondZO</t>
+  </si>
+  <si>
+    <t>FilterPressZO</t>
+  </si>
+  <si>
+    <t>WaterPumpingStationZO</t>
+  </si>
+  <si>
+    <t>WellFieldZO</t>
+  </si>
+  <si>
+    <t>IntrusionMitigationZO</t>
+  </si>
+  <si>
+    <t>InjectionWellDisposalZO</t>
+  </si>
+  <si>
+    <t>SurfaceDischargeZO</t>
+  </si>
+  <si>
+    <t>PhotothermalMembraneZO</t>
+  </si>
+  <si>
+    <t>CANDOPZO</t>
+  </si>
+  <si>
+    <t>AnaerobicMBRMECZO</t>
+  </si>
+  <si>
+    <t>ATHTLZO</t>
+  </si>
+  <si>
+    <t>SecondaryTreatmentWWTPZO</t>
+  </si>
+  <si>
+    <t>CofermentationZO</t>
+  </si>
+  <si>
+    <t>ConstructedWetlandsZO</t>
+  </si>
+  <si>
+    <t>GasSpargedMembraneZO</t>
+  </si>
+  <si>
+    <t>HTGZO</t>
+  </si>
+  <si>
+    <t>SaltPrecipitationZO</t>
+  </si>
+  <si>
+    <t>VFARecoveryZO</t>
+  </si>
+  <si>
+    <t>autothermal_hydrothermal_liquefaction_zo</t>
+  </si>
+  <si>
+    <t>hydrothermal_gasification_zo</t>
+  </si>
+  <si>
+    <t>supercritical_salt_precipitation_zo</t>
   </si>
 </sst>
 </file>
@@ -1578,24 +1830,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="33.3984375" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" customWidth="1"/>
-    <col min="6" max="6" width="20.265625" customWidth="1"/>
-    <col min="7" max="7" width="38.59765625" customWidth="1"/>
-    <col min="8" max="8" width="30.265625" customWidth="1"/>
-    <col min="9" max="9" width="25.59765625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" customWidth="1"/>
+    <col min="7" max="7" width="20.265625" customWidth="1"/>
+    <col min="8" max="8" width="38.59765625" customWidth="1"/>
+    <col min="9" max="9" width="30.265625" customWidth="1"/>
+    <col min="10" max="10" width="25.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1603,2455 +1856,2693 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="b">
+      <c r="F2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="str">
-        <f>IF(C2="basic","cost_power_law_flow")</f>
+      <c r="H2" s="3" t="str">
+        <f>IF(D2="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H2" s="3" t="str">
-        <f>IF(D2="SIDO","single-input, double-output",IF(D2="SISO","single-input, single-output",IF(D2="PT","pass-through",IF(D2="DISO","double-input, single-output",IF(D2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="I2" s="3" t="str">
+        <f>IF(E2="SIDO","single-input, double-output",IF(E2="SISO","single-input, single-output",IF(E2="PT","pass-through",IF(E2="DISO","double-input, single-output",IF(E2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I2" s="3" t="str">
-        <f>IF(D2="SIDO","sido_methods",IF(D2="SISO","siso_methods",IF(D2="PT","pt_methods",IF(D2="DISO","diso_methods",IF(D2="SIDO reactive","sidor_methods","")))))</f>
+      <c r="J2" s="3" t="str">
+        <f>IF(E2="SIDO","sido_methods",IF(E2="SISO","siso_methods",IF(E2="PT","pt_methods",IF(E2="DISO","diso_methods",IF(E2="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="b">
+      <c r="F3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="str">
-        <f t="shared" ref="G3:G65" si="0">IF(C3="basic","cost_power_law_flow")</f>
+      <c r="H3" s="3" t="str">
+        <f>IF(D3="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H3" s="3" t="str">
-        <f t="shared" ref="H3:H66" si="1">IF(D3="SIDO","single-input, double-output",IF(D3="SISO","single-input, single-output",IF(D3="PT","pass-through",IF(D3="DISO","double-input, single-output",IF(D3="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="I3" s="3" t="str">
+        <f>IF(E3="SIDO","single-input, double-output",IF(E3="SISO","single-input, single-output",IF(E3="PT","pass-through",IF(E3="DISO","double-input, single-output",IF(E3="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I3" s="3" t="str">
-        <f t="shared" ref="I3:I66" si="2">IF(D3="SIDO","sido_methods",IF(D3="SISO","siso_methods",IF(D3="PT","pt_methods",IF(D3="DISO","diso_methods",IF(D3="SIDO reactive","sidor_methods","")))))</f>
+      <c r="J3" s="3" t="str">
+        <f>IF(E3="SIDO","sido_methods",IF(E3="SISO","siso_methods",IF(E3="PT","pt_methods",IF(E3="DISO","diso_methods",IF(E3="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="b">
+      <c r="F4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H4" s="3" t="str">
+        <f>IF(D4="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H4" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I4" s="3" t="str">
+        <f>IF(E4="SIDO","single-input, double-output",IF(E4="SISO","single-input, single-output",IF(E4="PT","pass-through",IF(E4="DISO","double-input, single-output",IF(E4="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I4" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J4" s="3" t="str">
+        <f>IF(E4="SIDO","sido_methods",IF(E4="SISO","siso_methods",IF(E4="PT","pt_methods",IF(E4="DISO","diso_methods",IF(E4="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="b">
+      <c r="F5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H5" s="3" t="b">
+        <f>IF(D5="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I5" s="3" t="str">
+        <f>IF(E5="SIDO","single-input, double-output",IF(E5="SISO","single-input, single-output",IF(E5="PT","pass-through",IF(E5="DISO","double-input, single-output",IF(E5="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="I5" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J5" s="3" t="str">
+        <f>IF(E5="SIDO","sido_methods",IF(E5="SISO","siso_methods",IF(E5="PT","pt_methods",IF(E5="DISO","diso_methods",IF(E5="SIDO reactive","sidor_methods","")))))</f>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>380</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3" t="b">
+      <c r="F6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H6" s="3" t="str">
+        <f>IF(D6="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H6" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I6" s="3" t="str">
+        <f>IF(E6="SIDO","single-input, double-output",IF(E6="SISO","single-input, single-output",IF(E6="PT","pass-through",IF(E6="DISO","double-input, single-output",IF(E6="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I6" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J6" s="3" t="str">
+        <f>IF(E6="SIDO","sido_methods",IF(E6="SISO","siso_methods",IF(E6="PT","pt_methods",IF(E6="DISO","diso_methods",IF(E6="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
+        <v>381</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3" t="b">
+      <c r="F7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H7" s="3" t="str">
+        <f>IF(D7="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H7" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I7" s="3" t="str">
+        <f>IF(E7="SIDO","single-input, double-output",IF(E7="SISO","single-input, single-output",IF(E7="PT","pass-through",IF(E7="DISO","double-input, single-output",IF(E7="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I7" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J7" s="3" t="str">
+        <f>IF(E7="SIDO","sido_methods",IF(E7="SISO","siso_methods",IF(E7="PT","pt_methods",IF(E7="DISO","diso_methods",IF(E7="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="b">
+      <c r="F8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H8" s="3" t="str">
+        <f>IF(D8="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H8" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I8" s="3" t="str">
+        <f>IF(E8="SIDO","single-input, double-output",IF(E8="SISO","single-input, single-output",IF(E8="PT","pass-through",IF(E8="DISO","double-input, single-output",IF(E8="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I8" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J8" s="3" t="str">
+        <f>IF(E8="SIDO","sido_methods",IF(E8="SISO","siso_methods",IF(E8="PT","pt_methods",IF(E8="DISO","diso_methods",IF(E8="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>377</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
+        <v>382</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3" t="b">
+      <c r="F9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H9" s="3" t="str">
+        <f>IF(D9="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H9" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I9" s="3" t="str">
+        <f>IF(E9="SIDO","single-input, double-output",IF(E9="SISO","single-input, single-output",IF(E9="PT","pass-through",IF(E9="DISO","double-input, single-output",IF(E9="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I9" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J9" s="3" t="str">
+        <f>IF(E9="SIDO","sido_methods",IF(E9="SISO","siso_methods",IF(E9="PT","pt_methods",IF(E9="DISO","diso_methods",IF(E9="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
+        <v>433</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="4" t="b">
+      <c r="F10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I10" s="3" t="str">
+        <f>IF(E10="SIDO","single-input, double-output",IF(E10="SISO","single-input, single-output",IF(E10="PT","pass-through",IF(E10="DISO","double-input, single-output",IF(E10="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I10" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J10" s="3" t="str">
+        <f>IF(E10="SIDO","sido_methods",IF(E10="SISO","siso_methods",IF(E10="PT","pt_methods",IF(E10="DISO","diso_methods",IF(E10="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
+        <v>392</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="4" t="b">
+      <c r="F11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H11" s="3" t="str">
+        <f>IF(D11="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H11" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I11" s="3" t="str">
+        <f>IF(E11="SIDO","single-input, double-output",IF(E11="SISO","single-input, single-output",IF(E11="PT","pass-through",IF(E11="DISO","double-input, single-output",IF(E11="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I11" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J11" s="3" t="str">
+        <f>IF(E11="SIDO","sido_methods",IF(E11="SISO","siso_methods",IF(E11="PT","pt_methods",IF(E11="DISO","diso_methods",IF(E11="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
+        <v>450</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="4" t="b">
+      <c r="F12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I12" s="3" t="str">
+        <f>IF(E12="SIDO","single-input, double-output",IF(E12="SISO","single-input, single-output",IF(E12="PT","pass-through",IF(E12="DISO","double-input, single-output",IF(E12="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="I12" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J12" s="3" t="str">
+        <f>IF(E12="SIDO","sido_methods",IF(E12="SISO","siso_methods",IF(E12="PT","pt_methods",IF(E12="DISO","diso_methods",IF(E12="SIDO reactive","sidor_methods","")))))</f>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
+        <v>394</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="4" t="b">
+      <c r="F13" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H13" s="3" t="str">
+        <f>IF(D13="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H13" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I13" s="3" t="str">
+        <f>IF(E13="SIDO","single-input, double-output",IF(E13="SISO","single-input, single-output",IF(E13="PT","pass-through",IF(E13="DISO","double-input, single-output",IF(E13="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I13" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J13" s="3" t="str">
+        <f>IF(E13="SIDO","sido_methods",IF(E13="SISO","siso_methods",IF(E13="PT","pt_methods",IF(E13="DISO","diso_methods",IF(E13="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="4" t="b">
+      <c r="F14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I14" s="3" t="str">
+        <f>IF(E14="SIDO","single-input, double-output",IF(E14="SISO","single-input, single-output",IF(E14="PT","pass-through",IF(E14="DISO","double-input, single-output",IF(E14="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I14" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J14" s="3" t="str">
+        <f>IF(E14="SIDO","sido_methods",IF(E14="SISO","siso_methods",IF(E14="PT","pt_methods",IF(E14="DISO","diso_methods",IF(E14="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
+        <v>438</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="4" t="b">
+      <c r="F15" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I15" s="3" t="str">
+        <f>IF(E15="SIDO","single-input, double-output",IF(E15="SISO","single-input, single-output",IF(E15="PT","pass-through",IF(E15="DISO","double-input, single-output",IF(E15="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I15" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J15" s="3" t="str">
+        <f>IF(E15="SIDO","sido_methods",IF(E15="SISO","siso_methods",IF(E15="PT","pt_methods",IF(E15="DISO","diso_methods",IF(E15="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
+        <v>412</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="4" t="b">
+      <c r="F16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H16" s="3" t="str">
+        <f>IF(D16="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H16" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I16" s="3" t="str">
+        <f>IF(E16="SIDO","single-input, double-output",IF(E16="SISO","single-input, single-output",IF(E16="PT","pass-through",IF(E16="DISO","double-input, single-output",IF(E16="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I16" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J16" s="3" t="str">
+        <f>IF(E16="SIDO","sido_methods",IF(E16="SISO","siso_methods",IF(E16="PT","pt_methods",IF(E16="DISO","diso_methods",IF(E16="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
+        <v>440</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="4" t="b">
+      <c r="F17" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H17" s="3" t="str">
+        <f>IF(D17="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H17" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I17" s="3" t="str">
+        <f>IF(E17="SIDO","single-input, double-output",IF(E17="SISO","single-input, single-output",IF(E17="PT","pass-through",IF(E17="DISO","double-input, single-output",IF(E17="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I17" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J17" s="3" t="str">
+        <f>IF(E17="SIDO","sido_methods",IF(E17="SISO","siso_methods",IF(E17="PT","pt_methods",IF(E17="DISO","diso_methods",IF(E17="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
+        <v>421</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="4" t="b">
+      <c r="F18" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I18" s="3" t="str">
+        <f>IF(E18="SIDO","single-input, double-output",IF(E18="SISO","single-input, single-output",IF(E18="PT","pass-through",IF(E18="DISO","double-input, single-output",IF(E18="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I18" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J18" s="3" t="str">
+        <f>IF(E18="SIDO","sido_methods",IF(E18="SISO","siso_methods",IF(E18="PT","pt_methods",IF(E18="DISO","diso_methods",IF(E18="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
+        <v>454</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="4" t="b">
+      <c r="F19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H19" s="3" t="b">
+        <f>IF(D19="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="H19" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I19" s="3" t="str">
+        <f>IF(E19="SIDO","single-input, double-output",IF(E19="SISO","single-input, single-output",IF(E19="PT","pass-through",IF(E19="DISO","double-input, single-output",IF(E19="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>double-input, single-output</v>
       </c>
-      <c r="I19" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J19" s="3" t="str">
+        <f>IF(E19="SIDO","sido_methods",IF(E19="SISO","siso_methods",IF(E19="PT","pt_methods",IF(E19="DISO","diso_methods",IF(E19="SIDO reactive","sidor_methods","")))))</f>
         <v>diso_methods</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
+        <v>455</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="4" t="b">
+      <c r="F20" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H20" s="3" t="b">
+        <f>IF(D20="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="H20" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I20" s="3" t="str">
+        <f>IF(E20="SIDO","single-input, double-output",IF(E20="SISO","single-input, single-output",IF(E20="PT","pass-through",IF(E20="DISO","double-input, single-output",IF(E20="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I20" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J20" s="3" t="str">
+        <f>IF(E20="SIDO","sido_methods",IF(E20="SISO","siso_methods",IF(E20="PT","pt_methods",IF(E20="DISO","diso_methods",IF(E20="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>383</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="4" t="b">
+      <c r="F21" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H21" s="3" t="str">
+        <f>IF(D21="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H21" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I21" s="3" t="str">
+        <f>IF(E21="SIDO","single-input, double-output",IF(E21="SISO","single-input, single-output",IF(E21="PT","pass-through",IF(E21="DISO","double-input, single-output",IF(E21="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I21" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J21" s="3" t="str">
+        <f>IF(E21="SIDO","sido_methods",IF(E21="SISO","siso_methods",IF(E21="PT","pt_methods",IF(E21="DISO","diso_methods",IF(E21="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
+        <v>395</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="4" t="b">
+      <c r="F22" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H22" s="3" t="str">
+        <f>IF(D22="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H22" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I22" s="3" t="str">
+        <f>IF(E22="SIDO","single-input, double-output",IF(E22="SISO","single-input, single-output",IF(E22="PT","pass-through",IF(E22="DISO","double-input, single-output",IF(E22="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I22" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J22" s="3" t="str">
+        <f>IF(E22="SIDO","sido_methods",IF(E22="SISO","siso_methods",IF(E22="PT","pt_methods",IF(E22="DISO","diso_methods",IF(E22="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
+        <v>384</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="4" t="b">
+      <c r="F23" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H23" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I23" s="3" t="str">
+        <f>IF(E23="SIDO","single-input, double-output",IF(E23="SISO","single-input, single-output",IF(E23="PT","pass-through",IF(E23="DISO","double-input, single-output",IF(E23="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I23" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J23" s="3" t="str">
+        <f>IF(E23="SIDO","sido_methods",IF(E23="SISO","siso_methods",IF(E23="PT","pt_methods",IF(E23="DISO","diso_methods",IF(E23="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
+        <v>396</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="4" t="b">
+      <c r="F24" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H24" s="3" t="str">
+        <f>IF(D24="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H24" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I24" s="3" t="str">
+        <f>IF(E24="SIDO","single-input, double-output",IF(E24="SISO","single-input, single-output",IF(E24="PT","pass-through",IF(E24="DISO","double-input, single-output",IF(E24="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I24" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J24" s="3" t="str">
+        <f>IF(E24="SIDO","sido_methods",IF(E24="SISO","siso_methods",IF(E24="PT","pt_methods",IF(E24="DISO","diso_methods",IF(E24="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
+        <v>385</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="4" t="b">
+      <c r="F25" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I25" s="3" t="str">
+        <f>IF(E25="SIDO","single-input, double-output",IF(E25="SISO","single-input, single-output",IF(E25="PT","pass-through",IF(E25="DISO","double-input, single-output",IF(E25="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I25" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J25" s="3" t="str">
+        <f>IF(E25="SIDO","sido_methods",IF(E25="SISO","siso_methods",IF(E25="PT","pt_methods",IF(E25="DISO","diso_methods",IF(E25="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
+        <v>397</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="4" t="b">
+      <c r="F26" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H26" s="3" t="str">
+        <f>IF(D26="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H26" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I26" s="3" t="str">
+        <f>IF(E26="SIDO","single-input, double-output",IF(E26="SISO","single-input, single-output",IF(E26="PT","pass-through",IF(E26="DISO","double-input, single-output",IF(E26="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I26" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J26" s="3" t="str">
+        <f>IF(E26="SIDO","sido_methods",IF(E26="SISO","siso_methods",IF(E26="PT","pt_methods",IF(E26="DISO","diso_methods",IF(E26="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
+        <v>386</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="4" t="b">
+      <c r="F27" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H27" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I27" s="3" t="str">
+        <f>IF(E27="SIDO","single-input, double-output",IF(E27="SISO","single-input, single-output",IF(E27="PT","pass-through",IF(E27="DISO","double-input, single-output",IF(E27="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="I27" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J27" s="3" t="str">
+        <f>IF(E27="SIDO","sido_methods",IF(E27="SISO","siso_methods",IF(E27="PT","pt_methods",IF(E27="DISO","diso_methods",IF(E27="SIDO reactive","sidor_methods","")))))</f>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="4" t="b">
+      <c r="F28" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H28" s="3" t="str">
+        <f>IF(D28="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H28" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I28" s="3" t="str">
+        <f>IF(E28="SIDO","single-input, double-output",IF(E28="SISO","single-input, single-output",IF(E28="PT","pass-through",IF(E28="DISO","double-input, single-output",IF(E28="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I28" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J28" s="3" t="str">
+        <f>IF(E28="SIDO","sido_methods",IF(E28="SISO","siso_methods",IF(E28="PT","pt_methods",IF(E28="DISO","diso_methods",IF(E28="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="4" t="b">
+      <c r="F29" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H29" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I29" s="3" t="str">
+        <f>IF(E29="SIDO","single-input, double-output",IF(E29="SISO","single-input, single-output",IF(E29="PT","pass-through",IF(E29="DISO","double-input, single-output",IF(E29="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="I29" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J29" s="3" t="str">
+        <f>IF(E29="SIDO","sido_methods",IF(E29="SISO","siso_methods",IF(E29="PT","pt_methods",IF(E29="DISO","diso_methods",IF(E29="SIDO reactive","sidor_methods","")))))</f>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" t="s">
+        <v>387</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="4" t="b">
+      <c r="F30" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H30" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I30" s="3" t="str">
+        <f>IF(E30="SIDO","single-input, double-output",IF(E30="SISO","single-input, single-output",IF(E30="PT","pass-through",IF(E30="DISO","double-input, single-output",IF(E30="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I30" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J30" s="3" t="str">
+        <f>IF(E30="SIDO","sido_methods",IF(E30="SISO","siso_methods",IF(E30="PT","pt_methods",IF(E30="DISO","diso_methods",IF(E30="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" t="s">
+        <v>401</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="4" t="b">
+      <c r="F31" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H31" s="3" t="str">
+        <f>IF(D31="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H31" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I31" s="3" t="str">
+        <f>IF(E31="SIDO","single-input, double-output",IF(E31="SISO","single-input, single-output",IF(E31="PT","pass-through",IF(E31="DISO","double-input, single-output",IF(E31="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I31" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J31" s="3" t="str">
+        <f>IF(E31="SIDO","sido_methods",IF(E31="SISO","siso_methods",IF(E31="PT","pt_methods",IF(E31="DISO","diso_methods",IF(E31="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
+        <v>442</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="4" t="b">
+      <c r="F32" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I32" s="3" t="str">
+        <f>IF(E32="SIDO","single-input, double-output",IF(E32="SISO","single-input, single-output",IF(E32="PT","pass-through",IF(E32="DISO","double-input, single-output",IF(E32="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I32" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J32" s="3" t="str">
+        <f>IF(E32="SIDO","sido_methods",IF(E32="SISO","siso_methods",IF(E32="PT","pt_methods",IF(E32="DISO","diso_methods",IF(E32="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
+        <v>398</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="4" t="b">
+      <c r="F33" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H33" s="3" t="str">
+        <f>IF(D33="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H33" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I33" s="3" t="str">
+        <f>IF(E33="SIDO","single-input, double-output",IF(E33="SISO","single-input, single-output",IF(E33="PT","pass-through",IF(E33="DISO","double-input, single-output",IF(E33="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I33" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J33" s="3" t="str">
+        <f>IF(E33="SIDO","sido_methods",IF(E33="SISO","siso_methods",IF(E33="PT","pt_methods",IF(E33="DISO","diso_methods",IF(E33="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
+        <v>399</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="4" t="b">
+      <c r="F34" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H34" s="3" t="b">
+        <f>IF(D34="basic","cost_power_law_flow")</f>
         <v>0</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J34" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
+        <v>443</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="4" t="b">
+      <c r="F35" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H35" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I35" s="3" t="str">
+        <f>IF(E35="SIDO","single-input, double-output",IF(E35="SISO","single-input, single-output",IF(E35="PT","pass-through",IF(E35="DISO","double-input, single-output",IF(E35="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I35" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J35" s="3" t="str">
+        <f>IF(E35="SIDO","sido_methods",IF(E35="SISO","siso_methods",IF(E35="PT","pt_methods",IF(E35="DISO","diso_methods",IF(E35="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" t="s">
+        <v>428</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="4" t="b">
+      <c r="F36" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H36" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I36" s="3" t="str">
+        <f>IF(E36="SIDO","single-input, double-output",IF(E36="SISO","single-input, single-output",IF(E36="PT","pass-through",IF(E36="DISO","double-input, single-output",IF(E36="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I36" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J36" s="3" t="str">
+        <f>IF(E36="SIDO","sido_methods",IF(E36="SISO","siso_methods",IF(E36="PT","pt_methods",IF(E36="DISO","diso_methods",IF(E36="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" t="s">
+        <v>434</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="4" t="b">
+      <c r="F37" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H37" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I37" s="3" t="str">
+        <f>IF(E37="SIDO","single-input, double-output",IF(E37="SISO","single-input, single-output",IF(E37="PT","pass-through",IF(E37="DISO","double-input, single-output",IF(E37="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I37" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J37" s="3" t="str">
+        <f>IF(E37="SIDO","sido_methods",IF(E37="SISO","siso_methods",IF(E37="PT","pt_methods",IF(E37="DISO","diso_methods",IF(E37="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
+        <v>456</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="4" t="b">
+      <c r="F38" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H38" s="3" t="b">
+        <f>IF(D38="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="I38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="J38" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
+        <v>447</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="4" t="b">
+      <c r="F39" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H39" s="3" t="str">
+        <f>IF(D39="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H39" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I39" s="3" t="str">
+        <f>IF(E39="SIDO","single-input, double-output",IF(E39="SISO","single-input, single-output",IF(E39="PT","pass-through",IF(E39="DISO","double-input, single-output",IF(E39="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I39" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J39" s="3" t="str">
+        <f>IF(E39="SIDO","sido_methods",IF(E39="SISO","siso_methods",IF(E39="PT","pt_methods",IF(E39="DISO","diso_methods",IF(E39="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
+        <v>446</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E40" s="4" t="b">
+      <c r="F40" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H40" s="3" t="str">
+        <f>IF(D40="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H40" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I40" s="3" t="str">
+        <f>IF(E40="SIDO","single-input, double-output",IF(E40="SISO","single-input, single-output",IF(E40="PT","pass-through",IF(E40="DISO","double-input, single-output",IF(E40="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I40" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J40" s="3" t="str">
+        <f>IF(E40="SIDO","sido_methods",IF(E40="SISO","siso_methods",IF(E40="PT","pt_methods",IF(E40="DISO","diso_methods",IF(E40="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" t="s">
+        <v>432</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="4" t="b">
+      <c r="F41" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H41" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I41" s="3" t="str">
+        <f>IF(E41="SIDO","single-input, double-output",IF(E41="SISO","single-input, single-output",IF(E41="PT","pass-through",IF(E41="DISO","double-input, single-output",IF(E41="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I41" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J41" s="3" t="str">
+        <f>IF(E41="SIDO","sido_methods",IF(E41="SISO","siso_methods",IF(E41="PT","pt_methods",IF(E41="DISO","diso_methods",IF(E41="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
+        <v>402</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="4" t="b">
+      <c r="F42" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H42" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I42" s="3" t="str">
+        <f>IF(E42="SIDO","single-input, double-output",IF(E42="SISO","single-input, single-output",IF(E42="PT","pass-through",IF(E42="DISO","double-input, single-output",IF(E42="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I42" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J42" s="3" t="str">
+        <f>IF(E42="SIDO","sido_methods",IF(E42="SISO","siso_methods",IF(E42="PT","pt_methods",IF(E42="DISO","diso_methods",IF(E42="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
+        <v>403</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="4" t="b">
+      <c r="F43" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H43" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I43" s="3" t="str">
+        <f>IF(E43="SIDO","single-input, double-output",IF(E43="SISO","single-input, single-output",IF(E43="PT","pass-through",IF(E43="DISO","double-input, single-output",IF(E43="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I43" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J43" s="3" t="str">
+        <f>IF(E43="SIDO","sido_methods",IF(E43="SISO","siso_methods",IF(E43="PT","pt_methods",IF(E43="DISO","diso_methods",IF(E43="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
+        <v>405</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="4" t="b">
+      <c r="F44" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H44" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I44" s="3" t="str">
+        <f>IF(E44="SIDO","single-input, double-output",IF(E44="SISO","single-input, single-output",IF(E44="PT","pass-through",IF(E44="DISO","double-input, single-output",IF(E44="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="I44" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J44" s="3" t="str">
+        <f>IF(E44="SIDO","sido_methods",IF(E44="SISO","siso_methods",IF(E44="PT","pt_methods",IF(E44="DISO","diso_methods",IF(E44="SIDO reactive","sidor_methods","")))))</f>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
+        <v>406</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="4" t="b">
+      <c r="F45" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H45" s="3" t="str">
+        <f>IF(D45="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H45" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I45" s="3" t="str">
+        <f>IF(E45="SIDO","single-input, double-output",IF(E45="SISO","single-input, single-output",IF(E45="PT","pass-through",IF(E45="DISO","double-input, single-output",IF(E45="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I45" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J45" s="3" t="str">
+        <f>IF(E45="SIDO","sido_methods",IF(E45="SISO","siso_methods",IF(E45="PT","pt_methods",IF(E45="DISO","diso_methods",IF(E45="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" t="s">
+        <v>407</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="4" t="b">
+      <c r="F46" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H46" s="3" t="str">
+        <f>IF(D46="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H46" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I46" s="3" t="str">
+        <f>IF(E46="SIDO","single-input, double-output",IF(E46="SISO","single-input, single-output",IF(E46="PT","pass-through",IF(E46="DISO","double-input, single-output",IF(E46="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I46" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J46" s="3" t="str">
+        <f>IF(E46="SIDO","sido_methods",IF(E46="SISO","siso_methods",IF(E46="PT","pt_methods",IF(E46="DISO","diso_methods",IF(E46="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
+        <v>391</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="4" t="b">
+      <c r="F47" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="H47" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I47" s="3" t="str">
+        <f>IF(E47="SIDO","single-input, double-output",IF(E47="SISO","single-input, single-output",IF(E47="PT","pass-through",IF(E47="DISO","double-input, single-output",IF(E47="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="I47" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J47" s="3" t="str">
+        <f>IF(E47="SIDO","sido_methods",IF(E47="SISO","siso_methods",IF(E47="PT","pt_methods",IF(E47="DISO","diso_methods",IF(E47="SIDO reactive","sidor_methods","")))))</f>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" t="s">
+        <v>408</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="4" t="b">
+      <c r="F48" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G48" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H48" s="3" t="str">
+        <f>IF(D48="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H48" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I48" s="3" t="str">
+        <f>IF(E48="SIDO","single-input, double-output",IF(E48="SISO","single-input, single-output",IF(E48="PT","pass-through",IF(E48="DISO","double-input, single-output",IF(E48="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I48" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J48" s="3" t="str">
+        <f>IF(E48="SIDO","sido_methods",IF(E48="SISO","siso_methods",IF(E48="PT","pt_methods",IF(E48="DISO","diso_methods",IF(E48="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" t="s">
+        <v>409</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="4" t="b">
+      <c r="F49" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H49" s="3" t="str">
+        <f>IF(D49="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H49" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I49" s="3" t="str">
+        <f>IF(E49="SIDO","single-input, double-output",IF(E49="SISO","single-input, single-output",IF(E49="PT","pass-through",IF(E49="DISO","double-input, single-output",IF(E49="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I49" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J49" s="3" t="str">
+        <f>IF(E49="SIDO","sido_methods",IF(E49="SISO","siso_methods",IF(E49="PT","pt_methods",IF(E49="DISO","diso_methods",IF(E49="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" t="s">
+        <v>429</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="4" t="b">
+      <c r="F50" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H50" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I50" s="3" t="str">
+        <f>IF(E50="SIDO","single-input, double-output",IF(E50="SISO","single-input, single-output",IF(E50="PT","pass-through",IF(E50="DISO","double-input, single-output",IF(E50="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I50" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J50" s="3" t="str">
+        <f>IF(E50="SIDO","sido_methods",IF(E50="SISO","siso_methods",IF(E50="PT","pt_methods",IF(E50="DISO","diso_methods",IF(E50="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" t="s">
+        <v>410</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="4" t="b">
+      <c r="F51" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="G51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H51" s="3" t="str">
+        <f>IF(D51="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H51" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I51" s="3" t="str">
+        <f>IF(E51="SIDO","single-input, double-output",IF(E51="SISO","single-input, single-output",IF(E51="PT","pass-through",IF(E51="DISO","double-input, single-output",IF(E51="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I51" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J51" s="3" t="str">
+        <f>IF(E51="SIDO","sido_methods",IF(E51="SISO","siso_methods",IF(E51="PT","pt_methods",IF(E51="DISO","diso_methods",IF(E51="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" t="s">
+        <v>411</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="4" t="b">
+      <c r="F52" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H52" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I52" s="3" t="str">
+        <f>IF(E52="SIDO","single-input, double-output",IF(E52="SISO","single-input, single-output",IF(E52="PT","pass-through",IF(E52="DISO","double-input, single-output",IF(E52="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I52" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J52" s="3" t="str">
+        <f>IF(E52="SIDO","sido_methods",IF(E52="SISO","siso_methods",IF(E52="PT","pt_methods",IF(E52="DISO","diso_methods",IF(E52="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" t="s">
+        <v>431</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="4" t="b">
+      <c r="F53" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H53" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I53" s="3" t="str">
+        <f>IF(E53="SIDO","single-input, double-output",IF(E53="SISO","single-input, single-output",IF(E53="PT","pass-through",IF(E53="DISO","double-input, single-output",IF(E53="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I53" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J53" s="3" t="str">
+        <f>IF(E53="SIDO","sido_methods",IF(E53="SISO","siso_methods",IF(E53="PT","pt_methods",IF(E53="DISO","diso_methods",IF(E53="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" t="s">
+        <v>430</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E54" s="4" t="b">
+      <c r="F54" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="H54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H54" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I54" s="3" t="str">
+        <f>IF(E54="SIDO","single-input, double-output",IF(E54="SISO","single-input, single-output",IF(E54="PT","pass-through",IF(E54="DISO","double-input, single-output",IF(E54="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I54" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J54" s="3" t="str">
+        <f>IF(E54="SIDO","sido_methods",IF(E54="SISO","siso_methods",IF(E54="PT","pt_methods",IF(E54="DISO","diso_methods",IF(E54="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" t="s">
+        <v>449</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="4" t="b">
+      <c r="F55" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="H55" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="H55" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I55" s="3" t="str">
+        <f>IF(E55="SIDO","single-input, double-output",IF(E55="SISO","single-input, single-output",IF(E55="PT","pass-through",IF(E55="DISO","double-input, single-output",IF(E55="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I55" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J55" s="3" t="str">
+        <f>IF(E55="SIDO","sido_methods",IF(E55="SISO","siso_methods",IF(E55="PT","pt_methods",IF(E55="DISO","diso_methods",IF(E55="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" t="s">
+        <v>413</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="4" t="b">
+      <c r="F56" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G56" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H56" s="3" t="str">
+        <f>IF(D56="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H56" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I56" s="3" t="str">
+        <f>IF(E56="SIDO","single-input, double-output",IF(E56="SISO","single-input, single-output",IF(E56="PT","pass-through",IF(E56="DISO","double-input, single-output",IF(E56="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I56" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J56" s="3" t="str">
+        <f>IF(E56="SIDO","sido_methods",IF(E56="SISO","siso_methods",IF(E56="PT","pt_methods",IF(E56="DISO","diso_methods",IF(E56="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" t="s">
+        <v>404</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="4" t="b">
+      <c r="F57" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H57" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I57" s="3" t="str">
+        <f>IF(E57="SIDO","single-input, double-output",IF(E57="SISO","single-input, single-output",IF(E57="PT","pass-through",IF(E57="DISO","double-input, single-output",IF(E57="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I57" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J57" s="3" t="str">
+        <f>IF(E57="SIDO","sido_methods",IF(E57="SISO","siso_methods",IF(E57="PT","pt_methods",IF(E57="DISO","diso_methods",IF(E57="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" t="s">
+        <v>414</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E58" s="4" t="b">
+      <c r="F58" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G58" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H58" s="3" t="str">
+        <f>IF(D58="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H58" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I58" s="3" t="str">
+        <f>IF(E58="SIDO","single-input, double-output",IF(E58="SISO","single-input, single-output",IF(E58="PT","pass-through",IF(E58="DISO","double-input, single-output",IF(E58="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I58" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J58" s="3" t="str">
+        <f>IF(E58="SIDO","sido_methods",IF(E58="SISO","siso_methods",IF(E58="PT","pt_methods",IF(E58="DISO","diso_methods",IF(E58="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" t="s">
+        <v>415</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E59" s="4" t="b">
+      <c r="F59" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G59" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H59" s="3" t="str">
+        <f>IF(D59="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H59" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I59" s="3" t="str">
+        <f>IF(E59="SIDO","single-input, double-output",IF(E59="SISO","single-input, single-output",IF(E59="PT","pass-through",IF(E59="DISO","double-input, single-output",IF(E59="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I59" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J59" s="3" t="str">
+        <f>IF(E59="SIDO","sido_methods",IF(E59="SISO","siso_methods",IF(E59="PT","pt_methods",IF(E59="DISO","diso_methods",IF(E59="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>160</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" t="s">
+        <v>453</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="4" t="b">
+      <c r="F60" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H60" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I60" s="3" t="str">
+        <f>IF(E60="SIDO","single-input, double-output",IF(E60="SISO","single-input, single-output",IF(E60="PT","pass-through",IF(E60="DISO","double-input, single-output",IF(E60="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I60" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J60" s="3" t="str">
+        <f>IF(E60="SIDO","sido_methods",IF(E60="SISO","siso_methods",IF(E60="PT","pt_methods",IF(E60="DISO","diso_methods",IF(E60="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" t="s">
+        <v>416</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="4" t="b">
+      <c r="F61" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="H61" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I61" s="3" t="str">
+        <f>IF(E61="SIDO","single-input, double-output",IF(E61="SISO","single-input, single-output",IF(E61="PT","pass-through",IF(E61="DISO","double-input, single-output",IF(E61="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I61" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J61" s="3" t="str">
+        <f>IF(E61="SIDO","sido_methods",IF(E61="SISO","siso_methods",IF(E61="PT","pt_methods",IF(E61="DISO","diso_methods",IF(E61="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" t="s">
+        <v>417</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="4" t="b">
+      <c r="F62" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G62" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H62" s="3" t="str">
+        <f>IF(D62="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H62" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I62" s="3" t="str">
+        <f>IF(E62="SIDO","single-input, double-output",IF(E62="SISO","single-input, single-output",IF(E62="PT","pass-through",IF(E62="DISO","double-input, single-output",IF(E62="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I62" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J62" s="3" t="str">
+        <f>IF(E62="SIDO","sido_methods",IF(E62="SISO","siso_methods",IF(E62="PT","pt_methods",IF(E62="DISO","diso_methods",IF(E62="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" t="s">
+        <v>441</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E63" s="4" t="b">
+      <c r="F63" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G63" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H63" s="3" t="str">
+        <f>IF(D63="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H63" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I63" s="3" t="str">
+        <f>IF(E63="SIDO","single-input, double-output",IF(E63="SISO","single-input, single-output",IF(E63="PT","pass-through",IF(E63="DISO","double-input, single-output",IF(E63="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I63" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J63" s="3" t="str">
+        <f>IF(E63="SIDO","sido_methods",IF(E63="SISO","siso_methods",IF(E63="PT","pt_methods",IF(E63="DISO","diso_methods",IF(E63="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>169</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" t="s">
+        <v>418</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E64" s="4" t="b">
+      <c r="F64" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="G64" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G64" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H64" s="3" t="str">
+        <f>IF(D64="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H64" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I64" s="3" t="str">
+        <f>IF(E64="SIDO","single-input, double-output",IF(E64="SISO","single-input, single-output",IF(E64="PT","pass-through",IF(E64="DISO","double-input, single-output",IF(E64="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I64" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J64" s="3" t="str">
+        <f>IF(E64="SIDO","sido_methods",IF(E64="SISO","siso_methods",IF(E64="PT","pt_methods",IF(E64="DISO","diso_methods",IF(E64="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" t="s">
+        <v>439</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E65" s="4" t="b">
+      <c r="F65" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G65" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H65" s="3" t="str">
+        <f>IF(D65="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H65" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I65" s="3" t="str">
+        <f>IF(E65="SIDO","single-input, double-output",IF(E65="SISO","single-input, single-output",IF(E65="PT","pass-through",IF(E65="DISO","double-input, single-output",IF(E65="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I65" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J65" s="3" t="str">
+        <f>IF(E65="SIDO","sido_methods",IF(E65="SISO","siso_methods",IF(E65="PT","pt_methods",IF(E65="DISO","diso_methods",IF(E65="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" t="s">
+        <v>436</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E66" s="4" t="b">
+      <c r="F66" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H66" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I66" s="3" t="str">
+        <f>IF(E66="SIDO","single-input, double-output",IF(E66="SISO","single-input, single-output",IF(E66="PT","pass-through",IF(E66="DISO","double-input, single-output",IF(E66="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I66" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J66" s="3" t="str">
+        <f>IF(E66="SIDO","sido_methods",IF(E66="SISO","siso_methods",IF(E66="PT","pt_methods",IF(E66="DISO","diso_methods",IF(E66="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" t="s">
+        <v>448</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E67" s="4" t="b">
+      <c r="F67" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="H67" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H67" s="3" t="str">
-        <f t="shared" ref="H67:H78" si="3">IF(D67="SIDO","single-input, double-output",IF(D67="SISO","single-input, single-output",IF(D67="PT","pass-through",IF(D67="DISO","double-input, single-output",IF(D67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="I67" s="3" t="str">
+        <f>IF(E67="SIDO","single-input, double-output",IF(E67="SISO","single-input, single-output",IF(E67="PT","pass-through",IF(E67="DISO","double-input, single-output",IF(E67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I67" s="3" t="str">
-        <f t="shared" ref="I67:I78" si="4">IF(D67="SIDO","sido_methods",IF(D67="SISO","siso_methods",IF(D67="PT","pt_methods",IF(D67="DISO","diso_methods",IF(D67="SIDO reactive","sidor_methods","")))))</f>
+      <c r="J67" s="3" t="str">
+        <f>IF(E67="SIDO","sido_methods",IF(E67="SISO","siso_methods",IF(E67="PT","pt_methods",IF(E67="DISO","diso_methods",IF(E67="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>179</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" t="s">
+        <v>437</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E68" s="4" t="b">
+      <c r="F68" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G68" s="3" t="str">
-        <f t="shared" ref="G68:G76" si="5">IF(C68="basic","cost_power_law_flow")</f>
+      <c r="H68" s="3" t="str">
+        <f>IF(D68="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H68" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I68" s="3" t="str">
+        <f>IF(E68="SIDO","single-input, double-output",IF(E68="SISO","single-input, single-output",IF(E68="PT","pass-through",IF(E68="DISO","double-input, single-output",IF(E68="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I68" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J68" s="3" t="str">
+        <f>IF(E68="SIDO","sido_methods",IF(E68="SISO","siso_methods",IF(E68="PT","pt_methods",IF(E68="DISO","diso_methods",IF(E68="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" t="s">
+        <v>419</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E69" s="4" t="b">
+      <c r="F69" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="G69" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G69" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H69" s="3" t="str">
+        <f>IF(D69="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H69" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I69" s="3" t="str">
+        <f>IF(E69="SIDO","single-input, double-output",IF(E69="SISO","single-input, single-output",IF(E69="PT","pass-through",IF(E69="DISO","double-input, single-output",IF(E69="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I69" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J69" s="3" t="str">
+        <f>IF(E69="SIDO","sido_methods",IF(E69="SISO","siso_methods",IF(E69="PT","pt_methods",IF(E69="DISO","diso_methods",IF(E69="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" t="s">
+        <v>420</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="4" t="b">
+      <c r="F70" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G70" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H70" s="3" t="str">
+        <f>IF(D70="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H70" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I70" s="3" t="str">
+        <f>IF(E70="SIDO","single-input, double-output",IF(E70="SISO","single-input, single-output",IF(E70="PT","pass-through",IF(E70="DISO","double-input, single-output",IF(E70="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I70" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J70" s="3" t="str">
+        <f>IF(E70="SIDO","sido_methods",IF(E70="SISO","siso_methods",IF(E70="PT","pt_methods",IF(E70="DISO","diso_methods",IF(E70="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" t="s">
+        <v>422</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E71" s="4" t="b">
+      <c r="F71" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="G71" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G71" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H71" s="3" t="str">
+        <f>IF(D71="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H71" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I71" s="3" t="str">
+        <f>IF(E71="SIDO","single-input, double-output",IF(E71="SISO","single-input, single-output",IF(E71="PT","pass-through",IF(E71="DISO","double-input, single-output",IF(E71="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I71" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J71" s="3" t="str">
+        <f>IF(E71="SIDO","sido_methods",IF(E71="SISO","siso_methods",IF(E71="PT","pt_methods",IF(E71="DISO","diso_methods",IF(E71="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" t="s">
+        <v>424</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="4" t="b">
+      <c r="F72" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="G72" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G72" s="3" t="s">
+      <c r="H72" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H72" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I72" s="3" t="str">
+        <f>IF(E72="SIDO","single-input, double-output",IF(E72="SISO","single-input, single-output",IF(E72="PT","pass-through",IF(E72="DISO","double-input, single-output",IF(E72="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I72" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J72" s="3" t="str">
+        <f>IF(E72="SIDO","sido_methods",IF(E72="SISO","siso_methods",IF(E72="PT","pt_methods",IF(E72="DISO","diso_methods",IF(E72="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" t="s">
+        <v>423</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E73" s="4" t="b">
+      <c r="F73" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="G73" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="H73" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H73" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I73" s="3" t="str">
+        <f>IF(E73="SIDO","single-input, double-output",IF(E73="SISO","single-input, single-output",IF(E73="PT","pass-through",IF(E73="DISO","double-input, single-output",IF(E73="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="I73" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J73" s="3" t="str">
+        <f>IF(E73="SIDO","sido_methods",IF(E73="SISO","siso_methods",IF(E73="PT","pt_methods",IF(E73="DISO","diso_methods",IF(E73="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" t="s">
+        <v>459</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="4" t="b">
+      <c r="F74" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="G74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G74" s="3" t="b">
-        <f t="shared" si="5"/>
+      <c r="H74" s="3" t="b">
+        <f>IF(D74="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="H74" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I74" s="3" t="str">
+        <f>IF(E74="SIDO","single-input, double-output",IF(E74="SISO","single-input, single-output",IF(E74="PT","pass-through",IF(E74="DISO","double-input, single-output",IF(E74="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I74" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J74" s="3" t="str">
+        <f>IF(E74="SIDO","sido_methods",IF(E74="SISO","siso_methods",IF(E74="PT","pt_methods",IF(E74="DISO","diso_methods",IF(E74="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" t="s">
+        <v>426</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="4" t="b">
+      <c r="F75" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G75" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H75" s="3" t="str">
+        <f>IF(D75="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H75" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I75" s="3" t="str">
+        <f>IF(E75="SIDO","single-input, double-output",IF(E75="SISO","single-input, single-output",IF(E75="PT","pass-through",IF(E75="DISO","double-input, single-output",IF(E75="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I75" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J75" s="3" t="str">
+        <f>IF(E75="SIDO","sido_methods",IF(E75="SISO","siso_methods",IF(E75="PT","pt_methods",IF(E75="DISO","diso_methods",IF(E75="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" t="s">
+        <v>425</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E76" s="4" t="b">
+      <c r="F76" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="G76" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G76" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H76" s="3" t="str">
+        <f>IF(D76="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="H76" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I76" s="3" t="str">
+        <f>IF(E76="SIDO","single-input, double-output",IF(E76="SISO","single-input, single-output",IF(E76="PT","pass-through",IF(E76="DISO","double-input, single-output",IF(E76="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="I76" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J76" s="3" t="str">
+        <f>IF(E76="SIDO","sido_methods",IF(E76="SISO","siso_methods",IF(E76="PT","pt_methods",IF(E76="DISO","diso_methods",IF(E76="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" t="s">
+        <v>444</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E77" s="4" t="b">
+      <c r="F77" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="G77" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="H77" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H77" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I77" s="3" t="str">
+        <f>IF(E77="SIDO","single-input, double-output",IF(E77="SISO","single-input, single-output",IF(E77="PT","pass-through",IF(E77="DISO","double-input, single-output",IF(E77="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I77" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J77" s="3" t="str">
+        <f>IF(E77="SIDO","sido_methods",IF(E77="SISO","siso_methods",IF(E77="PT","pt_methods",IF(E77="DISO","diso_methods",IF(E77="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>201</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" t="s">
+        <v>445</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E78" s="4" t="b">
+      <c r="F78" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="G78" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H78" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="H78" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I78" s="3" t="str">
+        <f>IF(E78="SIDO","single-input, double-output",IF(E78="SISO","single-input, single-output",IF(E78="PT","pass-through",IF(E78="DISO","double-input, single-output",IF(E78="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="I78" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="J78" s="3" t="str">
+        <f>IF(E78="SIDO","sido_methods",IF(E78="SISO","siso_methods",IF(E78="PT","pt_methods",IF(E78="DISO","diso_methods",IF(E78="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+    <sortCondition ref="B2:B78"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5540,12 +6031,661 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C80"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="37.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>376</v>
+      </c>
+      <c r="C9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>461</v>
+      </c>
+      <c r="C39" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" t="s">
+        <v>375</v>
+      </c>
+      <c r="C54" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B63" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B66" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B67" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B68" t="s">
+        <v>462</v>
+      </c>
+      <c r="C68" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B69" t="s">
+        <v>177</v>
+      </c>
+      <c r="C69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B70" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B71" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B72" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B73" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B75" t="s">
+        <v>191</v>
+      </c>
+      <c r="C75" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B76" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B77" t="s">
+        <v>196</v>
+      </c>
+      <c r="C77" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B78" t="s">
+        <v>198</v>
+      </c>
+      <c r="C78" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B79" t="s">
+        <v>200</v>
+      </c>
+      <c r="C79" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B80" t="s">
+        <v>202</v>
+      </c>
+      <c r="C80" t="s">
+        <v>445</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:C80">
+    <sortCondition ref="B1:B80"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
change municipal_drinking_zo to basic since it has no additional variables
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3159F15A-AF51-45D4-9255-499A24D3C4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C6B7C6-F553-4615-B270-3D97951EC2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1833,7 +1833,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1903,15 +1903,15 @@
         <v>12</v>
       </c>
       <c r="H2" s="3" t="str">
-        <f>IF(D2="basic","cost_power_law_flow")</f>
+        <f t="shared" ref="H2:H9" si="0">IF(D2="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
       <c r="I2" s="3" t="str">
-        <f>IF(E2="SIDO","single-input, double-output",IF(E2="SISO","single-input, single-output",IF(E2="PT","pass-through",IF(E2="DISO","double-input, single-output",IF(E2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" ref="I2:I33" si="1">IF(E2="SIDO","single-input, double-output",IF(E2="SISO","single-input, single-output",IF(E2="PT","pass-through",IF(E2="DISO","double-input, single-output",IF(E2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
       <c r="J2" s="3" t="str">
-        <f>IF(E2="SIDO","sido_methods",IF(E2="SISO","siso_methods",IF(E2="PT","pt_methods",IF(E2="DISO","diso_methods",IF(E2="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" ref="J2:J33" si="2">IF(E2="SIDO","sido_methods",IF(E2="SISO","siso_methods",IF(E2="PT","pt_methods",IF(E2="DISO","diso_methods",IF(E2="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
@@ -1938,15 +1938,15 @@
         <v>12</v>
       </c>
       <c r="H3" s="3" t="str">
-        <f>IF(D3="basic","cost_power_law_flow")</f>
+        <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
       <c r="I3" s="3" t="str">
-        <f>IF(E3="SIDO","single-input, double-output",IF(E3="SISO","single-input, single-output",IF(E3="PT","pass-through",IF(E3="DISO","double-input, single-output",IF(E3="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J3" s="3" t="str">
-        <f>IF(E3="SIDO","sido_methods",IF(E3="SISO","siso_methods",IF(E3="PT","pt_methods",IF(E3="DISO","diso_methods",IF(E3="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -1973,15 +1973,15 @@
         <v>12</v>
       </c>
       <c r="H4" s="3" t="str">
-        <f>IF(D4="basic","cost_power_law_flow")</f>
+        <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f>IF(E4="SIDO","single-input, double-output",IF(E4="SISO","single-input, single-output",IF(E4="PT","pass-through",IF(E4="DISO","double-input, single-output",IF(E4="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J4" s="3" t="str">
-        <f>IF(E4="SIDO","sido_methods",IF(E4="SISO","siso_methods",IF(E4="PT","pt_methods",IF(E4="DISO","diso_methods",IF(E4="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2008,15 +2008,15 @@
         <v>12</v>
       </c>
       <c r="H5" s="3" t="b">
-        <f>IF(D5="basic","cost_power_law_flow")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5" s="3" t="str">
-        <f>IF(E5="SIDO","single-input, double-output",IF(E5="SISO","single-input, single-output",IF(E5="PT","pass-through",IF(E5="DISO","double-input, single-output",IF(E5="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J5" s="3" t="str">
-        <f>IF(E5="SIDO","sido_methods",IF(E5="SISO","siso_methods",IF(E5="PT","pt_methods",IF(E5="DISO","diso_methods",IF(E5="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
@@ -2043,15 +2043,15 @@
         <v>23</v>
       </c>
       <c r="H6" s="3" t="str">
-        <f>IF(D6="basic","cost_power_law_flow")</f>
+        <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
       <c r="I6" s="3" t="str">
-        <f>IF(E6="SIDO","single-input, double-output",IF(E6="SISO","single-input, single-output",IF(E6="PT","pass-through",IF(E6="DISO","double-input, single-output",IF(E6="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J6" s="3" t="str">
-        <f>IF(E6="SIDO","sido_methods",IF(E6="SISO","siso_methods",IF(E6="PT","pt_methods",IF(E6="DISO","diso_methods",IF(E6="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2078,15 +2078,15 @@
         <v>12</v>
       </c>
       <c r="H7" s="3" t="str">
-        <f>IF(D7="basic","cost_power_law_flow")</f>
+        <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f>IF(E7="SIDO","single-input, double-output",IF(E7="SISO","single-input, single-output",IF(E7="PT","pass-through",IF(E7="DISO","double-input, single-output",IF(E7="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J7" s="3" t="str">
-        <f>IF(E7="SIDO","sido_methods",IF(E7="SISO","siso_methods",IF(E7="PT","pt_methods",IF(E7="DISO","diso_methods",IF(E7="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2113,15 +2113,15 @@
         <v>12</v>
       </c>
       <c r="H8" s="3" t="str">
-        <f>IF(D8="basic","cost_power_law_flow")</f>
+        <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f>IF(E8="SIDO","single-input, double-output",IF(E8="SISO","single-input, single-output",IF(E8="PT","pass-through",IF(E8="DISO","double-input, single-output",IF(E8="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J8" s="3" t="str">
-        <f>IF(E8="SIDO","sido_methods",IF(E8="SISO","siso_methods",IF(E8="PT","pt_methods",IF(E8="DISO","diso_methods",IF(E8="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -2148,15 +2148,15 @@
         <v>12</v>
       </c>
       <c r="H9" s="3" t="str">
-        <f>IF(D9="basic","cost_power_law_flow")</f>
+        <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
       <c r="I9" s="3" t="str">
-        <f>IF(E9="SIDO","single-input, double-output",IF(E9="SISO","single-input, single-output",IF(E9="PT","pass-through",IF(E9="DISO","double-input, single-output",IF(E9="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J9" s="3" t="str">
-        <f>IF(E9="SIDO","sido_methods",IF(E9="SISO","siso_methods",IF(E9="PT","pt_methods",IF(E9="DISO","diso_methods",IF(E9="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2186,11 +2186,11 @@
         <v>34</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f>IF(E10="SIDO","single-input, double-output",IF(E10="SISO","single-input, single-output",IF(E10="PT","pass-through",IF(E10="DISO","double-input, single-output",IF(E10="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J10" s="3" t="str">
-        <f>IF(E10="SIDO","sido_methods",IF(E10="SISO","siso_methods",IF(E10="PT","pt_methods",IF(E10="DISO","diso_methods",IF(E10="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2221,11 +2221,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I11" s="3" t="str">
-        <f>IF(E11="SIDO","single-input, double-output",IF(E11="SISO","single-input, single-output",IF(E11="PT","pass-through",IF(E11="DISO","double-input, single-output",IF(E11="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J11" s="3" t="str">
-        <f>IF(E11="SIDO","sido_methods",IF(E11="SISO","siso_methods",IF(E11="PT","pt_methods",IF(E11="DISO","diso_methods",IF(E11="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2255,11 +2255,11 @@
         <v>39</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f>IF(E12="SIDO","single-input, double-output",IF(E12="SISO","single-input, single-output",IF(E12="PT","pass-through",IF(E12="DISO","double-input, single-output",IF(E12="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J12" s="3" t="str">
-        <f>IF(E12="SIDO","sido_methods",IF(E12="SISO","siso_methods",IF(E12="PT","pt_methods",IF(E12="DISO","diso_methods",IF(E12="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
@@ -2290,11 +2290,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f>IF(E13="SIDO","single-input, double-output",IF(E13="SISO","single-input, single-output",IF(E13="PT","pass-through",IF(E13="DISO","double-input, single-output",IF(E13="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J13" s="3" t="str">
-        <f>IF(E13="SIDO","sido_methods",IF(E13="SISO","siso_methods",IF(E13="PT","pt_methods",IF(E13="DISO","diso_methods",IF(E13="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2324,11 +2324,11 @@
         <v>44</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f>IF(E14="SIDO","single-input, double-output",IF(E14="SISO","single-input, single-output",IF(E14="PT","pass-through",IF(E14="DISO","double-input, single-output",IF(E14="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J14" s="3" t="str">
-        <f>IF(E14="SIDO","sido_methods",IF(E14="SISO","siso_methods",IF(E14="PT","pt_methods",IF(E14="DISO","diso_methods",IF(E14="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2358,11 +2358,11 @@
         <v>47</v>
       </c>
       <c r="I15" s="3" t="str">
-        <f>IF(E15="SIDO","single-input, double-output",IF(E15="SISO","single-input, single-output",IF(E15="PT","pass-through",IF(E15="DISO","double-input, single-output",IF(E15="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J15" s="3" t="str">
-        <f>IF(E15="SIDO","sido_methods",IF(E15="SISO","siso_methods",IF(E15="PT","pt_methods",IF(E15="DISO","diso_methods",IF(E15="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -2393,11 +2393,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f>IF(E16="SIDO","single-input, double-output",IF(E16="SISO","single-input, single-output",IF(E16="PT","pass-through",IF(E16="DISO","double-input, single-output",IF(E16="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J16" s="3" t="str">
-        <f>IF(E16="SIDO","sido_methods",IF(E16="SISO","siso_methods",IF(E16="PT","pt_methods",IF(E16="DISO","diso_methods",IF(E16="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2428,11 +2428,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I17" s="3" t="str">
-        <f>IF(E17="SIDO","single-input, double-output",IF(E17="SISO","single-input, single-output",IF(E17="PT","pass-through",IF(E17="DISO","double-input, single-output",IF(E17="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J17" s="3" t="str">
-        <f>IF(E17="SIDO","sido_methods",IF(E17="SISO","siso_methods",IF(E17="PT","pt_methods",IF(E17="DISO","diso_methods",IF(E17="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2462,11 +2462,11 @@
         <v>54</v>
       </c>
       <c r="I18" s="3" t="str">
-        <f>IF(E18="SIDO","single-input, double-output",IF(E18="SISO","single-input, single-output",IF(E18="PT","pass-through",IF(E18="DISO","double-input, single-output",IF(E18="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J18" s="3" t="str">
-        <f>IF(E18="SIDO","sido_methods",IF(E18="SISO","siso_methods",IF(E18="PT","pt_methods",IF(E18="DISO","diso_methods",IF(E18="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2497,11 +2497,11 @@
         <v>0</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f>IF(E19="SIDO","single-input, double-output",IF(E19="SISO","single-input, single-output",IF(E19="PT","pass-through",IF(E19="DISO","double-input, single-output",IF(E19="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>double-input, single-output</v>
       </c>
       <c r="J19" s="3" t="str">
-        <f>IF(E19="SIDO","sido_methods",IF(E19="SISO","siso_methods",IF(E19="PT","pt_methods",IF(E19="DISO","diso_methods",IF(E19="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>diso_methods</v>
       </c>
     </row>
@@ -2532,11 +2532,11 @@
         <v>0</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f>IF(E20="SIDO","single-input, double-output",IF(E20="SISO","single-input, single-output",IF(E20="PT","pass-through",IF(E20="DISO","double-input, single-output",IF(E20="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J20" s="3" t="str">
-        <f>IF(E20="SIDO","sido_methods",IF(E20="SISO","siso_methods",IF(E20="PT","pt_methods",IF(E20="DISO","diso_methods",IF(E20="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -2567,11 +2567,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f>IF(E21="SIDO","single-input, double-output",IF(E21="SISO","single-input, single-output",IF(E21="PT","pass-through",IF(E21="DISO","double-input, single-output",IF(E21="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J21" s="3" t="str">
-        <f>IF(E21="SIDO","sido_methods",IF(E21="SISO","siso_methods",IF(E21="PT","pt_methods",IF(E21="DISO","diso_methods",IF(E21="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2602,11 +2602,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f>IF(E22="SIDO","single-input, double-output",IF(E22="SISO","single-input, single-output",IF(E22="PT","pass-through",IF(E22="DISO","double-input, single-output",IF(E22="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f>IF(E22="SIDO","sido_methods",IF(E22="SISO","siso_methods",IF(E22="PT","pt_methods",IF(E22="DISO","diso_methods",IF(E22="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2636,11 +2636,11 @@
         <v>68</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f>IF(E23="SIDO","single-input, double-output",IF(E23="SISO","single-input, single-output",IF(E23="PT","pass-through",IF(E23="DISO","double-input, single-output",IF(E23="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J23" s="3" t="str">
-        <f>IF(E23="SIDO","sido_methods",IF(E23="SISO","siso_methods",IF(E23="PT","pt_methods",IF(E23="DISO","diso_methods",IF(E23="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2671,11 +2671,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I24" s="3" t="str">
-        <f>IF(E24="SIDO","single-input, double-output",IF(E24="SISO","single-input, single-output",IF(E24="PT","pass-through",IF(E24="DISO","double-input, single-output",IF(E24="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J24" s="3" t="str">
-        <f>IF(E24="SIDO","sido_methods",IF(E24="SISO","siso_methods",IF(E24="PT","pt_methods",IF(E24="DISO","diso_methods",IF(E24="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -2705,11 +2705,11 @@
         <v>73</v>
       </c>
       <c r="I25" s="3" t="str">
-        <f>IF(E25="SIDO","single-input, double-output",IF(E25="SISO","single-input, single-output",IF(E25="PT","pass-through",IF(E25="DISO","double-input, single-output",IF(E25="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J25" s="3" t="str">
-        <f>IF(E25="SIDO","sido_methods",IF(E25="SISO","siso_methods",IF(E25="PT","pt_methods",IF(E25="DISO","diso_methods",IF(E25="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2740,11 +2740,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I26" s="3" t="str">
-        <f>IF(E26="SIDO","single-input, double-output",IF(E26="SISO","single-input, single-output",IF(E26="PT","pass-through",IF(E26="DISO","double-input, single-output",IF(E26="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J26" s="3" t="str">
-        <f>IF(E26="SIDO","sido_methods",IF(E26="SISO","siso_methods",IF(E26="PT","pt_methods",IF(E26="DISO","diso_methods",IF(E26="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2774,11 +2774,11 @@
         <v>78</v>
       </c>
       <c r="I27" s="3" t="str">
-        <f>IF(E27="SIDO","single-input, double-output",IF(E27="SISO","single-input, single-output",IF(E27="PT","pass-through",IF(E27="DISO","double-input, single-output",IF(E27="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J27" s="3" t="str">
-        <f>IF(E27="SIDO","sido_methods",IF(E27="SISO","siso_methods",IF(E27="PT","pt_methods",IF(E27="DISO","diso_methods",IF(E27="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
@@ -2809,11 +2809,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I28" s="3" t="str">
-        <f>IF(E28="SIDO","single-input, double-output",IF(E28="SISO","single-input, single-output",IF(E28="PT","pass-through",IF(E28="DISO","double-input, single-output",IF(E28="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J28" s="3" t="str">
-        <f>IF(E28="SIDO","sido_methods",IF(E28="SISO","siso_methods",IF(E28="PT","pt_methods",IF(E28="DISO","diso_methods",IF(E28="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2843,11 +2843,11 @@
         <v>83</v>
       </c>
       <c r="I29" s="3" t="str">
-        <f>IF(E29="SIDO","single-input, double-output",IF(E29="SISO","single-input, single-output",IF(E29="PT","pass-through",IF(E29="DISO","double-input, single-output",IF(E29="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J29" s="3" t="str">
-        <f>IF(E29="SIDO","sido_methods",IF(E29="SISO","siso_methods",IF(E29="PT","pt_methods",IF(E29="DISO","diso_methods",IF(E29="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
@@ -2877,11 +2877,11 @@
         <v>68</v>
       </c>
       <c r="I30" s="3" t="str">
-        <f>IF(E30="SIDO","single-input, double-output",IF(E30="SISO","single-input, single-output",IF(E30="PT","pass-through",IF(E30="DISO","double-input, single-output",IF(E30="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J30" s="3" t="str">
-        <f>IF(E30="SIDO","sido_methods",IF(E30="SISO","siso_methods",IF(E30="PT","pt_methods",IF(E30="DISO","diso_methods",IF(E30="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2912,11 +2912,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I31" s="3" t="str">
-        <f>IF(E31="SIDO","single-input, double-output",IF(E31="SISO","single-input, single-output",IF(E31="PT","pass-through",IF(E31="DISO","double-input, single-output",IF(E31="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J31" s="3" t="str">
-        <f>IF(E31="SIDO","sido_methods",IF(E31="SISO","siso_methods",IF(E31="PT","pt_methods",IF(E31="DISO","diso_methods",IF(E31="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -2946,11 +2946,11 @@
         <v>90</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f>IF(E32="SIDO","single-input, double-output",IF(E32="SISO","single-input, single-output",IF(E32="PT","pass-through",IF(E32="DISO","double-input, single-output",IF(E32="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J32" s="3" t="str">
-        <f>IF(E32="SIDO","sido_methods",IF(E32="SISO","siso_methods",IF(E32="PT","pt_methods",IF(E32="DISO","diso_methods",IF(E32="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -2981,11 +2981,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I33" s="3" t="str">
-        <f>IF(E33="SIDO","single-input, double-output",IF(E33="SISO","single-input, single-output",IF(E33="PT","pass-through",IF(E33="DISO","double-input, single-output",IF(E33="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
       <c r="J33" s="3" t="str">
-        <f>IF(E33="SIDO","sido_methods",IF(E33="SISO","siso_methods",IF(E33="PT","pt_methods",IF(E33="DISO","diso_methods",IF(E33="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3184,11 +3184,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I39" s="3" t="str">
-        <f>IF(E39="SIDO","single-input, double-output",IF(E39="SISO","single-input, single-output",IF(E39="PT","pass-through",IF(E39="DISO","double-input, single-output",IF(E39="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" ref="I39:I78" si="3">IF(E39="SIDO","single-input, double-output",IF(E39="SISO","single-input, single-output",IF(E39="PT","pass-through",IF(E39="DISO","double-input, single-output",IF(E39="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
       <c r="J39" s="3" t="str">
-        <f>IF(E39="SIDO","sido_methods",IF(E39="SISO","siso_methods",IF(E39="PT","pt_methods",IF(E39="DISO","diso_methods",IF(E39="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" ref="J39:J78" si="4">IF(E39="SIDO","sido_methods",IF(E39="SISO","siso_methods",IF(E39="PT","pt_methods",IF(E39="DISO","diso_methods",IF(E39="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3219,11 +3219,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I40" s="3" t="str">
-        <f>IF(E40="SIDO","single-input, double-output",IF(E40="SISO","single-input, single-output",IF(E40="PT","pass-through",IF(E40="DISO","double-input, single-output",IF(E40="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J40" s="3" t="str">
-        <f>IF(E40="SIDO","sido_methods",IF(E40="SISO","siso_methods",IF(E40="PT","pt_methods",IF(E40="DISO","diso_methods",IF(E40="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3253,11 +3253,11 @@
         <v>115</v>
       </c>
       <c r="I41" s="3" t="str">
-        <f>IF(E41="SIDO","single-input, double-output",IF(E41="SISO","single-input, single-output",IF(E41="PT","pass-through",IF(E41="DISO","double-input, single-output",IF(E41="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J41" s="3" t="str">
-        <f>IF(E41="SIDO","sido_methods",IF(E41="SISO","siso_methods",IF(E41="PT","pt_methods",IF(E41="DISO","diso_methods",IF(E41="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3287,11 +3287,11 @@
         <v>118</v>
       </c>
       <c r="I42" s="3" t="str">
-        <f>IF(E42="SIDO","single-input, double-output",IF(E42="SISO","single-input, single-output",IF(E42="PT","pass-through",IF(E42="DISO","double-input, single-output",IF(E42="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J42" s="3" t="str">
-        <f>IF(E42="SIDO","sido_methods",IF(E42="SISO","siso_methods",IF(E42="PT","pt_methods",IF(E42="DISO","diso_methods",IF(E42="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3321,11 +3321,11 @@
         <v>121</v>
       </c>
       <c r="I43" s="3" t="str">
-        <f>IF(E43="SIDO","single-input, double-output",IF(E43="SISO","single-input, single-output",IF(E43="PT","pass-through",IF(E43="DISO","double-input, single-output",IF(E43="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J43" s="3" t="str">
-        <f>IF(E43="SIDO","sido_methods",IF(E43="SISO","siso_methods",IF(E43="PT","pt_methods",IF(E43="DISO","diso_methods",IF(E43="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3355,11 +3355,11 @@
         <v>124</v>
       </c>
       <c r="I44" s="3" t="str">
-        <f>IF(E44="SIDO","single-input, double-output",IF(E44="SISO","single-input, single-output",IF(E44="PT","pass-through",IF(E44="DISO","double-input, single-output",IF(E44="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J44" s="3" t="str">
-        <f>IF(E44="SIDO","sido_methods",IF(E44="SISO","siso_methods",IF(E44="PT","pt_methods",IF(E44="DISO","diso_methods",IF(E44="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sidor_methods</v>
       </c>
     </row>
@@ -3390,11 +3390,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I45" s="3" t="str">
-        <f>IF(E45="SIDO","single-input, double-output",IF(E45="SISO","single-input, single-output",IF(E45="PT","pass-through",IF(E45="DISO","double-input, single-output",IF(E45="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J45" s="3" t="str">
-        <f>IF(E45="SIDO","sido_methods",IF(E45="SISO","siso_methods",IF(E45="PT","pt_methods",IF(E45="DISO","diso_methods",IF(E45="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3425,11 +3425,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I46" s="3" t="str">
-        <f>IF(E46="SIDO","single-input, double-output",IF(E46="SISO","single-input, single-output",IF(E46="PT","pass-through",IF(E46="DISO","double-input, single-output",IF(E46="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J46" s="3" t="str">
-        <f>IF(E46="SIDO","sido_methods",IF(E46="SISO","siso_methods",IF(E46="PT","pt_methods",IF(E46="DISO","diso_methods",IF(E46="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3459,11 +3459,11 @@
         <v>131</v>
       </c>
       <c r="I47" s="3" t="str">
-        <f>IF(E47="SIDO","single-input, double-output",IF(E47="SISO","single-input, single-output",IF(E47="PT","pass-through",IF(E47="DISO","double-input, single-output",IF(E47="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J47" s="3" t="str">
-        <f>IF(E47="SIDO","sido_methods",IF(E47="SISO","siso_methods",IF(E47="PT","pt_methods",IF(E47="DISO","diso_methods",IF(E47="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sidor_methods</v>
       </c>
     </row>
@@ -3494,11 +3494,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I48" s="3" t="str">
-        <f>IF(E48="SIDO","single-input, double-output",IF(E48="SISO","single-input, single-output",IF(E48="PT","pass-through",IF(E48="DISO","double-input, single-output",IF(E48="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J48" s="3" t="str">
-        <f>IF(E48="SIDO","sido_methods",IF(E48="SISO","siso_methods",IF(E48="PT","pt_methods",IF(E48="DISO","diso_methods",IF(E48="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3529,11 +3529,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I49" s="3" t="str">
-        <f>IF(E49="SIDO","single-input, double-output",IF(E49="SISO","single-input, single-output",IF(E49="PT","pass-through",IF(E49="DISO","double-input, single-output",IF(E49="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J49" s="3" t="str">
-        <f>IF(E49="SIDO","sido_methods",IF(E49="SISO","siso_methods",IF(E49="PT","pt_methods",IF(E49="DISO","diso_methods",IF(E49="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3548,7 +3548,7 @@
         <v>429</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>29</v>
@@ -3563,11 +3563,11 @@
         <v>68</v>
       </c>
       <c r="I50" s="3" t="str">
-        <f>IF(E50="SIDO","single-input, double-output",IF(E50="SISO","single-input, single-output",IF(E50="PT","pass-through",IF(E50="DISO","double-input, single-output",IF(E50="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J50" s="3" t="str">
-        <f>IF(E50="SIDO","sido_methods",IF(E50="SISO","siso_methods",IF(E50="PT","pt_methods",IF(E50="DISO","diso_methods",IF(E50="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3598,11 +3598,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I51" s="3" t="str">
-        <f>IF(E51="SIDO","single-input, double-output",IF(E51="SISO","single-input, single-output",IF(E51="PT","pass-through",IF(E51="DISO","double-input, single-output",IF(E51="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J51" s="3" t="str">
-        <f>IF(E51="SIDO","sido_methods",IF(E51="SISO","siso_methods",IF(E51="PT","pt_methods",IF(E51="DISO","diso_methods",IF(E51="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3632,11 +3632,11 @@
         <v>142</v>
       </c>
       <c r="I52" s="3" t="str">
-        <f>IF(E52="SIDO","single-input, double-output",IF(E52="SISO","single-input, single-output",IF(E52="PT","pass-through",IF(E52="DISO","double-input, single-output",IF(E52="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J52" s="3" t="str">
-        <f>IF(E52="SIDO","sido_methods",IF(E52="SISO","siso_methods",IF(E52="PT","pt_methods",IF(E52="DISO","diso_methods",IF(E52="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3666,11 +3666,11 @@
         <v>144</v>
       </c>
       <c r="I53" s="3" t="str">
-        <f>IF(E53="SIDO","single-input, double-output",IF(E53="SISO","single-input, single-output",IF(E53="PT","pass-through",IF(E53="DISO","double-input, single-output",IF(E53="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J53" s="3" t="str">
-        <f>IF(E53="SIDO","sido_methods",IF(E53="SISO","siso_methods",IF(E53="PT","pt_methods",IF(E53="DISO","diso_methods",IF(E53="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -3700,11 +3700,11 @@
         <v>147</v>
       </c>
       <c r="I54" s="3" t="str">
-        <f>IF(E54="SIDO","single-input, double-output",IF(E54="SISO","single-input, single-output",IF(E54="PT","pass-through",IF(E54="DISO","double-input, single-output",IF(E54="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J54" s="3" t="str">
-        <f>IF(E54="SIDO","sido_methods",IF(E54="SISO","siso_methods",IF(E54="PT","pt_methods",IF(E54="DISO","diso_methods",IF(E54="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -3734,11 +3734,11 @@
         <v>150</v>
       </c>
       <c r="I55" s="3" t="str">
-        <f>IF(E55="SIDO","single-input, double-output",IF(E55="SISO","single-input, single-output",IF(E55="PT","pass-through",IF(E55="DISO","double-input, single-output",IF(E55="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J55" s="3" t="str">
-        <f>IF(E55="SIDO","sido_methods",IF(E55="SISO","siso_methods",IF(E55="PT","pt_methods",IF(E55="DISO","diso_methods",IF(E55="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3769,11 +3769,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I56" s="3" t="str">
-        <f>IF(E56="SIDO","single-input, double-output",IF(E56="SISO","single-input, single-output",IF(E56="PT","pass-through",IF(E56="DISO","double-input, single-output",IF(E56="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J56" s="3" t="str">
-        <f>IF(E56="SIDO","sido_methods",IF(E56="SISO","siso_methods",IF(E56="PT","pt_methods",IF(E56="DISO","diso_methods",IF(E56="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3803,11 +3803,11 @@
         <v>155</v>
       </c>
       <c r="I57" s="3" t="str">
-        <f>IF(E57="SIDO","single-input, double-output",IF(E57="SISO","single-input, single-output",IF(E57="PT","pass-through",IF(E57="DISO","double-input, single-output",IF(E57="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J57" s="3" t="str">
-        <f>IF(E57="SIDO","sido_methods",IF(E57="SISO","siso_methods",IF(E57="PT","pt_methods",IF(E57="DISO","diso_methods",IF(E57="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3838,11 +3838,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I58" s="3" t="str">
-        <f>IF(E58="SIDO","single-input, double-output",IF(E58="SISO","single-input, single-output",IF(E58="PT","pass-through",IF(E58="DISO","double-input, single-output",IF(E58="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J58" s="3" t="str">
-        <f>IF(E58="SIDO","sido_methods",IF(E58="SISO","siso_methods",IF(E58="PT","pt_methods",IF(E58="DISO","diso_methods",IF(E58="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -3873,11 +3873,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I59" s="3" t="str">
-        <f>IF(E59="SIDO","single-input, double-output",IF(E59="SISO","single-input, single-output",IF(E59="PT","pass-through",IF(E59="DISO","double-input, single-output",IF(E59="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J59" s="3" t="str">
-        <f>IF(E59="SIDO","sido_methods",IF(E59="SISO","siso_methods",IF(E59="PT","pt_methods",IF(E59="DISO","diso_methods",IF(E59="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3907,11 +3907,11 @@
         <v>68</v>
       </c>
       <c r="I60" s="3" t="str">
-        <f>IF(E60="SIDO","single-input, double-output",IF(E60="SISO","single-input, single-output",IF(E60="PT","pass-through",IF(E60="DISO","double-input, single-output",IF(E60="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J60" s="3" t="str">
-        <f>IF(E60="SIDO","sido_methods",IF(E60="SISO","siso_methods",IF(E60="PT","pt_methods",IF(E60="DISO","diso_methods",IF(E60="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3941,11 +3941,11 @@
         <v>164</v>
       </c>
       <c r="I61" s="3" t="str">
-        <f>IF(E61="SIDO","single-input, double-output",IF(E61="SISO","single-input, single-output",IF(E61="PT","pass-through",IF(E61="DISO","double-input, single-output",IF(E61="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J61" s="3" t="str">
-        <f>IF(E61="SIDO","sido_methods",IF(E61="SISO","siso_methods",IF(E61="PT","pt_methods",IF(E61="DISO","diso_methods",IF(E61="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3976,11 +3976,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I62" s="3" t="str">
-        <f>IF(E62="SIDO","single-input, double-output",IF(E62="SISO","single-input, single-output",IF(E62="PT","pass-through",IF(E62="DISO","double-input, single-output",IF(E62="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J62" s="3" t="str">
-        <f>IF(E62="SIDO","sido_methods",IF(E62="SISO","siso_methods",IF(E62="PT","pt_methods",IF(E62="DISO","diso_methods",IF(E62="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -4011,11 +4011,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I63" s="3" t="str">
-        <f>IF(E63="SIDO","single-input, double-output",IF(E63="SISO","single-input, single-output",IF(E63="PT","pass-through",IF(E63="DISO","double-input, single-output",IF(E63="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J63" s="3" t="str">
-        <f>IF(E63="SIDO","sido_methods",IF(E63="SISO","siso_methods",IF(E63="PT","pt_methods",IF(E63="DISO","diso_methods",IF(E63="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -4046,11 +4046,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I64" s="3" t="str">
-        <f>IF(E64="SIDO","single-input, double-output",IF(E64="SISO","single-input, single-output",IF(E64="PT","pass-through",IF(E64="DISO","double-input, single-output",IF(E64="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J64" s="3" t="str">
-        <f>IF(E64="SIDO","sido_methods",IF(E64="SISO","siso_methods",IF(E64="PT","pt_methods",IF(E64="DISO","diso_methods",IF(E64="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -4081,11 +4081,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I65" s="3" t="str">
-        <f>IF(E65="SIDO","single-input, double-output",IF(E65="SISO","single-input, single-output",IF(E65="PT","pass-through",IF(E65="DISO","double-input, single-output",IF(E65="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J65" s="3" t="str">
-        <f>IF(E65="SIDO","sido_methods",IF(E65="SISO","siso_methods",IF(E65="PT","pt_methods",IF(E65="DISO","diso_methods",IF(E65="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -4115,11 +4115,11 @@
         <v>175</v>
       </c>
       <c r="I66" s="3" t="str">
-        <f>IF(E66="SIDO","single-input, double-output",IF(E66="SISO","single-input, single-output",IF(E66="PT","pass-through",IF(E66="DISO","double-input, single-output",IF(E66="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J66" s="3" t="str">
-        <f>IF(E66="SIDO","sido_methods",IF(E66="SISO","siso_methods",IF(E66="PT","pt_methods",IF(E66="DISO","diso_methods",IF(E66="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -4149,11 +4149,11 @@
         <v>178</v>
       </c>
       <c r="I67" s="3" t="str">
-        <f>IF(E67="SIDO","single-input, double-output",IF(E67="SISO","single-input, single-output",IF(E67="PT","pass-through",IF(E67="DISO","double-input, single-output",IF(E67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J67" s="3" t="str">
-        <f>IF(E67="SIDO","sido_methods",IF(E67="SISO","siso_methods",IF(E67="PT","pt_methods",IF(E67="DISO","diso_methods",IF(E67="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -4184,11 +4184,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I68" s="3" t="str">
-        <f>IF(E68="SIDO","single-input, double-output",IF(E68="SISO","single-input, single-output",IF(E68="PT","pass-through",IF(E68="DISO","double-input, single-output",IF(E68="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J68" s="3" t="str">
-        <f>IF(E68="SIDO","sido_methods",IF(E68="SISO","siso_methods",IF(E68="PT","pt_methods",IF(E68="DISO","diso_methods",IF(E68="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -4219,11 +4219,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I69" s="3" t="str">
-        <f>IF(E69="SIDO","single-input, double-output",IF(E69="SISO","single-input, single-output",IF(E69="PT","pass-through",IF(E69="DISO","double-input, single-output",IF(E69="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J69" s="3" t="str">
-        <f>IF(E69="SIDO","sido_methods",IF(E69="SISO","siso_methods",IF(E69="PT","pt_methods",IF(E69="DISO","diso_methods",IF(E69="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -4254,11 +4254,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I70" s="3" t="str">
-        <f>IF(E70="SIDO","single-input, double-output",IF(E70="SISO","single-input, single-output",IF(E70="PT","pass-through",IF(E70="DISO","double-input, single-output",IF(E70="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J70" s="3" t="str">
-        <f>IF(E70="SIDO","sido_methods",IF(E70="SISO","siso_methods",IF(E70="PT","pt_methods",IF(E70="DISO","diso_methods",IF(E70="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -4289,11 +4289,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I71" s="3" t="str">
-        <f>IF(E71="SIDO","single-input, double-output",IF(E71="SISO","single-input, single-output",IF(E71="PT","pass-through",IF(E71="DISO","double-input, single-output",IF(E71="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J71" s="3" t="str">
-        <f>IF(E71="SIDO","sido_methods",IF(E71="SISO","siso_methods",IF(E71="PT","pt_methods",IF(E71="DISO","diso_methods",IF(E71="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -4323,11 +4323,11 @@
         <v>189</v>
       </c>
       <c r="I72" s="3" t="str">
-        <f>IF(E72="SIDO","single-input, double-output",IF(E72="SISO","single-input, single-output",IF(E72="PT","pass-through",IF(E72="DISO","double-input, single-output",IF(E72="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J72" s="3" t="str">
-        <f>IF(E72="SIDO","sido_methods",IF(E72="SISO","siso_methods",IF(E72="PT","pt_methods",IF(E72="DISO","diso_methods",IF(E72="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -4357,11 +4357,11 @@
         <v>192</v>
       </c>
       <c r="I73" s="3" t="str">
-        <f>IF(E73="SIDO","single-input, double-output",IF(E73="SISO","single-input, single-output",IF(E73="PT","pass-through",IF(E73="DISO","double-input, single-output",IF(E73="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J73" s="3" t="str">
-        <f>IF(E73="SIDO","sido_methods",IF(E73="SISO","siso_methods",IF(E73="PT","pt_methods",IF(E73="DISO","diso_methods",IF(E73="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -4392,11 +4392,11 @@
         <v>0</v>
       </c>
       <c r="I74" s="3" t="str">
-        <f>IF(E74="SIDO","single-input, double-output",IF(E74="SISO","single-input, single-output",IF(E74="PT","pass-through",IF(E74="DISO","double-input, single-output",IF(E74="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J74" s="3" t="str">
-        <f>IF(E74="SIDO","sido_methods",IF(E74="SISO","siso_methods",IF(E74="PT","pt_methods",IF(E74="DISO","diso_methods",IF(E74="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -4427,11 +4427,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I75" s="3" t="str">
-        <f>IF(E75="SIDO","single-input, double-output",IF(E75="SISO","single-input, single-output",IF(E75="PT","pass-through",IF(E75="DISO","double-input, single-output",IF(E75="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J75" s="3" t="str">
-        <f>IF(E75="SIDO","sido_methods",IF(E75="SISO","siso_methods",IF(E75="PT","pt_methods",IF(E75="DISO","diso_methods",IF(E75="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -4462,11 +4462,11 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I76" s="3" t="str">
-        <f>IF(E76="SIDO","single-input, double-output",IF(E76="SISO","single-input, single-output",IF(E76="PT","pass-through",IF(E76="DISO","double-input, single-output",IF(E76="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J76" s="3" t="str">
-        <f>IF(E76="SIDO","sido_methods",IF(E76="SISO","siso_methods",IF(E76="PT","pt_methods",IF(E76="DISO","diso_methods",IF(E76="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
@@ -4496,11 +4496,11 @@
         <v>68</v>
       </c>
       <c r="I77" s="3" t="str">
-        <f>IF(E77="SIDO","single-input, double-output",IF(E77="SISO","single-input, single-output",IF(E77="PT","pass-through",IF(E77="DISO","double-input, single-output",IF(E77="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J77" s="3" t="str">
-        <f>IF(E77="SIDO","sido_methods",IF(E77="SISO","siso_methods",IF(E77="PT","pt_methods",IF(E77="DISO","diso_methods",IF(E77="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -4530,11 +4530,11 @@
         <v>203</v>
       </c>
       <c r="I78" s="3" t="str">
-        <f>IF(E78="SIDO","single-input, double-output",IF(E78="SISO","single-input, single-output",IF(E78="PT","pass-through",IF(E78="DISO","double-input, single-output",IF(E78="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
       <c r="J78" s="3" t="str">
-        <f>IF(E78="SIDO","sido_methods",IF(E78="SISO","siso_methods",IF(E78="PT","pt_methods",IF(E78="DISO","diso_methods",IF(E78="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Custom ZO Docs (#585)
* add ref for zo costing package in unit files

* run automate script to update all rst files

* Add dictionaries for unit doc sections that require unique customization; first test with updating titles for those that need the update; add Additional Variables section if unit non-basic

* starting a func to grab additional variables

* Automate  inclusion of additional variables for non-basic units with description from doc strings

* fix csv-table spacing

* try to fix CANDOP doc error

* change municipal_drinking_zo to basic since it has no additional variables

* add units to variable table; add section title for additional constraints

* revise Configerror tests

* trying to add path to data/technoeconomic but commented out for now

* add additional constraints for non-basic units

* fix addition of constraints and customized energy consumption message
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AD6B36-2DD8-4668-8E1E-D2B182143B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C6B7C6-F553-4615-B270-3D97951EC2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$78</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="463">
   <si>
     <t>Name</t>
   </si>
@@ -1166,6 +1166,261 @@
   </si>
   <si>
     <t>blending reservoir</t>
+  </si>
+  <si>
+    <t>energy_helper_func</t>
+  </si>
+  <si>
+    <t>class_name</t>
+  </si>
+  <si>
+    <t>BackwashSolidsHandlingZO</t>
+  </si>
+  <si>
+    <t>BioActiveFiltrationZO</t>
+  </si>
+  <si>
+    <t>BlendingReservoirZO</t>
+  </si>
+  <si>
+    <t>CASZO</t>
+  </si>
+  <si>
+    <t>CoolingTowerZO</t>
+  </si>
+  <si>
+    <t>DeepWellInjectionZO</t>
+  </si>
+  <si>
+    <t>DMBRZO</t>
+  </si>
+  <si>
+    <t>ElectrodialysisReversalZO</t>
+  </si>
+  <si>
+    <t>AerationBasinZO</t>
+  </si>
+  <si>
+    <t>AirFlotationZO</t>
+  </si>
+  <si>
+    <t>BioreactorZO</t>
+  </si>
+  <si>
+    <t>MetabZO</t>
+  </si>
+  <si>
+    <t>BufferTankZO</t>
+  </si>
+  <si>
+    <t>ChemicalAdditionZO</t>
+  </si>
+  <si>
+    <t>CartridgeFiltrationZO</t>
+  </si>
+  <si>
+    <t>CoolingSupplyZO</t>
+  </si>
+  <si>
+    <t>DecarbonatorZO</t>
+  </si>
+  <si>
+    <t>DissolvedAirFlotationZO</t>
+  </si>
+  <si>
+    <t>FeedWaterTankZO</t>
+  </si>
+  <si>
+    <t>FeedZO</t>
+  </si>
+  <si>
+    <t>ElectroNPZO</t>
+  </si>
+  <si>
+    <t>EnergyRecoveryZO</t>
+  </si>
+  <si>
+    <t>IronManganeseRemovalZO</t>
+  </si>
+  <si>
+    <t>LandfillZO</t>
+  </si>
+  <si>
+    <t>PumpElectricityZO</t>
+  </si>
+  <si>
+    <t>MABRZO</t>
+  </si>
+  <si>
+    <t>MBRZO</t>
+  </si>
+  <si>
+    <t>MediaFiltrationZO</t>
+  </si>
+  <si>
+    <t>MicroFiltrationZO</t>
+  </si>
+  <si>
+    <t>MicroscreenFiltrationZO</t>
+  </si>
+  <si>
+    <t>MunicipalWWTPZO</t>
+  </si>
+  <si>
+    <t>NanofiltrationZO</t>
+  </si>
+  <si>
+    <t>ClarifierZO</t>
+  </si>
+  <si>
+    <t>PrimarySeparatorZO</t>
+  </si>
+  <si>
+    <t>PumpZO</t>
+  </si>
+  <si>
+    <t>ScreenZO</t>
+  </si>
+  <si>
+    <t>SedimentationZO</t>
+  </si>
+  <si>
+    <t>SettlingPondZO</t>
+  </si>
+  <si>
+    <t>SMPZO</t>
+  </si>
+  <si>
+    <t>TrampOilTankZO</t>
+  </si>
+  <si>
+    <t>TriMediaFiltrationZO</t>
+  </si>
+  <si>
+    <t>CoagulationFlocculationZO</t>
+  </si>
+  <si>
+    <t>UltraFiltrationZO</t>
+  </si>
+  <si>
+    <t>UVZO</t>
+  </si>
+  <si>
+    <t>UVAOPZO</t>
+  </si>
+  <si>
+    <t>WalnutShellFilterZO</t>
+  </si>
+  <si>
+    <t>WAIVZO</t>
+  </si>
+  <si>
+    <t>AnaerobicDigestionOxidationZO</t>
+  </si>
+  <si>
+    <t>FixedBedZO</t>
+  </si>
+  <si>
+    <t>MunicipalDrinkingZO</t>
+  </si>
+  <si>
+    <t>OzoneZO</t>
+  </si>
+  <si>
+    <t>OzoneAOPZO</t>
+  </si>
+  <si>
+    <t>IonExchangeZO</t>
+  </si>
+  <si>
+    <t>BrineConcentratorZO</t>
+  </si>
+  <si>
+    <t>GACZO</t>
+  </si>
+  <si>
+    <t>DualMediaFiltrationZO</t>
+  </si>
+  <si>
+    <t>StorageTankZO</t>
+  </si>
+  <si>
+    <t>SWOnshoreIntakeZO</t>
+  </si>
+  <si>
+    <t>ChlorinationZO</t>
+  </si>
+  <si>
+    <t>StaticMixerZO</t>
+  </si>
+  <si>
+    <t>CO2AdditionZO</t>
+  </si>
+  <si>
+    <t>SludgeTankZO</t>
+  </si>
+  <si>
+    <t>EvaporationPondZO</t>
+  </si>
+  <si>
+    <t>FilterPressZO</t>
+  </si>
+  <si>
+    <t>WaterPumpingStationZO</t>
+  </si>
+  <si>
+    <t>WellFieldZO</t>
+  </si>
+  <si>
+    <t>IntrusionMitigationZO</t>
+  </si>
+  <si>
+    <t>InjectionWellDisposalZO</t>
+  </si>
+  <si>
+    <t>SurfaceDischargeZO</t>
+  </si>
+  <si>
+    <t>PhotothermalMembraneZO</t>
+  </si>
+  <si>
+    <t>CANDOPZO</t>
+  </si>
+  <si>
+    <t>AnaerobicMBRMECZO</t>
+  </si>
+  <si>
+    <t>ATHTLZO</t>
+  </si>
+  <si>
+    <t>SecondaryTreatmentWWTPZO</t>
+  </si>
+  <si>
+    <t>CofermentationZO</t>
+  </si>
+  <si>
+    <t>ConstructedWetlandsZO</t>
+  </si>
+  <si>
+    <t>GasSpargedMembraneZO</t>
+  </si>
+  <si>
+    <t>HTGZO</t>
+  </si>
+  <si>
+    <t>SaltPrecipitationZO</t>
+  </si>
+  <si>
+    <t>VFARecoveryZO</t>
+  </si>
+  <si>
+    <t>autothermal_hydrothermal_liquefaction_zo</t>
+  </si>
+  <si>
+    <t>hydrothermal_gasification_zo</t>
+  </si>
+  <si>
+    <t>supercritical_salt_precipitation_zo</t>
   </si>
 </sst>
 </file>
@@ -1231,11 +1486,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1574,24 +1830,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="33.3984375" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" customWidth="1"/>
-    <col min="5" max="5" width="20.265625" customWidth="1"/>
-    <col min="6" max="6" width="38.59765625" customWidth="1"/>
-    <col min="7" max="7" width="30.265625" customWidth="1"/>
-    <col min="8" max="8" width="25.59765625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" customWidth="1"/>
+    <col min="7" max="7" width="20.265625" customWidth="1"/>
+    <col min="8" max="8" width="38.59765625" customWidth="1"/>
+    <col min="9" max="9" width="30.265625" customWidth="1"/>
+    <col min="10" max="10" width="25.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1599,2221 +1856,2693 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="str">
-        <f>IF(C2="basic","cost_power_law_flow")</f>
+      <c r="H2" s="3" t="str">
+        <f t="shared" ref="H2:H9" si="0">IF(D2="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G2" s="3" t="str">
-        <f>IF(D2="SIDO","single-input, double-output",IF(D2="SISO","single-input, single-output",IF(D2="PT","pass-through",IF(D2="DISO","double-input, single-output",IF(D2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="I2" s="3" t="str">
+        <f t="shared" ref="I2:I33" si="1">IF(E2="SIDO","single-input, double-output",IF(E2="SISO","single-input, single-output",IF(E2="PT","pass-through",IF(E2="DISO","double-input, single-output",IF(E2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="H2" s="3" t="str">
-        <f>IF(D2="SIDO","sido_methods",IF(D2="SISO","siso_methods",IF(D2="PT","pt_methods",IF(D2="DISO","diso_methods",IF(D2="SIDO reactive","sidor_methods","")))))</f>
+      <c r="J2" s="3" t="str">
+        <f t="shared" ref="J2:J33" si="2">IF(E2="SIDO","sido_methods",IF(E2="SISO","siso_methods",IF(E2="PT","pt_methods",IF(E2="DISO","diso_methods",IF(E2="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F65" si="0">IF(C3="basic","cost_power_law_flow")</f>
+      <c r="H3" s="3" t="str">
+        <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G3" s="3" t="str">
-        <f t="shared" ref="G3:G66" si="1">IF(D3="SIDO","single-input, double-output",IF(D3="SISO","single-input, single-output",IF(D3="PT","pass-through",IF(D3="DISO","double-input, single-output",IF(D3="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="I3" s="3" t="str">
+        <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H3" s="3" t="str">
-        <f t="shared" ref="H3:H66" si="2">IF(D3="SIDO","sido_methods",IF(D3="SISO","siso_methods",IF(D3="PT","pt_methods",IF(D3="DISO","diso_methods",IF(D3="SIDO reactive","sidor_methods","")))))</f>
+      <c r="J3" s="3" t="str">
+        <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="H4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G4" s="3" t="str">
+      <c r="I4" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H4" s="3" t="str">
+      <c r="J4" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3" t="b">
+      <c r="H5" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="3" t="str">
+      <c r="I5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H5" s="3" t="str">
+      <c r="J5" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>380</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="H6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G6" s="3" t="str">
+      <c r="I6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H6" s="3" t="str">
+      <c r="J6" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
+        <v>381</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="H7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="I7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="J7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="3" t="str">
+      <c r="H8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G8" s="3" t="str">
+      <c r="I8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H8" s="3" t="str">
+      <c r="J8" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>377</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
+        <v>382</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="H9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="I9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="J9" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
+        <v>433</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="3" t="str">
+      <c r="I10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H10" s="3" t="str">
+      <c r="J10" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
+        <v>392</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H11" s="3" t="str">
+        <f>IF(D11="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G11" s="3" t="str">
+      <c r="I11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H11" s="3" t="str">
+      <c r="J11" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
+        <v>450</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="3" t="str">
+      <c r="I12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H12" s="3" t="str">
+      <c r="J12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
+        <v>394</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H13" s="3" t="str">
+        <f>IF(D13="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G13" s="3" t="str">
+      <c r="I13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H13" s="3" t="str">
+      <c r="J13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="3" t="str">
+      <c r="I14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H14" s="3" t="str">
+      <c r="J14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
+        <v>438</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="3" t="str">
+      <c r="I15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H15" s="3" t="str">
+      <c r="J15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
+        <v>412</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H16" s="3" t="str">
+        <f>IF(D16="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G16" s="3" t="str">
+      <c r="I16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H16" s="3" t="str">
+      <c r="J16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
+        <v>440</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H17" s="3" t="str">
+        <f>IF(D17="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G17" s="3" t="str">
+      <c r="I17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H17" s="3" t="str">
+      <c r="J17" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
+        <v>421</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="3" t="str">
+      <c r="I18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H18" s="3" t="str">
+      <c r="J18" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
+        <v>454</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H19" s="3" t="b">
+        <f>IF(D19="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="G19" s="3" t="str">
+      <c r="I19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>double-input, single-output</v>
       </c>
-      <c r="H19" s="3" t="str">
+      <c r="J19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>diso_methods</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
+        <v>455</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H20" s="3" t="b">
+        <f>IF(D20="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="G20" s="3" t="str">
+      <c r="I20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H20" s="3" t="str">
+      <c r="J20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>383</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H21" s="3" t="str">
+        <f>IF(D21="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G21" s="3" t="str">
+      <c r="I21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H21" s="3" t="str">
+      <c r="J21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
+        <v>395</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H22" s="3" t="str">
+        <f>IF(D22="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G22" s="3" t="str">
+      <c r="I22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H22" s="3" t="str">
+      <c r="J22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
+        <v>384</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="3" t="str">
+      <c r="I23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H23" s="3" t="str">
+      <c r="J23" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
+        <v>396</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H24" s="3" t="str">
+        <f>IF(D24="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G24" s="3" t="str">
+      <c r="I24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H24" s="3" t="str">
+      <c r="J24" s="3" t="str">
         <f t="shared" si="2"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
+        <v>385</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="3" t="str">
+      <c r="I25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H25" s="3" t="str">
+      <c r="J25" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
+        <v>397</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H26" s="3" t="str">
+        <f>IF(D26="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G26" s="3" t="str">
+      <c r="I26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H26" s="3" t="str">
+      <c r="J26" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
+        <v>386</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="F27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="3" t="str">
+      <c r="I27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H27" s="3" t="str">
+      <c r="J27" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H28" s="3" t="str">
+        <f>IF(D28="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G28" s="3" t="str">
+      <c r="I28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H28" s="3" t="str">
+      <c r="J28" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="3" t="str">
+      <c r="I29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H29" s="3" t="str">
+      <c r="J29" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" t="s">
+        <v>387</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G30" s="3" t="str">
+      <c r="I30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H30" s="3" t="str">
+      <c r="J30" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" t="s">
+        <v>401</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H31" s="3" t="str">
+        <f>IF(D31="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G31" s="3" t="str">
+      <c r="I31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H31" s="3" t="str">
+      <c r="J31" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
+        <v>442</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="3" t="str">
+      <c r="I32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H32" s="3" t="str">
+      <c r="J32" s="3" t="str">
         <f t="shared" si="2"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
+        <v>398</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H33" s="3" t="str">
+        <f>IF(D33="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G33" s="3" t="str">
+      <c r="I33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>pass-through</v>
       </c>
-      <c r="H33" s="3" t="str">
+      <c r="J33" s="3" t="str">
         <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
+        <v>399</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F34" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="F34" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="3" t="b">
+        <f>IF(D34="basic","cost_power_law_flow")</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
+        <v>443</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="F35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G35" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I35" s="3" t="str">
+        <f>IF(E35="SIDO","single-input, double-output",IF(E35="SISO","single-input, single-output",IF(E35="PT","pass-through",IF(E35="DISO","double-input, single-output",IF(E35="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="H35" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J35" s="3" t="str">
+        <f>IF(E35="SIDO","sido_methods",IF(E35="SISO","siso_methods",IF(E35="PT","pt_methods",IF(E35="DISO","diso_methods",IF(E35="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" t="s">
+        <v>428</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="F36" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G36" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I36" s="3" t="str">
+        <f>IF(E36="SIDO","single-input, double-output",IF(E36="SISO","single-input, single-output",IF(E36="PT","pass-through",IF(E36="DISO","double-input, single-output",IF(E36="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, single-output</v>
       </c>
-      <c r="H36" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J36" s="3" t="str">
+        <f>IF(E36="SIDO","sido_methods",IF(E36="SISO","siso_methods",IF(E36="PT","pt_methods",IF(E36="DISO","diso_methods",IF(E36="SIDO reactive","sidor_methods","")))))</f>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" t="s">
+        <v>434</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I37" s="3" t="str">
+        <f>IF(E37="SIDO","single-input, double-output",IF(E37="SISO","single-input, single-output",IF(E37="PT","pass-through",IF(E37="DISO","double-input, single-output",IF(E37="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
-      <c r="H37" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J37" s="3" t="str">
+        <f>IF(E37="SIDO","sido_methods",IF(E37="SISO","siso_methods",IF(E37="PT","pt_methods",IF(E37="DISO","diso_methods",IF(E37="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
+        <v>456</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="3" t="b">
-        <f t="shared" si="0"/>
+      <c r="H38" s="3" t="b">
+        <f>IF(D38="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="I38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="J38" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
+        <v>447</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="F39" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H39" s="3" t="str">
+        <f>IF(D39="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G39" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I39" s="3" t="str">
+        <f t="shared" ref="I39:I78" si="3">IF(E39="SIDO","single-input, double-output",IF(E39="SISO","single-input, single-output",IF(E39="PT","pass-through",IF(E39="DISO","double-input, single-output",IF(E39="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
-      <c r="H39" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J39" s="3" t="str">
+        <f t="shared" ref="J39:J78" si="4">IF(E39="SIDO","sido_methods",IF(E39="SISO","siso_methods",IF(E39="PT","pt_methods",IF(E39="DISO","diso_methods",IF(E39="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
+        <v>446</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="F40" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H40" s="3" t="str">
+        <f>IF(D40="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G40" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I40" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H40" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J40" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" t="s">
+        <v>432</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="F41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G41" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I41" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H41" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J41" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
+        <v>402</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="F42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G42" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I42" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H42" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J42" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
+        <v>403</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="G43" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I43" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H43" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J43" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
+        <v>405</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="F44" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G44" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I44" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H44" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J44" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
+        <v>406</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H45" s="3" t="str">
+        <f>IF(D45="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G45" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I45" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H45" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J45" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" t="s">
+        <v>407</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F46" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H46" s="3" t="str">
+        <f>IF(D46="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G46" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I46" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H46" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J46" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
+        <v>391</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="F47" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G47" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I47" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
-      <c r="H47" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J47" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" t="s">
+        <v>408</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H48" s="3" t="str">
+        <f>IF(D48="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G48" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I48" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H48" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J48" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" t="s">
+        <v>409</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="F49" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H49" s="3" t="str">
+        <f>IF(D49="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G49" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I49" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H49" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J49" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>32</v>
+      <c r="C50" t="s">
+        <v>429</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="F50" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I50" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H50" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J50" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" t="s">
+        <v>410</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="F51" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F51" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H51" s="3" t="str">
+        <f>IF(D51="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G51" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I51" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H51" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J51" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" t="s">
+        <v>411</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G52" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I52" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H52" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J52" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" t="s">
+        <v>431</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="F53" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G53" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I53" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H53" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J53" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" t="s">
+        <v>430</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="F54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="H54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G54" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I54" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H54" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J54" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" t="s">
+        <v>449</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="F55" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="H55" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G55" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I55" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H55" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J55" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" t="s">
+        <v>413</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="F56" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H56" s="3" t="str">
+        <f>IF(D56="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G56" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I56" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H56" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J56" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" t="s">
+        <v>404</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="F57" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G57" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I57" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H57" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J57" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" t="s">
+        <v>414</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="F58" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H58" s="3" t="str">
+        <f>IF(D58="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G58" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I58" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H58" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J58" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" t="s">
+        <v>415</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="F59" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H59" s="3" t="str">
+        <f>IF(D59="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G59" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I59" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H59" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J59" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>160</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" t="s">
+        <v>453</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="F60" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G60" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I60" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H60" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J60" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" t="s">
+        <v>416</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="F61" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G61" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I61" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H61" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J61" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" t="s">
+        <v>417</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="F62" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H62" s="3" t="str">
+        <f>IF(D62="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G62" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I62" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H62" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J62" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" t="s">
+        <v>441</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="F63" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F63" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H63" s="3" t="str">
+        <f>IF(D63="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G63" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I63" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H63" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J63" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>169</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" t="s">
+        <v>418</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="F64" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H64" s="3" t="str">
+        <f>IF(D64="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G64" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I64" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H64" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J64" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" t="s">
+        <v>439</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="F65" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H65" s="3" t="str">
+        <f>IF(D65="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G65" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I65" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H65" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J65" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" t="s">
+        <v>436</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="F66" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G66" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="I66" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H66" s="3" t="str">
-        <f t="shared" si="2"/>
+      <c r="J66" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" t="s">
+        <v>448</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="F67" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="H67" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="G67" s="3" t="str">
-        <f t="shared" ref="G67:G78" si="3">IF(D67="SIDO","single-input, double-output",IF(D67="SISO","single-input, single-output",IF(D67="PT","pass-through",IF(D67="DISO","double-input, single-output",IF(D67="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+      <c r="I67" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H67" s="3" t="str">
-        <f t="shared" ref="H67:H78" si="4">IF(D67="SIDO","sido_methods",IF(D67="SISO","siso_methods",IF(D67="PT","pt_methods",IF(D67="DISO","diso_methods",IF(D67="SIDO reactive","sidor_methods","")))))</f>
+      <c r="J67" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>179</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" t="s">
+        <v>437</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="F68" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G68" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="3" t="str">
-        <f t="shared" ref="F68:F76" si="5">IF(C68="basic","cost_power_law_flow")</f>
+      <c r="H68" s="3" t="str">
+        <f>IF(D68="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G68" s="3" t="str">
+      <c r="I68" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H68" s="3" t="str">
+      <c r="J68" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" t="s">
+        <v>419</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="F69" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G69" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F69" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H69" s="3" t="str">
+        <f>IF(D69="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G69" s="3" t="str">
+      <c r="I69" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H69" s="3" t="str">
+      <c r="J69" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" t="s">
+        <v>420</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="F70" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H70" s="3" t="str">
+        <f>IF(D70="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G70" s="3" t="str">
+      <c r="I70" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H70" s="3" t="str">
+      <c r="J70" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" t="s">
+        <v>422</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="F71" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F71" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H71" s="3" t="str">
+        <f>IF(D71="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G71" s="3" t="str">
+      <c r="I71" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H71" s="3" t="str">
+      <c r="J71" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" t="s">
+        <v>424</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="F72" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G72" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="H72" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G72" s="3" t="str">
+      <c r="I72" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H72" s="3" t="str">
+      <c r="J72" s="3" t="str">
         <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" t="s">
+        <v>423</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="F73" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G73" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="H73" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G73" s="3" t="str">
+      <c r="I73" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="H73" s="3" t="str">
+      <c r="J73" s="3" t="str">
         <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" t="s">
+        <v>459</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="F74" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F74" s="3" t="b">
-        <f t="shared" si="5"/>
+      <c r="H74" s="3" t="b">
+        <f>IF(D74="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="G74" s="3" t="str">
+      <c r="I74" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H74" s="3" t="str">
+      <c r="J74" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" t="s">
+        <v>426</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="F75" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F75" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H75" s="3" t="str">
+        <f>IF(D75="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G75" s="3" t="str">
+      <c r="I75" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H75" s="3" t="str">
+      <c r="J75" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" t="s">
+        <v>425</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="F76" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F76" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="H76" s="3" t="str">
+        <f>IF(D76="basic","cost_power_law_flow")</f>
         <v>cost_power_law_flow</v>
       </c>
-      <c r="G76" s="3" t="str">
+      <c r="I76" s="3" t="str">
         <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
-      <c r="H76" s="3" t="str">
+      <c r="J76" s="3" t="str">
         <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" t="s">
+        <v>444</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="F77" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="H77" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G77" s="3" t="str">
+      <c r="I77" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H77" s="3" t="str">
+      <c r="J77" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>201</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" t="s">
+        <v>445</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F78" s="3" t="s">
+      <c r="F78" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H78" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="G78" s="3" t="str">
+      <c r="I78" s="3" t="str">
         <f t="shared" si="3"/>
         <v>pass-through</v>
       </c>
-      <c r="H78" s="3" t="str">
+      <c r="J78" s="3" t="str">
         <f t="shared" si="4"/>
         <v>pt_methods</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+    <sortCondition ref="B2:B78"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5302,12 +6031,661 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C80"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="37.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>376</v>
+      </c>
+      <c r="C9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>461</v>
+      </c>
+      <c r="C39" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" t="s">
+        <v>375</v>
+      </c>
+      <c r="C54" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B63" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B66" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B67" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B68" t="s">
+        <v>462</v>
+      </c>
+      <c r="C68" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B69" t="s">
+        <v>177</v>
+      </c>
+      <c r="C69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B70" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B71" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B72" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B73" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B75" t="s">
+        <v>191</v>
+      </c>
+      <c r="C75" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B76" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B77" t="s">
+        <v>196</v>
+      </c>
+      <c r="C77" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B78" t="s">
+        <v>198</v>
+      </c>
+      <c r="C78" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B79" t="s">
+        <v>200</v>
+      </c>
+      <c r="C79" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B80" t="s">
+        <v>202</v>
+      </c>
+      <c r="C80" t="s">
+        <v>445</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:C80">
+    <sortCondition ref="B1:B80"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update excel table to reflect latest updates in AMO units and rerun automation script
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C6B7C6-F553-4615-B270-3D97951EC2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34BA98C-B3D2-4082-9B02-B9E9363B72D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="466">
   <si>
     <t>Name</t>
   </si>
@@ -205,9 +205,6 @@
     <t>cofermentation_zo</t>
   </si>
   <si>
-    <t>DISO</t>
-  </si>
-  <si>
     <t xml:space="preserve">constructed wetlands </t>
   </si>
   <si>
@@ -1421,6 +1418,18 @@
   </si>
   <si>
     <t>supercritical_salt_precipitation_zo</t>
+  </si>
+  <si>
+    <t>cost_anaerobic_mbr_mec</t>
+  </si>
+  <si>
+    <t>cost_cofermentation</t>
+  </si>
+  <si>
+    <t>cost_constructed_wetlands</t>
+  </si>
+  <si>
+    <t>cost_vfa_recovery</t>
   </si>
 </sst>
 </file>
@@ -1832,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1856,7 +1865,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1865,7 +1874,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -1888,7 +1897,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -1923,7 +1932,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -1958,7 +1967,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -1993,7 +2002,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>19</v>
@@ -2005,11 +2014,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>462</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2028,7 +2036,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -2063,7 +2071,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -2098,7 +2106,7 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -2127,13 +2135,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -2168,7 +2176,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>32</v>
@@ -2202,7 +2210,7 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
@@ -2237,7 +2245,7 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>32</v>
@@ -2271,7 +2279,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>10</v>
@@ -2306,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>32</v>
@@ -2340,7 +2348,7 @@
         <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>32</v>
@@ -2374,7 +2382,7 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>10</v>
@@ -2409,7 +2417,7 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>10</v>
@@ -2444,7 +2452,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>32</v>
@@ -2478,45 +2486,44 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="F19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="3" t="b">
-        <f>IF(D19="basic","cost_power_law_flow")</f>
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>463</v>
       </c>
       <c r="I19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>double-input, single-output</v>
+        <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J19" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>diso_methods</v>
+        <v>sidor_methods</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" t="s">
+        <v>454</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>455</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>28</v>
@@ -2525,11 +2532,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="3" t="b">
-        <f>IF(D20="basic","cost_power_law_flow")</f>
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>464</v>
       </c>
       <c r="I20" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2542,13 +2548,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>10</v>
@@ -2577,13 +2583,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="C22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>10</v>
@@ -2612,13 +2618,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="C23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -2633,7 +2639,7 @@
         <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I23" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2646,13 +2652,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="C24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>10</v>
@@ -2681,13 +2687,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="C25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>32</v>
@@ -2702,7 +2708,7 @@
         <v>23</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I25" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2715,13 +2721,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>10</v>
@@ -2750,16 +2756,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="C27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>20</v>
@@ -2771,7 +2777,7 @@
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I27" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2784,13 +2790,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="C28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>10</v>
@@ -2819,13 +2825,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="C29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>19</v>
@@ -2840,7 +2846,7 @@
         <v>33</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I29" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2853,13 +2859,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="C30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>32</v>
@@ -2874,7 +2880,7 @@
         <v>33</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I30" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2887,13 +2893,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>10</v>
@@ -2922,13 +2928,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="C32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>32</v>
@@ -2943,7 +2949,7 @@
         <v>12</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I32" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2956,13 +2962,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="C33" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>10</v>
@@ -2991,46 +2997,46 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" t="s">
+        <v>398</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F34" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H34" s="3" t="b">
         <f>IF(D34="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>32</v>
@@ -3045,7 +3051,7 @@
         <v>33</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I35" s="3" t="str">
         <f>IF(E35="SIDO","single-input, double-output",IF(E35="SISO","single-input, single-output",IF(E35="PT","pass-through",IF(E35="DISO","double-input, single-output",IF(E35="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3058,13 +3064,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="C36" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>32</v>
@@ -3079,7 +3085,7 @@
         <v>12</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I36" s="3" t="str">
         <f>IF(E36="SIDO","single-input, double-output",IF(E36="SISO","single-input, single-output",IF(E36="PT","pass-through",IF(E36="DISO","double-input, single-output",IF(E36="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3092,13 +3098,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="C37" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>32</v>
@@ -3113,7 +3119,7 @@
         <v>33</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I37" s="3" t="str">
         <f>IF(E37="SIDO","single-input, double-output",IF(E37="SISO","single-input, single-output",IF(E37="PT","pass-through",IF(E37="DISO","double-input, single-output",IF(E37="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3126,19 +3132,19 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="C38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F38" s="4" t="b">
         <v>1</v>
@@ -3151,21 +3157,21 @@
         <v>0</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="C39" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>10</v>
@@ -3194,13 +3200,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="C40" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>10</v>
@@ -3229,13 +3235,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="C41" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>32</v>
@@ -3250,7 +3256,7 @@
         <v>23</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I41" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3263,13 +3269,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="C42" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>32</v>
@@ -3284,7 +3290,7 @@
         <v>33</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I42" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3297,13 +3303,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="C43" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>10</v>
@@ -3318,7 +3324,7 @@
         <v>12</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I43" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3331,13 +3337,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="C44" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>19</v>
@@ -3352,7 +3358,7 @@
         <v>12</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I44" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3365,13 +3371,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="C45" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>10</v>
@@ -3400,13 +3406,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="C46" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>10</v>
@@ -3435,13 +3441,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="C47" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>19</v>
@@ -3456,7 +3462,7 @@
         <v>33</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I47" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3469,13 +3475,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="C48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>10</v>
@@ -3504,13 +3510,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="C49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>10</v>
@@ -3539,13 +3545,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="C50" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>10</v>
@@ -3560,7 +3566,7 @@
         <v>23</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I50" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3573,13 +3579,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="C51" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>10</v>
@@ -3608,13 +3614,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="C52" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>32</v>
@@ -3629,7 +3635,7 @@
         <v>33</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I52" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3642,13 +3648,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C53" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>32</v>
@@ -3663,7 +3669,7 @@
         <v>33</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I53" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3676,13 +3682,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="C54" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>32</v>
@@ -3697,7 +3703,7 @@
         <v>33</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I54" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3710,13 +3716,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="C55" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>19</v>
@@ -3731,7 +3737,7 @@
         <v>33</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I55" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3744,13 +3750,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="C56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>10</v>
@@ -3779,13 +3785,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="C57" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>32</v>
@@ -3800,7 +3806,7 @@
         <v>33</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I57" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3813,13 +3819,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="C58" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>10</v>
@@ -3848,13 +3854,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="C59" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>10</v>
@@ -3883,16 +3889,16 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="C60" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>11</v>
@@ -3904,7 +3910,7 @@
         <v>12</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I60" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3917,13 +3923,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="C61" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>32</v>
@@ -3938,7 +3944,7 @@
         <v>12</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I61" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3951,13 +3957,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="C62" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>10</v>
@@ -3986,13 +3992,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="C63" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>10</v>
@@ -4021,13 +4027,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="C64" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>10</v>
@@ -4056,13 +4062,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="C65" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>10</v>
@@ -4091,13 +4097,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="C66" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>32</v>
@@ -4112,7 +4118,7 @@
         <v>12</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I66" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4125,13 +4131,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="C67" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>32</v>
@@ -4146,7 +4152,7 @@
         <v>23</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I67" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4159,13 +4165,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="C68" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>10</v>
@@ -4194,13 +4200,13 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="C69" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>10</v>
@@ -4229,13 +4235,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="C70" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>10</v>
@@ -4264,13 +4270,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="C71" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>10</v>
@@ -4299,13 +4305,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="C72" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>32</v>
@@ -4320,7 +4326,7 @@
         <v>12</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I72" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4333,13 +4339,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="C73" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>32</v>
@@ -4354,7 +4360,7 @@
         <v>12</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I73" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4367,16 +4373,16 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="C74" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>11</v>
@@ -4387,9 +4393,8 @@
       <c r="G74" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H74" s="3" t="b">
-        <f>IF(D74="basic","cost_power_law_flow")</f>
-        <v>0</v>
+      <c r="H74" s="3" t="s">
+        <v>465</v>
       </c>
       <c r="I74" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4402,13 +4407,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="C75" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>10</v>
@@ -4437,13 +4442,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>198</v>
-      </c>
       <c r="C76" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>10</v>
@@ -4472,13 +4477,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="C77" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>32</v>
@@ -4493,7 +4498,7 @@
         <v>33</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I77" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4506,13 +4511,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="C78" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>32</v>
@@ -4527,7 +4532,7 @@
         <v>23</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I78" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4539,7 +4544,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
     <sortCondition ref="B2:B78"/>
   </sortState>
@@ -4565,17 +4569,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE(A1,"_zo")</f>
         <v>aeration_basin_zo</v>
       </c>
       <c r="C1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" t="s">
         <v>205</v>
-      </c>
-      <c r="D1" t="s">
-        <v>206</v>
       </c>
       <c r="G1" t="str">
         <f>CONCATENATE(C1," ",D1)</f>
@@ -4584,17 +4588,17 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B65" si="0">CONCATENATE(A2,"_zo")</f>
         <v>air_flotation_zo</v>
       </c>
       <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" t="s">
         <v>208</v>
-      </c>
-      <c r="D2" t="s">
-        <v>209</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" si="1">CONCATENATE(C2," ",D2)</f>
@@ -4603,20 +4607,20 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_digestion_oxidation_zo</v>
+      </c>
+      <c r="C3" t="s">
         <v>210</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_digestion_oxidation_zo</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>211</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>212</v>
-      </c>
-      <c r="E3" t="s">
-        <v>213</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="1"/>
@@ -4625,20 +4629,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_mbr_mec_zo</v>
+      </c>
+      <c r="C4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" t="s">
         <v>214</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_mbr_mec_zo</v>
-      </c>
-      <c r="C4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>215</v>
-      </c>
-      <c r="E4" t="s">
-        <v>216</v>
       </c>
       <c r="G4" t="str">
         <f>CONCATENATE(C4," ",D4," ",E4)</f>
@@ -4647,20 +4651,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>backwash_solids_handling_zo</v>
+      </c>
+      <c r="C5" t="s">
         <v>217</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>backwash_solids_handling_zo</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>218</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>219</v>
-      </c>
-      <c r="E5" t="s">
-        <v>220</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ref="G5:G6" si="2">CONCATENATE(C5," ",D5," ",E5)</f>
@@ -4669,20 +4673,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>bio_active_filtration_zo</v>
+      </c>
+      <c r="C6" t="s">
         <v>221</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>bio_active_filtration_zo</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>222</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>223</v>
-      </c>
-      <c r="E6" t="s">
-        <v>224</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
@@ -4691,14 +4695,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>bioreactor_zo</v>
       </c>
       <c r="C7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -4707,17 +4711,17 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>blending_resevoir_zo</v>
+      </c>
+      <c r="C8" t="s">
         <v>226</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>blending_resevoir_zo</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>227</v>
-      </c>
-      <c r="D8" t="s">
-        <v>228</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
@@ -4726,17 +4730,17 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>brine_concentrator_zo</v>
+      </c>
+      <c r="C9" t="s">
         <v>229</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>brine_concentrator_zo</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>230</v>
-      </c>
-      <c r="D9" t="s">
-        <v>231</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -4745,17 +4749,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>buffer_tank_zo</v>
+      </c>
+      <c r="C10" t="s">
         <v>232</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>buffer_tank_zo</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>233</v>
-      </c>
-      <c r="D10" t="s">
-        <v>234</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -4764,14 +4768,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>CANDOP_zo</v>
       </c>
       <c r="C11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -4780,17 +4784,17 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>cartridge_filtration_zo</v>
+      </c>
+      <c r="C12" t="s">
         <v>236</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>cartridge_filtration_zo</v>
-      </c>
-      <c r="C12" t="s">
-        <v>237</v>
-      </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -4799,17 +4803,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>chemical_addition_zo</v>
+      </c>
+      <c r="C13" t="s">
         <v>238</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>chemical_addition_zo</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>239</v>
-      </c>
-      <c r="D13" t="s">
-        <v>240</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -4818,14 +4822,14 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>chlorination_zo</v>
       </c>
       <c r="C14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -4834,14 +4838,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>clarifier_zo</v>
       </c>
       <c r="C15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -4850,17 +4854,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>co2_addition_zo</v>
+      </c>
+      <c r="C16" t="s">
         <v>243</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>co2_addition_zo</v>
-      </c>
-      <c r="C16" t="s">
-        <v>244</v>
-      </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -4869,20 +4873,20 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>coag_and_floc_zo</v>
+      </c>
+      <c r="C17" t="s">
         <v>245</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>coag_and_floc_zo</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>246</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>247</v>
-      </c>
-      <c r="E17" t="s">
-        <v>248</v>
       </c>
       <c r="G17" t="str">
         <f>CONCATENATE(C17," ",D17," ",E17)</f>
@@ -4891,14 +4895,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>cofermentation_zo</v>
       </c>
       <c r="C18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ref="G18:G19" si="3">CONCATENATE(C18," ",D18," ",E18)</f>
@@ -4907,17 +4911,17 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>constructed_wetlands_zo</v>
+      </c>
+      <c r="C19" t="s">
         <v>250</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>constructed_wetlands_zo</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>251</v>
-      </c>
-      <c r="D19" t="s">
-        <v>252</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="3"/>
@@ -4926,20 +4930,20 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>conventional_activated_sludge_zo</v>
+      </c>
+      <c r="C20" t="s">
         <v>253</v>
       </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>conventional_activated_sludge_zo</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>254</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>255</v>
-      </c>
-      <c r="E20" t="s">
-        <v>256</v>
       </c>
       <c r="G20" t="str">
         <f>CONCATENATE(C20," ",D20," ",E20)</f>
@@ -4948,17 +4952,17 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>cooling_supply_zo</v>
+      </c>
+      <c r="C21" t="s">
         <v>257</v>
       </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>cooling_supply_zo</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>258</v>
-      </c>
-      <c r="D21" t="s">
-        <v>259</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ref="G21:G22" si="4">CONCATENATE(C21," ",D21," ",E21)</f>
@@ -4967,17 +4971,17 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>cooling_tower_zo</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" t="s">
         <v>260</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>cooling_tower_zo</v>
-      </c>
-      <c r="C22" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" t="s">
-        <v>261</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="4"/>
@@ -4986,14 +4990,14 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>decarbonator_zo</v>
       </c>
       <c r="C23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -5002,20 +5006,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>deep_well_injection_zo</v>
+      </c>
+      <c r="C24" t="s">
         <v>263</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>deep_well_injection_zo</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>264</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>265</v>
-      </c>
-      <c r="E24" t="s">
-        <v>266</v>
       </c>
       <c r="G24" t="str">
         <f>CONCATENATE(C24," ",D24," ",E24)</f>
@@ -5024,20 +5028,20 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>dissolved_air_flotation_zo</v>
+      </c>
+      <c r="C25" t="s">
         <v>267</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>dissolved_air_flotation_zo</v>
-      </c>
-      <c r="C25" t="s">
-        <v>268</v>
-      </c>
       <c r="D25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" t="s">
         <v>208</v>
-      </c>
-      <c r="E25" t="s">
-        <v>209</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ref="G25" si="5">CONCATENATE(C25," ",D25," ",E25)</f>
@@ -5046,14 +5050,14 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>dmbr_zo</v>
       </c>
       <c r="C26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G26" t="str">
         <f>CONCATENATE(C26," ",D26)</f>
@@ -5062,20 +5066,20 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>dual_media_filtration_zo</v>
+      </c>
+      <c r="C27" t="s">
         <v>270</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>dual_media_filtration_zo</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>271</v>
       </c>
-      <c r="D27" t="s">
-        <v>272</v>
-      </c>
       <c r="E27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G27" t="str">
         <f>CONCATENATE(C27," ",D27," ",E27)</f>
@@ -5084,20 +5088,20 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>electrochemical_nutrient_removal_zo</v>
+      </c>
+      <c r="C28" t="s">
         <v>273</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>electrochemical_nutrient_removal_zo</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>274</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>275</v>
-      </c>
-      <c r="E28" t="s">
-        <v>276</v>
       </c>
       <c r="G28" t="str">
         <f>CONCATENATE(C28," ",D28," ",E28)</f>
@@ -5106,17 +5110,17 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>electrodialysis_reversal_zo</v>
+      </c>
+      <c r="C29" t="s">
         <v>277</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>electrodialysis_reversal_zo</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>278</v>
-      </c>
-      <c r="D29" t="s">
-        <v>279</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -5125,7 +5129,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -5135,7 +5139,7 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -5144,17 +5148,17 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>evaporation_pond_zo</v>
+      </c>
+      <c r="C31" t="s">
         <v>282</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>evaporation_pond_zo</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>283</v>
-      </c>
-      <c r="D31" t="s">
-        <v>284</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -5163,20 +5167,20 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>feed_water_tank_zo</v>
+      </c>
+      <c r="C32" t="s">
         <v>285</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>feed_water_tank_zo</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>286</v>
       </c>
-      <c r="D32" t="s">
-        <v>287</v>
-      </c>
       <c r="E32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G32" t="str">
         <f>CONCATENATE(C32," ",D32," ",E32)</f>
@@ -5185,14 +5189,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>feed_zo</v>
       </c>
       <c r="C33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -5201,17 +5205,17 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>filter_press_zo</v>
+      </c>
+      <c r="C34" t="s">
         <v>288</v>
       </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>filter_press_zo</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>289</v>
-      </c>
-      <c r="D34" t="s">
-        <v>290</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -5220,17 +5224,17 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>fixed_bed_zo</v>
+      </c>
+      <c r="C35" t="s">
         <v>291</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>fixed_bed_zo</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>292</v>
-      </c>
-      <c r="D35" t="s">
-        <v>293</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -5239,14 +5243,14 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>gac_zo</v>
       </c>
       <c r="C36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -5255,20 +5259,20 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>gas_sparged_membrane_zo</v>
+      </c>
+      <c r="C37" t="s">
         <v>295</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>gas_sparged_membrane_zo</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>296</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>297</v>
-      </c>
-      <c r="E37" t="s">
-        <v>298</v>
       </c>
       <c r="G37" t="str">
         <f>CONCATENATE(C37," ",D37," ",E37)</f>
@@ -5277,20 +5281,20 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>injection_well_disposal_zo</v>
+      </c>
+      <c r="C38" t="s">
+        <v>265</v>
+      </c>
+      <c r="D38" t="s">
+        <v>264</v>
+      </c>
+      <c r="E38" t="s">
         <v>299</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>injection_well_disposal_zo</v>
-      </c>
-      <c r="C38" t="s">
-        <v>266</v>
-      </c>
-      <c r="D38" t="s">
-        <v>265</v>
-      </c>
-      <c r="E38" t="s">
-        <v>300</v>
       </c>
       <c r="G38" t="str">
         <f>CONCATENATE(C38," ",D38," ",E38)</f>
@@ -5299,17 +5303,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>intrusion_mitigation_zo</v>
+      </c>
+      <c r="C39" t="s">
         <v>301</v>
       </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>intrusion_mitigation_zo</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>302</v>
-      </c>
-      <c r="D39" t="s">
-        <v>303</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -5318,17 +5322,17 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>ion_exchange_zo</v>
+      </c>
+      <c r="C40" t="s">
         <v>304</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>ion_exchange_zo</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>305</v>
-      </c>
-      <c r="D40" t="s">
-        <v>306</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -5337,23 +5341,23 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>iron_and_manganese_removal_zo</v>
+      </c>
+      <c r="C41" t="s">
         <v>307</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>iron_and_manganese_removal_zo</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>246</v>
+      </c>
+      <c r="E41" t="s">
         <v>308</v>
       </c>
-      <c r="D41" t="s">
-        <v>247</v>
-      </c>
-      <c r="E41" t="s">
-        <v>309</v>
-      </c>
       <c r="F41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G41" t="str">
         <f>CONCATENATE(C41," ",D41," ",E41," ",F41)</f>
@@ -5362,14 +5366,14 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>landfill_zo</v>
       </c>
       <c r="C42" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -5378,14 +5382,14 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>mabr_zo</v>
       </c>
       <c r="C43" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -5394,14 +5398,14 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>mbr_zo</v>
       </c>
       <c r="C44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -5410,17 +5414,17 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>media_filtration_zo</v>
       </c>
       <c r="C45" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -5429,14 +5433,14 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>metab_zo</v>
       </c>
       <c r="C46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -5445,14 +5449,14 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>microfiltration_zo</v>
       </c>
       <c r="C47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -5461,17 +5465,17 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>microscreen_filtration_zo</v>
+      </c>
+      <c r="C48" t="s">
         <v>315</v>
       </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>microscreen_filtration_zo</v>
-      </c>
-      <c r="C48" t="s">
-        <v>316</v>
-      </c>
       <c r="D48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -5480,17 +5484,17 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>municipal_drinking_zo</v>
+      </c>
+      <c r="C49" t="s">
         <v>317</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>municipal_drinking_zo</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>318</v>
-      </c>
-      <c r="D49" t="s">
-        <v>319</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -5499,17 +5503,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>municipal_wwtp_zo</v>
+      </c>
+      <c r="C50" t="s">
+        <v>317</v>
+      </c>
+      <c r="D50" t="s">
         <v>320</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>municipal_wwtp_zo</v>
-      </c>
-      <c r="C50" t="s">
-        <v>318</v>
-      </c>
-      <c r="D50" t="s">
-        <v>321</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -5518,14 +5522,14 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>nanofiltration_zo</v>
       </c>
       <c r="C51" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -5534,17 +5538,17 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>ozone_aop _zo</v>
+      </c>
+      <c r="C52" t="s">
         <v>323</v>
       </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>ozone_aop _zo</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>324</v>
-      </c>
-      <c r="D52" t="s">
-        <v>325</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -5553,14 +5557,14 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>ozone_zo</v>
       </c>
       <c r="C53" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -5569,17 +5573,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>photothermal_membrane_zo</v>
+      </c>
+      <c r="C54" t="s">
         <v>326</v>
       </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>photothermal_membrane_zo</v>
-      </c>
-      <c r="C54" t="s">
-        <v>327</v>
-      </c>
       <c r="D54" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -5588,17 +5592,17 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>primary_separator_zo</v>
+      </c>
+      <c r="C55" t="s">
         <v>328</v>
       </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>primary_separator_zo</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>329</v>
-      </c>
-      <c r="D55" t="s">
-        <v>330</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -5614,10 +5618,10 @@
         <v>pump_electricity_zo</v>
       </c>
       <c r="C56" t="s">
+        <v>330</v>
+      </c>
+      <c r="D56" t="s">
         <v>331</v>
-      </c>
-      <c r="D56" t="s">
-        <v>332</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
@@ -5626,14 +5630,14 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
         <v>pump_zo</v>
       </c>
       <c r="C57" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -5642,14 +5646,14 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
         <v>screen_zo</v>
       </c>
       <c r="C58" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -5658,20 +5662,20 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>secondary_treatment_wwtp_zo</v>
+      </c>
+      <c r="C59" t="s">
         <v>334</v>
       </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>secondary_treatment_wwtp_zo</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>335</v>
       </c>
-      <c r="D59" t="s">
-        <v>336</v>
-      </c>
       <c r="E59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G59" t="str">
         <f>CONCATENATE(C59," ",D59," ",E59)</f>
@@ -5680,14 +5684,14 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
         <v>sedimentation_zo</v>
       </c>
       <c r="C60" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -5696,17 +5700,17 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>settling_pond_zo</v>
+      </c>
+      <c r="C61" t="s">
         <v>338</v>
       </c>
-      <c r="B61" t="str">
-        <f t="shared" si="0"/>
-        <v>settling_pond_zo</v>
-      </c>
-      <c r="C61" t="s">
-        <v>339</v>
-      </c>
       <c r="D61" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -5715,17 +5719,17 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
         <v>sludge_tank_zo</v>
       </c>
       <c r="C62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -5734,14 +5738,14 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
         <v>smp_zo</v>
       </c>
       <c r="C63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -5750,17 +5754,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>static_mixer_zo</v>
+      </c>
+      <c r="C64" t="s">
         <v>342</v>
       </c>
-      <c r="B64" t="str">
-        <f t="shared" si="0"/>
-        <v>static_mixer_zo</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>343</v>
-      </c>
-      <c r="D64" t="s">
-        <v>344</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -5769,17 +5773,17 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>storage_tank_zo</v>
+      </c>
+      <c r="C65" t="s">
         <v>345</v>
       </c>
-      <c r="B65" t="str">
-        <f t="shared" si="0"/>
-        <v>storage_tank_zo</v>
-      </c>
-      <c r="C65" t="s">
-        <v>346</v>
-      </c>
       <c r="D65" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -5788,17 +5792,17 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" ref="B66:B77" si="6">CONCATENATE(A66,"_zo")</f>
         <v>surface_discharge_zo</v>
       </c>
       <c r="C66" t="s">
+        <v>347</v>
+      </c>
+      <c r="D66" t="s">
         <v>348</v>
-      </c>
-      <c r="D66" t="s">
-        <v>349</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G77" si="7">CONCATENATE(C66," ",D66)</f>
@@ -5807,20 +5811,20 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="6"/>
         <v>sw_onshore_intake_zo</v>
       </c>
       <c r="C67" t="s">
+        <v>350</v>
+      </c>
+      <c r="D67" t="s">
         <v>351</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>352</v>
-      </c>
-      <c r="E67" t="s">
-        <v>353</v>
       </c>
       <c r="G67" t="str">
         <f>CONCATENATE(C67," ",D67," ",E67)</f>
@@ -5829,20 +5833,20 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="6"/>
         <v>tramp_oil_tank_zo</v>
       </c>
       <c r="C68" t="s">
+        <v>354</v>
+      </c>
+      <c r="D68" t="s">
         <v>355</v>
       </c>
-      <c r="D68" t="s">
-        <v>356</v>
-      </c>
       <c r="E68" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" ref="G68:G69" si="8">CONCATENATE(C68," ",D68," ",E68)</f>
@@ -5851,20 +5855,20 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="6"/>
         <v>tri_media_filtration_zo</v>
       </c>
       <c r="C69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D69" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="8"/>
@@ -5873,17 +5877,17 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="6"/>
         <v>ultra_filtration_zo</v>
       </c>
       <c r="C70" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="7"/>
@@ -5892,17 +5896,17 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="6"/>
         <v>uv_aop_zo</v>
       </c>
       <c r="C71" t="s">
+        <v>361</v>
+      </c>
+      <c r="D71" t="s">
         <v>362</v>
-      </c>
-      <c r="D71" t="s">
-        <v>363</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="7"/>
@@ -5911,14 +5915,14 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="6"/>
         <v>uv_zo</v>
       </c>
       <c r="C72" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="7"/>
@@ -5927,17 +5931,17 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="6"/>
         <v>vfa_recovery_zo</v>
       </c>
       <c r="C73" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D73" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="7"/>
@@ -5946,14 +5950,14 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="6"/>
         <v>waiv_zo</v>
       </c>
       <c r="C74" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="7"/>
@@ -5962,20 +5966,20 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="6"/>
         <v>walnut_shell_filter_zo</v>
       </c>
       <c r="C75" t="s">
+        <v>367</v>
+      </c>
+      <c r="D75" t="s">
         <v>368</v>
       </c>
-      <c r="D75" t="s">
-        <v>369</v>
-      </c>
       <c r="E75" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ref="G75:G76" si="9">CONCATENATE(C75," ",D75," ",E75)</f>
@@ -5984,20 +5988,20 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="6"/>
         <v>water_pumping_station_zo</v>
       </c>
       <c r="C76" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D76" t="s">
+        <v>370</v>
+      </c>
+      <c r="E76" t="s">
         <v>371</v>
-      </c>
-      <c r="E76" t="s">
-        <v>372</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="9"/>
@@ -6006,17 +6010,17 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="6"/>
         <v>well_field_zo</v>
       </c>
       <c r="C77" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D77" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="7"/>
@@ -6047,7 +6051,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
@@ -6055,7 +6059,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -6063,7 +6067,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -6071,15 +6075,15 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
@@ -6087,7 +6091,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
@@ -6095,7 +6099,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
@@ -6103,15 +6107,15 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
@@ -6119,7 +6123,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
@@ -6127,7 +6131,7 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
@@ -6135,7 +6139,7 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
@@ -6143,7 +6147,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -6151,7 +6155,7 @@
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
@@ -6159,7 +6163,7 @@
         <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
@@ -6167,7 +6171,7 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
@@ -6175,7 +6179,7 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
@@ -6183,7 +6187,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
@@ -6191,495 +6195,495 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C39" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C49" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C52" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C54" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C55" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C58" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C59" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C60" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C61" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C63" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C64" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C65" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C66" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C68" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C70" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C71" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C72" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C73" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C74" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C75" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C76" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C77" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C78" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C79" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C80" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revise addition of variable/constraints
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34BA98C-B3D2-4082-9B02-B9E9363B72D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29BAF7A-B4E3-4317-B961-9BA64D3FFDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="464">
   <si>
     <t>Name</t>
   </si>
@@ -91,9 +91,6 @@
     <t>anaerobic_mbr_mec_zo</t>
   </si>
   <si>
-    <t>AMO</t>
-  </si>
-  <si>
     <t>SIDO reactive</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
   </si>
   <si>
     <t>gas_sparged_membrane_zo</t>
-  </si>
-  <si>
-    <t>custom</t>
   </si>
   <si>
     <t>injection well disposal</t>
@@ -1841,8 +1835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1865,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1874,7 +1868,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -1897,7 +1891,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -1932,7 +1926,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -1967,7 +1961,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -2002,22 +1996,22 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2030,13 +2024,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -2048,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2065,13 +2059,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -2100,19 +2094,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="C8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>1</v>
@@ -2135,19 +2129,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>1</v>
@@ -2170,16 +2164,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
+        <v>430</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>432</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
@@ -2188,10 +2182,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2204,19 +2198,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="C11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="4" t="b">
         <v>1</v>
@@ -2239,28 +2233,28 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="C12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2273,13 +2267,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>10</v>
@@ -2308,28 +2302,28 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2342,19 +2336,19 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C15" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="b">
         <v>1</v>
@@ -2363,7 +2357,7 @@
         <v>12</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I15" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2376,13 +2370,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="C16" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>10</v>
@@ -2411,19 +2405,19 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C17" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" s="4" t="b">
         <v>1</v>
@@ -2446,28 +2440,28 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="C18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I18" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2480,28 +2474,28 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C19" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I19" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2514,28 +2508,28 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="C20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I20" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2548,13 +2542,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C21" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>10</v>
@@ -2583,19 +2577,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="C22" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="4" t="b">
         <v>1</v>
@@ -2618,16 +2612,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="C23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>11</v>
@@ -2639,7 +2633,7 @@
         <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I23" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2652,19 +2646,19 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="C24" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24" s="4" t="b">
         <v>1</v>
@@ -2687,28 +2681,28 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I25" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2721,13 +2715,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="C26" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>10</v>
@@ -2756,19 +2750,19 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="C27" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="4" t="b">
         <v>1</v>
@@ -2777,7 +2771,7 @@
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I27" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2790,13 +2784,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="C28" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>10</v>
@@ -2825,28 +2819,28 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="C29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F29" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I29" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2859,16 +2853,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>11</v>
@@ -2877,10 +2871,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I30" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2893,19 +2887,19 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="C31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F31" s="4" t="b">
         <v>1</v>
@@ -2928,16 +2922,16 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="C32" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>11</v>
@@ -2949,7 +2943,7 @@
         <v>12</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I32" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2962,19 +2956,19 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="C33" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F33" s="4" t="b">
         <v>1</v>
@@ -2997,49 +2991,49 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" t="s">
+        <v>396</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C34" t="s">
-        <v>398</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F34" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H34" s="3" t="b">
         <f>IF(D34="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="C35" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>11</v>
@@ -3048,10 +3042,10 @@
         <v>0</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I35" s="3" t="str">
         <f>IF(E35="SIDO","single-input, double-output",IF(E35="SISO","single-input, single-output",IF(E35="PT","pass-through",IF(E35="DISO","double-input, single-output",IF(E35="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3064,19 +3058,19 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="C36" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="4" t="b">
         <v>1</v>
@@ -3085,7 +3079,7 @@
         <v>12</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I36" s="3" t="str">
         <f>IF(E36="SIDO","single-input, double-output",IF(E36="SISO","single-input, single-output",IF(E36="PT","pass-through",IF(E36="DISO","double-input, single-output",IF(E36="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3098,16 +3092,16 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C37" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>11</v>
@@ -3116,10 +3110,10 @@
         <v>0</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I37" s="3" t="str">
         <f>IF(E37="SIDO","single-input, double-output",IF(E37="SISO","single-input, single-output",IF(E37="PT","pass-through",IF(E37="DISO","double-input, single-output",IF(E37="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
@@ -3132,52 +3126,54 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="C38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="F38" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H38" s="3" t="b">
         <f>IF(D38="basic","cost_power_law_flow")</f>
         <v>0</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>95</v>
+      <c r="I38" s="3" t="str">
+        <f>IF(E38="SIDO","single-input, double-output",IF(E38="SISO","single-input, single-output",IF(E38="PT","pass-through",IF(E38="DISO","double-input, single-output",IF(E38="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <v>single-input, double-output</v>
+      </c>
+      <c r="J38" s="3" t="str">
+        <f>IF(E38="SIDO","sido_methods",IF(E38="SISO","siso_methods",IF(E38="PT","pt_methods",IF(E38="DISO","diso_methods",IF(E38="SIDO reactive","sidor_methods","")))))</f>
+        <v>sido_methods</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F39" s="4" t="b">
         <v>1</v>
@@ -3200,19 +3196,19 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F40" s="4" t="b">
         <v>1</v>
@@ -3235,16 +3231,16 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>11</v>
@@ -3253,10 +3249,10 @@
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I41" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3269,16 +3265,16 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>11</v>
@@ -3287,10 +3283,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I42" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3303,19 +3299,19 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F43" s="4" t="b">
         <v>1</v>
@@ -3324,7 +3320,7 @@
         <v>12</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I43" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3337,19 +3333,19 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F44" s="4" t="b">
         <v>1</v>
@@ -3358,7 +3354,7 @@
         <v>12</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I44" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3371,13 +3367,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>10</v>
@@ -3406,13 +3402,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>10</v>
@@ -3441,28 +3437,28 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F47" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I47" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3475,13 +3471,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C48" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>10</v>
@@ -3510,13 +3506,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C49" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>10</v>
@@ -3545,28 +3541,28 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F50" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I50" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3579,19 +3575,19 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F51" s="4" t="b">
         <v>1</v>
@@ -3614,16 +3610,16 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C52" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>11</v>
@@ -3632,10 +3628,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I52" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3648,28 +3644,28 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C53" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F53" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I53" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3682,28 +3678,28 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F54" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I54" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3716,16 +3712,16 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C55" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>11</v>
@@ -3734,10 +3730,10 @@
         <v>0</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I55" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3750,13 +3746,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>10</v>
@@ -3785,28 +3781,28 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F57" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I57" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3819,19 +3815,19 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C58" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F58" s="4" t="b">
         <v>1</v>
@@ -3854,13 +3850,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C59" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>10</v>
@@ -3889,16 +3885,16 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C60" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>11</v>
@@ -3910,7 +3906,7 @@
         <v>12</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I60" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3923,16 +3919,16 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C61" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>11</v>
@@ -3944,7 +3940,7 @@
         <v>12</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I61" s="3" t="str">
         <f t="shared" si="3"/>
@@ -3957,13 +3953,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C62" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>10</v>
@@ -3992,13 +3988,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C63" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>10</v>
@@ -4027,19 +4023,19 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C64" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F64" s="4" t="b">
         <v>1</v>
@@ -4062,19 +4058,19 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C65" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F65" s="4" t="b">
         <v>1</v>
@@ -4097,19 +4093,19 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C66" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F66" s="4" t="b">
         <v>1</v>
@@ -4118,7 +4114,7 @@
         <v>12</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I66" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4131,28 +4127,28 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C67" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F67" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I67" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4165,25 +4161,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F68" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H68" s="3" t="str">
         <f>IF(D68="basic","cost_power_law_flow")</f>
@@ -4200,19 +4196,19 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C69" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F69" s="4" t="b">
         <v>1</v>
@@ -4235,13 +4231,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C70" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>10</v>
@@ -4270,13 +4266,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C71" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>10</v>
@@ -4305,19 +4301,19 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C72" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F72" s="4" t="b">
         <v>1</v>
@@ -4326,7 +4322,7 @@
         <v>12</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I72" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4339,19 +4335,19 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C73" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F73" s="4" t="b">
         <v>1</v>
@@ -4360,7 +4356,7 @@
         <v>12</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I73" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4373,16 +4369,16 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C74" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>11</v>
@@ -4394,7 +4390,7 @@
         <v>12</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I74" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4407,13 +4403,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C75" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>10</v>
@@ -4442,13 +4438,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C76" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>10</v>
@@ -4477,28 +4473,28 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C77" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F77" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I77" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4511,28 +4507,28 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C78" t="s">
+        <v>442</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F78" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H78" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C78" t="s">
-        <v>444</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F78" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="I78" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4569,17 +4565,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE(A1,"_zo")</f>
         <v>aeration_basin_zo</v>
       </c>
       <c r="C1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G1" t="str">
         <f>CONCATENATE(C1," ",D1)</f>
@@ -4588,17 +4584,17 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B65" si="0">CONCATENATE(A2,"_zo")</f>
         <v>air_flotation_zo</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" si="1">CONCATENATE(C2," ",D2)</f>
@@ -4607,20 +4603,20 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_digestion_oxidation_zo</v>
+      </c>
+      <c r="C3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" t="s">
         <v>209</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_digestion_oxidation_zo</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>210</v>
-      </c>
-      <c r="D3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" t="s">
-        <v>212</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="1"/>
@@ -4629,20 +4625,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>anaerobic_mbr_mec_zo</v>
+      </c>
+      <c r="C4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" t="s">
         <v>213</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>anaerobic_mbr_mec_zo</v>
-      </c>
-      <c r="C4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E4" t="s">
-        <v>215</v>
       </c>
       <c r="G4" t="str">
         <f>CONCATENATE(C4," ",D4," ",E4)</f>
@@ -4651,20 +4647,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>backwash_solids_handling_zo</v>
+      </c>
+      <c r="C5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5" t="s">
         <v>216</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>backwash_solids_handling_zo</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>217</v>
-      </c>
-      <c r="D5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E5" t="s">
-        <v>219</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ref="G5:G6" si="2">CONCATENATE(C5," ",D5," ",E5)</f>
@@ -4673,20 +4669,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>bio_active_filtration_zo</v>
+      </c>
+      <c r="C6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" t="s">
         <v>220</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>bio_active_filtration_zo</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>221</v>
-      </c>
-      <c r="D6" t="s">
-        <v>222</v>
-      </c>
-      <c r="E6" t="s">
-        <v>223</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
@@ -4695,14 +4691,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>bioreactor_zo</v>
       </c>
       <c r="C7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -4711,17 +4707,17 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>blending_resevoir_zo</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
         <v>225</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>blending_resevoir_zo</v>
-      </c>
-      <c r="C8" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" t="s">
-        <v>227</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
@@ -4730,17 +4726,17 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>brine_concentrator_zo</v>
+      </c>
+      <c r="C9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" t="s">
         <v>228</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>brine_concentrator_zo</v>
-      </c>
-      <c r="C9" t="s">
-        <v>229</v>
-      </c>
-      <c r="D9" t="s">
-        <v>230</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -4749,17 +4745,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>buffer_tank_zo</v>
+      </c>
+      <c r="C10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" t="s">
         <v>231</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>buffer_tank_zo</v>
-      </c>
-      <c r="C10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D10" t="s">
-        <v>233</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -4768,14 +4764,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>CANDOP_zo</v>
       </c>
       <c r="C11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -4784,17 +4780,17 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>cartridge_filtration_zo</v>
       </c>
       <c r="C12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -4803,17 +4799,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>chemical_addition_zo</v>
+      </c>
+      <c r="C13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" t="s">
         <v>237</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>chemical_addition_zo</v>
-      </c>
-      <c r="C13" t="s">
-        <v>238</v>
-      </c>
-      <c r="D13" t="s">
-        <v>239</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -4822,14 +4818,14 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>chlorination_zo</v>
       </c>
       <c r="C14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -4838,14 +4834,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>clarifier_zo</v>
       </c>
       <c r="C15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -4854,17 +4850,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>co2_addition_zo</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -4873,20 +4869,20 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>coag_and_floc_zo</v>
+      </c>
+      <c r="C17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D17" t="s">
         <v>244</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>coag_and_floc_zo</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>245</v>
-      </c>
-      <c r="D17" t="s">
-        <v>246</v>
-      </c>
-      <c r="E17" t="s">
-        <v>247</v>
       </c>
       <c r="G17" t="str">
         <f>CONCATENATE(C17," ",D17," ",E17)</f>
@@ -4895,14 +4891,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>cofermentation_zo</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ref="G18:G19" si="3">CONCATENATE(C18," ",D18," ",E18)</f>
@@ -4911,17 +4907,17 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>constructed_wetlands_zo</v>
+      </c>
+      <c r="C19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" t="s">
         <v>249</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>constructed_wetlands_zo</v>
-      </c>
-      <c r="C19" t="s">
-        <v>250</v>
-      </c>
-      <c r="D19" t="s">
-        <v>251</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="3"/>
@@ -4930,20 +4926,20 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>conventional_activated_sludge_zo</v>
+      </c>
+      <c r="C20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20" t="s">
         <v>252</v>
       </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>conventional_activated_sludge_zo</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>253</v>
-      </c>
-      <c r="D20" t="s">
-        <v>254</v>
-      </c>
-      <c r="E20" t="s">
-        <v>255</v>
       </c>
       <c r="G20" t="str">
         <f>CONCATENATE(C20," ",D20," ",E20)</f>
@@ -4952,17 +4948,17 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>cooling_supply_zo</v>
+      </c>
+      <c r="C21" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" t="s">
         <v>256</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>cooling_supply_zo</v>
-      </c>
-      <c r="C21" t="s">
-        <v>257</v>
-      </c>
-      <c r="D21" t="s">
-        <v>258</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ref="G21:G22" si="4">CONCATENATE(C21," ",D21," ",E21)</f>
@@ -4971,17 +4967,17 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>cooling_tower_zo</v>
       </c>
       <c r="C22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="4"/>
@@ -4990,14 +4986,14 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>decarbonator_zo</v>
       </c>
       <c r="C23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -5006,20 +5002,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>deep_well_injection_zo</v>
+      </c>
+      <c r="C24" t="s">
+        <v>261</v>
+      </c>
+      <c r="D24" t="s">
         <v>262</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>deep_well_injection_zo</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>263</v>
-      </c>
-      <c r="D24" t="s">
-        <v>264</v>
-      </c>
-      <c r="E24" t="s">
-        <v>265</v>
       </c>
       <c r="G24" t="str">
         <f>CONCATENATE(C24," ",D24," ",E24)</f>
@@ -5028,20 +5024,20 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>dissolved_air_flotation_zo</v>
       </c>
       <c r="C25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E25" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ref="G25" si="5">CONCATENATE(C25," ",D25," ",E25)</f>
@@ -5050,14 +5046,14 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>dmbr_zo</v>
       </c>
       <c r="C26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G26" t="str">
         <f>CONCATENATE(C26," ",D26)</f>
@@ -5066,20 +5062,20 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>dual_media_filtration_zo</v>
+      </c>
+      <c r="C27" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" t="s">
         <v>269</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>dual_media_filtration_zo</v>
-      </c>
-      <c r="C27" t="s">
-        <v>270</v>
-      </c>
-      <c r="D27" t="s">
-        <v>271</v>
-      </c>
       <c r="E27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G27" t="str">
         <f>CONCATENATE(C27," ",D27," ",E27)</f>
@@ -5088,20 +5084,20 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>electrochemical_nutrient_removal_zo</v>
+      </c>
+      <c r="C28" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" t="s">
         <v>272</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>electrochemical_nutrient_removal_zo</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>273</v>
-      </c>
-      <c r="D28" t="s">
-        <v>274</v>
-      </c>
-      <c r="E28" t="s">
-        <v>275</v>
       </c>
       <c r="G28" t="str">
         <f>CONCATENATE(C28," ",D28," ",E28)</f>
@@ -5110,17 +5106,17 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>electrodialysis_reversal_zo</v>
+      </c>
+      <c r="C29" t="s">
+        <v>275</v>
+      </c>
+      <c r="D29" t="s">
         <v>276</v>
-      </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>electrodialysis_reversal_zo</v>
-      </c>
-      <c r="C29" t="s">
-        <v>277</v>
-      </c>
-      <c r="D29" t="s">
-        <v>278</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -5129,7 +5125,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -5139,7 +5135,7 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -5148,17 +5144,17 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>evaporation_pond_zo</v>
+      </c>
+      <c r="C31" t="s">
+        <v>280</v>
+      </c>
+      <c r="D31" t="s">
         <v>281</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>evaporation_pond_zo</v>
-      </c>
-      <c r="C31" t="s">
-        <v>282</v>
-      </c>
-      <c r="D31" t="s">
-        <v>283</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -5167,20 +5163,20 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>feed_water_tank_zo</v>
+      </c>
+      <c r="C32" t="s">
+        <v>283</v>
+      </c>
+      <c r="D32" t="s">
         <v>284</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>feed_water_tank_zo</v>
-      </c>
-      <c r="C32" t="s">
-        <v>285</v>
-      </c>
-      <c r="D32" t="s">
-        <v>286</v>
-      </c>
       <c r="E32" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G32" t="str">
         <f>CONCATENATE(C32," ",D32," ",E32)</f>
@@ -5189,14 +5185,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>feed_zo</v>
       </c>
       <c r="C33" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -5205,17 +5201,17 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>filter_press_zo</v>
+      </c>
+      <c r="C34" t="s">
+        <v>286</v>
+      </c>
+      <c r="D34" t="s">
         <v>287</v>
-      </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>filter_press_zo</v>
-      </c>
-      <c r="C34" t="s">
-        <v>288</v>
-      </c>
-      <c r="D34" t="s">
-        <v>289</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -5224,17 +5220,17 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>fixed_bed_zo</v>
+      </c>
+      <c r="C35" t="s">
+        <v>289</v>
+      </c>
+      <c r="D35" t="s">
         <v>290</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>fixed_bed_zo</v>
-      </c>
-      <c r="C35" t="s">
-        <v>291</v>
-      </c>
-      <c r="D35" t="s">
-        <v>292</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -5243,14 +5239,14 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>gac_zo</v>
       </c>
       <c r="C36" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -5259,20 +5255,20 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>gas_sparged_membrane_zo</v>
+      </c>
+      <c r="C37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D37" t="s">
         <v>294</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>gas_sparged_membrane_zo</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>295</v>
-      </c>
-      <c r="D37" t="s">
-        <v>296</v>
-      </c>
-      <c r="E37" t="s">
-        <v>297</v>
       </c>
       <c r="G37" t="str">
         <f>CONCATENATE(C37," ",D37," ",E37)</f>
@@ -5281,20 +5277,20 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>injection_well_disposal_zo</v>
       </c>
       <c r="C38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D38" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E38" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G38" t="str">
         <f>CONCATENATE(C38," ",D38," ",E38)</f>
@@ -5303,17 +5299,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>intrusion_mitigation_zo</v>
+      </c>
+      <c r="C39" t="s">
+        <v>299</v>
+      </c>
+      <c r="D39" t="s">
         <v>300</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>intrusion_mitigation_zo</v>
-      </c>
-      <c r="C39" t="s">
-        <v>301</v>
-      </c>
-      <c r="D39" t="s">
-        <v>302</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -5322,17 +5318,17 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>ion_exchange_zo</v>
+      </c>
+      <c r="C40" t="s">
+        <v>302</v>
+      </c>
+      <c r="D40" t="s">
         <v>303</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>ion_exchange_zo</v>
-      </c>
-      <c r="C40" t="s">
-        <v>304</v>
-      </c>
-      <c r="D40" t="s">
-        <v>305</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -5341,23 +5337,23 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>iron_and_manganese_removal_zo</v>
+      </c>
+      <c r="C41" t="s">
+        <v>305</v>
+      </c>
+      <c r="D41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E41" t="s">
         <v>306</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>iron_and_manganese_removal_zo</v>
-      </c>
-      <c r="C41" t="s">
-        <v>307</v>
-      </c>
-      <c r="D41" t="s">
-        <v>246</v>
-      </c>
-      <c r="E41" t="s">
-        <v>308</v>
-      </c>
       <c r="F41" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G41" t="str">
         <f>CONCATENATE(C41," ",D41," ",E41," ",F41)</f>
@@ -5366,14 +5362,14 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>landfill_zo</v>
       </c>
       <c r="C42" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -5382,14 +5378,14 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>mabr_zo</v>
       </c>
       <c r="C43" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -5398,14 +5394,14 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>mbr_zo</v>
       </c>
       <c r="C44" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -5414,17 +5410,17 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>media_filtration_zo</v>
       </c>
       <c r="C45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -5433,14 +5429,14 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>metab_zo</v>
       </c>
       <c r="C46" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -5449,14 +5445,14 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>microfiltration_zo</v>
       </c>
       <c r="C47" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -5465,17 +5461,17 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
         <v>microscreen_filtration_zo</v>
       </c>
       <c r="C48" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D48" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -5484,17 +5480,17 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>municipal_drinking_zo</v>
+      </c>
+      <c r="C49" t="s">
+        <v>315</v>
+      </c>
+      <c r="D49" t="s">
         <v>316</v>
-      </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>municipal_drinking_zo</v>
-      </c>
-      <c r="C49" t="s">
-        <v>317</v>
-      </c>
-      <c r="D49" t="s">
-        <v>318</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -5503,17 +5499,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
         <v>municipal_wwtp_zo</v>
       </c>
       <c r="C50" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -5522,14 +5518,14 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>nanofiltration_zo</v>
       </c>
       <c r="C51" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -5538,17 +5534,17 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>ozone_aop _zo</v>
+      </c>
+      <c r="C52" t="s">
+        <v>321</v>
+      </c>
+      <c r="D52" t="s">
         <v>322</v>
-      </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>ozone_aop _zo</v>
-      </c>
-      <c r="C52" t="s">
-        <v>323</v>
-      </c>
-      <c r="D52" t="s">
-        <v>324</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -5557,14 +5553,14 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>ozone_zo</v>
       </c>
       <c r="C53" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -5573,17 +5569,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
         <v>photothermal_membrane_zo</v>
       </c>
       <c r="C54" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D54" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -5592,17 +5588,17 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>primary_separator_zo</v>
+      </c>
+      <c r="C55" t="s">
+        <v>326</v>
+      </c>
+      <c r="D55" t="s">
         <v>327</v>
-      </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>primary_separator_zo</v>
-      </c>
-      <c r="C55" t="s">
-        <v>328</v>
-      </c>
-      <c r="D55" t="s">
-        <v>329</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -5611,17 +5607,17 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="0"/>
         <v>pump_electricity_zo</v>
       </c>
       <c r="C56" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D56" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
@@ -5630,14 +5626,14 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
         <v>pump_zo</v>
       </c>
       <c r="C57" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -5646,14 +5642,14 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
         <v>screen_zo</v>
       </c>
       <c r="C58" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -5662,20 +5658,20 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>secondary_treatment_wwtp_zo</v>
+      </c>
+      <c r="C59" t="s">
+        <v>332</v>
+      </c>
+      <c r="D59" t="s">
         <v>333</v>
       </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>secondary_treatment_wwtp_zo</v>
-      </c>
-      <c r="C59" t="s">
-        <v>334</v>
-      </c>
-      <c r="D59" t="s">
-        <v>335</v>
-      </c>
       <c r="E59" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G59" t="str">
         <f>CONCATENATE(C59," ",D59," ",E59)</f>
@@ -5684,14 +5680,14 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
         <v>sedimentation_zo</v>
       </c>
       <c r="C60" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -5700,17 +5696,17 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="0"/>
         <v>settling_pond_zo</v>
       </c>
       <c r="C61" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D61" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -5719,17 +5715,17 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
         <v>sludge_tank_zo</v>
       </c>
       <c r="C62" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D62" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -5738,14 +5734,14 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
         <v>smp_zo</v>
       </c>
       <c r="C63" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -5754,17 +5750,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>static_mixer_zo</v>
+      </c>
+      <c r="C64" t="s">
+        <v>340</v>
+      </c>
+      <c r="D64" t="s">
         <v>341</v>
-      </c>
-      <c r="B64" t="str">
-        <f t="shared" si="0"/>
-        <v>static_mixer_zo</v>
-      </c>
-      <c r="C64" t="s">
-        <v>342</v>
-      </c>
-      <c r="D64" t="s">
-        <v>343</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -5773,17 +5769,17 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="0"/>
         <v>storage_tank_zo</v>
       </c>
       <c r="C65" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D65" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -5792,17 +5788,17 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" ref="B66:B77" si="6">CONCATENATE(A66,"_zo")</f>
         <v>surface_discharge_zo</v>
       </c>
       <c r="C66" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D66" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G77" si="7">CONCATENATE(C66," ",D66)</f>
@@ -5811,20 +5807,20 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="6"/>
         <v>sw_onshore_intake_zo</v>
       </c>
       <c r="C67" t="s">
+        <v>348</v>
+      </c>
+      <c r="D67" t="s">
+        <v>349</v>
+      </c>
+      <c r="E67" t="s">
         <v>350</v>
-      </c>
-      <c r="D67" t="s">
-        <v>351</v>
-      </c>
-      <c r="E67" t="s">
-        <v>352</v>
       </c>
       <c r="G67" t="str">
         <f>CONCATENATE(C67," ",D67," ",E67)</f>
@@ -5833,20 +5829,20 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="6"/>
         <v>tramp_oil_tank_zo</v>
       </c>
       <c r="C68" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D68" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E68" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" ref="G68:G69" si="8">CONCATENATE(C68," ",D68," ",E68)</f>
@@ -5855,20 +5851,20 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="6"/>
         <v>tri_media_filtration_zo</v>
       </c>
       <c r="C69" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D69" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E69" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="8"/>
@@ -5877,17 +5873,17 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="6"/>
         <v>ultra_filtration_zo</v>
       </c>
       <c r="C70" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D70" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="7"/>
@@ -5896,17 +5892,17 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="6"/>
         <v>uv_aop_zo</v>
       </c>
       <c r="C71" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D71" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="7"/>
@@ -5915,14 +5911,14 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="6"/>
         <v>uv_zo</v>
       </c>
       <c r="C72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="7"/>
@@ -5931,17 +5927,17 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="6"/>
         <v>vfa_recovery_zo</v>
       </c>
       <c r="C73" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D73" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="7"/>
@@ -5950,14 +5946,14 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="6"/>
         <v>waiv_zo</v>
       </c>
       <c r="C74" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="7"/>
@@ -5966,20 +5962,20 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="6"/>
         <v>walnut_shell_filter_zo</v>
       </c>
       <c r="C75" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D75" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E75" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ref="G75:G76" si="9">CONCATENATE(C75," ",D75," ",E75)</f>
@@ -5988,20 +5984,20 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="6"/>
         <v>water_pumping_station_zo</v>
       </c>
       <c r="C76" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D76" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E76" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="9"/>
@@ -6010,17 +6006,17 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="6"/>
         <v>well_field_zo</v>
       </c>
       <c r="C77" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D77" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="7"/>
@@ -6051,7 +6047,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
@@ -6059,7 +6055,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -6067,7 +6063,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -6075,615 +6071,615 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C39" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C44" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C49" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C52" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C53" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C54" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C57" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C59" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C60" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C61" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C62" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C63" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C64" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C65" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C66" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C67" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C68" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C69" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C70" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C72" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C73" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C74" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C75" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C76" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C77" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C78" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C79" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C80" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to address comments
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EA464E-9D46-4515-A3BC-843168647946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592FA0B6-2293-4B38-A619-6793CEE2CE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="507">
   <si>
     <t>Name</t>
   </si>
@@ -340,9 +340,6 @@
     <t>gac_zo</t>
   </si>
   <si>
-    <t>cost_gac</t>
-  </si>
-  <si>
     <t>gas sparged membrane</t>
   </si>
   <si>
@@ -1426,9 +1423,6 @@
     <t>AnaerobicDigestionReactiveZO</t>
   </si>
   <si>
-    <t>anaerobic digestion oxidation</t>
-  </si>
-  <si>
     <t>anaerobic digestion reactive</t>
   </si>
   <si>
@@ -1556,6 +1550,9 @@
   </si>
   <si>
     <t>cost_supercritical_salt_precipitation</t>
+  </si>
+  <si>
+    <t>anaerobic digestion</t>
   </si>
 </sst>
 </file>
@@ -1965,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1990,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1999,7 +1996,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -2022,7 +2019,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -2057,7 +2054,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -2086,13 +2083,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>464</v>
+        <v>506</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -2121,13 +2118,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D5" t="s">
         <v>30</v>
@@ -2161,7 +2158,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
@@ -2176,7 +2173,7 @@
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
@@ -2189,13 +2186,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
@@ -2210,7 +2207,7 @@
         <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
@@ -2229,7 +2226,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -2264,7 +2261,7 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2299,7 +2296,7 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -2328,13 +2325,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -2369,7 +2366,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
@@ -2403,7 +2400,7 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -2438,7 +2435,7 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D14" t="s">
         <v>30</v>
@@ -2472,7 +2469,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -2501,13 +2498,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>467</v>
+      </c>
+      <c r="B16" t="s">
+        <v>468</v>
+      </c>
+      <c r="C16" t="s">
         <v>469</v>
-      </c>
-      <c r="B16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C16" t="s">
-        <v>471</v>
       </c>
       <c r="D16" t="s">
         <v>30</v>
@@ -2522,7 +2519,7 @@
         <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
@@ -2541,7 +2538,7 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
@@ -2575,7 +2572,7 @@
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D18" t="s">
         <v>30</v>
@@ -2609,7 +2606,7 @@
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -2638,13 +2635,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>471</v>
+      </c>
+      <c r="B20" t="s">
+        <v>472</v>
+      </c>
+      <c r="C20" t="s">
         <v>473</v>
-      </c>
-      <c r="B20" t="s">
-        <v>474</v>
-      </c>
-      <c r="C20" t="s">
-        <v>475</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -2678,7 +2675,7 @@
         <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -2713,7 +2710,7 @@
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D22" t="s">
         <v>30</v>
@@ -2747,7 +2744,7 @@
         <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D23" t="s">
         <v>30</v>
@@ -2762,7 +2759,7 @@
         <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
@@ -2781,7 +2778,7 @@
         <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
@@ -2796,7 +2793,7 @@
         <v>58</v>
       </c>
       <c r="H24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="1"/>
@@ -2815,7 +2812,7 @@
         <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -2850,7 +2847,7 @@
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -2885,7 +2882,7 @@
         <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D27" t="s">
         <v>30</v>
@@ -2919,7 +2916,7 @@
         <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -2954,7 +2951,7 @@
         <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D29" t="s">
         <v>30</v>
@@ -2988,7 +2985,7 @@
         <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -3023,7 +3020,7 @@
         <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D31" t="s">
         <v>57</v>
@@ -3057,7 +3054,7 @@
         <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -3092,7 +3089,7 @@
         <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D33" t="s">
         <v>30</v>
@@ -3126,7 +3123,7 @@
         <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D34" t="s">
         <v>30</v>
@@ -3160,7 +3157,7 @@
         <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -3195,7 +3192,7 @@
         <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D36" t="s">
         <v>30</v>
@@ -3229,7 +3226,7 @@
         <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
@@ -3264,7 +3261,7 @@
         <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D38" t="s">
         <v>92</v>
@@ -3297,7 +3294,7 @@
         <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D39" t="s">
         <v>30</v>
@@ -3315,11 +3312,11 @@
         <v>96</v>
       </c>
       <c r="I39" t="str">
-        <f>IF(E39="SIDO","single-input, double-output",IF(E39="SISO","single-input, single-output",IF(E39="PT","pass-through",IF(E39="DISO","double-input, single-output",IF(E39="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" ref="I39:I44" si="3">IF(E39="SIDO","single-input, double-output",IF(E39="SISO","single-input, single-output",IF(E39="PT","pass-through",IF(E39="DISO","double-input, single-output",IF(E39="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
       <c r="J39" t="str">
-        <f>IF(E39="SIDO","sido_methods",IF(E39="SISO","siso_methods",IF(E39="PT","pt_methods",IF(E39="DISO","diso_methods",IF(E39="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" ref="J39:J44" si="4">IF(E39="SIDO","sido_methods",IF(E39="SISO","siso_methods",IF(E39="PT","pt_methods",IF(E39="DISO","diso_methods",IF(E39="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
@@ -3331,7 +3328,7 @@
         <v>98</v>
       </c>
       <c r="C40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D40" t="s">
         <v>30</v>
@@ -3349,11 +3346,11 @@
         <v>99</v>
       </c>
       <c r="I40" t="str">
-        <f>IF(E40="SIDO","single-input, double-output",IF(E40="SISO","single-input, single-output",IF(E40="PT","pass-through",IF(E40="DISO","double-input, single-output",IF(E40="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J40" t="str">
-        <f>IF(E40="SIDO","sido_methods",IF(E40="SISO","siso_methods",IF(E40="PT","pt_methods",IF(E40="DISO","diso_methods",IF(E40="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
@@ -3365,7 +3362,7 @@
         <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D41" t="s">
         <v>30</v>
@@ -3379,27 +3376,28 @@
       <c r="G41" t="s">
         <v>31</v>
       </c>
-      <c r="H41" t="s">
-        <v>102</v>
+      <c r="H41" t="b">
+        <f>IF(D38="basic","cost_power_law_flow")</f>
+        <v>0</v>
       </c>
       <c r="I41" t="str">
-        <f>IF(E41="SIDO","single-input, double-output",IF(E41="SISO","single-input, single-output",IF(E41="PT","pass-through",IF(E41="DISO","double-input, single-output",IF(E41="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J41" t="str">
-        <f>IF(E41="SIDO","sido_methods",IF(E41="SISO","siso_methods",IF(E41="PT","pt_methods",IF(E41="DISO","diso_methods",IF(E41="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" t="s">
         <v>103</v>
       </c>
-      <c r="B42" t="s">
-        <v>104</v>
-      </c>
       <c r="C42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
@@ -3417,23 +3415,23 @@
         <v>65</v>
       </c>
       <c r="I42" t="str">
-        <f>IF(E42="SIDO","single-input, double-output",IF(E42="SISO","single-input, single-output",IF(E42="PT","pass-through",IF(E42="DISO","double-input, single-output",IF(E42="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J42" t="str">
-        <f>IF(E42="SIDO","sido_methods",IF(E42="SISO","siso_methods",IF(E42="PT","pt_methods",IF(E42="DISO","diso_methods",IF(E42="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B43" t="s">
+        <v>474</v>
+      </c>
+      <c r="C43" t="s">
         <v>476</v>
-      </c>
-      <c r="C43" t="s">
-        <v>478</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
@@ -3448,26 +3446,26 @@
         <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I43" t="str">
-        <f>IF(E43="SIDO","single-input, double-output",IF(E43="SISO","single-input, single-output",IF(E43="PT","pass-through",IF(E43="DISO","double-input, single-output",IF(E43="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J43" t="str">
-        <f>IF(E43="SIDO","sido_methods",IF(E43="SISO","siso_methods",IF(E43="PT","pt_methods",IF(E43="DISO","diso_methods",IF(E43="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sidor_methods</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B44" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C44" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D44" t="s">
         <v>30</v>
@@ -3482,26 +3480,26 @@
         <v>31</v>
       </c>
       <c r="H44" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I44" t="str">
-        <f>IF(E44="SIDO","single-input, double-output",IF(E44="SISO","single-input, single-output",IF(E44="PT","pass-through",IF(E44="DISO","double-input, single-output",IF(E44="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" si="3"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J44" t="str">
-        <f>IF(E44="SIDO","sido_methods",IF(E44="SISO","siso_methods",IF(E44="PT","pt_methods",IF(E44="DISO","diso_methods",IF(E44="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" si="4"/>
         <v>sidor_methods</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
         <v>105</v>
       </c>
-      <c r="B45" t="s">
-        <v>106</v>
-      </c>
       <c r="C45" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D45" t="s">
         <v>10</v>
@@ -3520,23 +3518,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" ref="I45:I91" si="3">IF(E45="SIDO","single-input, double-output",IF(E45="SISO","single-input, single-output",IF(E45="PT","pass-through",IF(E45="DISO","double-input, single-output",IF(E45="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" ref="I45:I91" si="5">IF(E45="SIDO","single-input, double-output",IF(E45="SISO","single-input, single-output",IF(E45="PT","pass-through",IF(E45="DISO","double-input, single-output",IF(E45="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>pass-through</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" ref="J45:J91" si="4">IF(E45="SIDO","sido_methods",IF(E45="SISO","siso_methods",IF(E45="PT","pt_methods",IF(E45="DISO","diso_methods",IF(E45="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" ref="J45:J91" si="6">IF(E45="SIDO","sido_methods",IF(E45="SISO","siso_methods",IF(E45="PT","pt_methods",IF(E45="DISO","diso_methods",IF(E45="SIDO reactive","sidor_methods","")))))</f>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" t="s">
         <v>107</v>
       </c>
-      <c r="B46" t="s">
-        <v>108</v>
-      </c>
       <c r="C46" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
@@ -3555,23 +3553,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" t="s">
         <v>109</v>
       </c>
-      <c r="B47" t="s">
-        <v>110</v>
-      </c>
       <c r="C47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D47" t="s">
         <v>30</v>
@@ -3586,26 +3584,26 @@
         <v>21</v>
       </c>
       <c r="H47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" t="s">
         <v>112</v>
       </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
       <c r="C48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D48" t="s">
         <v>30</v>
@@ -3620,26 +3618,26 @@
         <v>31</v>
       </c>
       <c r="H48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" t="s">
         <v>115</v>
       </c>
-      <c r="B49" t="s">
-        <v>116</v>
-      </c>
       <c r="C49" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D49" t="s">
         <v>10</v>
@@ -3654,26 +3652,26 @@
         <v>12</v>
       </c>
       <c r="H49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
         <v>118</v>
       </c>
-      <c r="B50" t="s">
-        <v>119</v>
-      </c>
       <c r="C50" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D50" t="s">
         <v>30</v>
@@ -3688,26 +3686,26 @@
         <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sidor_methods</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>480</v>
+      </c>
+      <c r="B51" t="s">
+        <v>481</v>
+      </c>
+      <c r="C51" t="s">
         <v>482</v>
-      </c>
-      <c r="B51" t="s">
-        <v>483</v>
-      </c>
-      <c r="C51" t="s">
-        <v>484</v>
       </c>
       <c r="D51" t="s">
         <v>30</v>
@@ -3722,26 +3720,26 @@
         <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sidor_methods</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" t="s">
         <v>121</v>
       </c>
-      <c r="B52" t="s">
-        <v>122</v>
-      </c>
       <c r="C52" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D52" t="s">
         <v>10</v>
@@ -3760,23 +3758,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" t="s">
         <v>123</v>
       </c>
-      <c r="B53" t="s">
-        <v>124</v>
-      </c>
       <c r="C53" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D53" t="s">
         <v>10</v>
@@ -3795,23 +3793,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>484</v>
+      </c>
+      <c r="B54" t="s">
+        <v>485</v>
+      </c>
+      <c r="C54" t="s">
         <v>486</v>
-      </c>
-      <c r="B54" t="s">
-        <v>487</v>
-      </c>
-      <c r="C54" t="s">
-        <v>488</v>
       </c>
       <c r="D54" t="s">
         <v>30</v>
@@ -3826,26 +3824,26 @@
         <v>12</v>
       </c>
       <c r="H54" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" t="s">
         <v>125</v>
       </c>
-      <c r="B55" t="s">
-        <v>126</v>
-      </c>
       <c r="C55" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D55" t="s">
         <v>30</v>
@@ -3860,26 +3858,26 @@
         <v>31</v>
       </c>
       <c r="H55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sidor_methods</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>488</v>
+      </c>
+      <c r="B56" t="s">
+        <v>489</v>
+      </c>
+      <c r="C56" t="s">
         <v>490</v>
-      </c>
-      <c r="B56" t="s">
-        <v>491</v>
-      </c>
-      <c r="C56" t="s">
-        <v>492</v>
       </c>
       <c r="D56" t="s">
         <v>30</v>
@@ -3894,26 +3892,26 @@
         <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sidor_methods</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" t="s">
         <v>128</v>
       </c>
-      <c r="B57" t="s">
-        <v>129</v>
-      </c>
       <c r="C57" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
@@ -3932,23 +3930,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" t="s">
         <v>130</v>
       </c>
-      <c r="B58" t="s">
-        <v>131</v>
-      </c>
       <c r="C58" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
@@ -3967,23 +3965,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" t="s">
         <v>132</v>
       </c>
-      <c r="B59" t="s">
-        <v>133</v>
-      </c>
       <c r="C59" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
@@ -4001,23 +3999,23 @@
         <v>65</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" t="s">
         <v>134</v>
       </c>
-      <c r="B60" t="s">
-        <v>135</v>
-      </c>
       <c r="C60" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
@@ -4036,23 +4034,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" t="s">
         <v>136</v>
       </c>
-      <c r="B61" t="s">
-        <v>137</v>
-      </c>
       <c r="C61" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D61" t="s">
         <v>30</v>
@@ -4067,26 +4065,26 @@
         <v>31</v>
       </c>
       <c r="H61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B62" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C62" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D62" t="s">
         <v>30</v>
@@ -4101,26 +4099,26 @@
         <v>31</v>
       </c>
       <c r="H62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>siso_methods</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" t="s">
         <v>141</v>
       </c>
-      <c r="B63" t="s">
-        <v>142</v>
-      </c>
       <c r="C63" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D63" t="s">
         <v>30</v>
@@ -4135,26 +4133,26 @@
         <v>31</v>
       </c>
       <c r="H63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>siso_methods</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>492</v>
+      </c>
+      <c r="B64" t="s">
+        <v>493</v>
+      </c>
+      <c r="C64" t="s">
         <v>494</v>
-      </c>
-      <c r="B64" t="s">
-        <v>495</v>
-      </c>
-      <c r="C64" t="s">
-        <v>496</v>
       </c>
       <c r="D64" t="s">
         <v>30</v>
@@ -4169,26 +4167,26 @@
         <v>12</v>
       </c>
       <c r="H64" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sidor_methods</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" t="s">
         <v>144</v>
       </c>
-      <c r="B65" t="s">
-        <v>145</v>
-      </c>
       <c r="C65" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D65" t="s">
         <v>30</v>
@@ -4203,26 +4201,26 @@
         <v>31</v>
       </c>
       <c r="H65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" t="s">
         <v>147</v>
       </c>
-      <c r="B66" t="s">
-        <v>148</v>
-      </c>
       <c r="C66" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D66" t="s">
         <v>10</v>
@@ -4241,23 +4239,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67" t="s">
         <v>149</v>
       </c>
-      <c r="B67" t="s">
-        <v>150</v>
-      </c>
       <c r="C67" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D67" t="s">
         <v>30</v>
@@ -4272,26 +4270,26 @@
         <v>31</v>
       </c>
       <c r="H67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" t="s">
         <v>152</v>
       </c>
-      <c r="B68" t="s">
-        <v>153</v>
-      </c>
       <c r="C68" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
@@ -4310,23 +4308,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" t="s">
         <v>154</v>
       </c>
-      <c r="B69" t="s">
-        <v>155</v>
-      </c>
       <c r="C69" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
@@ -4345,23 +4343,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" t="s">
         <v>156</v>
       </c>
-      <c r="B70" t="s">
-        <v>157</v>
-      </c>
       <c r="C70" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D70" t="s">
         <v>57</v>
@@ -4379,23 +4377,23 @@
         <v>65</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" t="s">
         <v>158</v>
       </c>
-      <c r="B71" t="s">
-        <v>159</v>
-      </c>
       <c r="C71" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D71" t="s">
         <v>30</v>
@@ -4410,26 +4408,26 @@
         <v>12</v>
       </c>
       <c r="H71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" t="s">
         <v>161</v>
       </c>
-      <c r="B72" t="s">
-        <v>162</v>
-      </c>
       <c r="C72" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
@@ -4448,23 +4446,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73" t="s">
         <v>163</v>
       </c>
-      <c r="B73" t="s">
-        <v>164</v>
-      </c>
       <c r="C73" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D73" t="s">
         <v>10</v>
@@ -4483,23 +4481,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" t="s">
         <v>165</v>
       </c>
-      <c r="B74" t="s">
-        <v>166</v>
-      </c>
       <c r="C74" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
@@ -4518,23 +4516,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" t="s">
         <v>167</v>
       </c>
-      <c r="B75" t="s">
-        <v>168</v>
-      </c>
       <c r="C75" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
@@ -4553,23 +4551,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" t="s">
         <v>169</v>
       </c>
-      <c r="B76" t="s">
-        <v>170</v>
-      </c>
       <c r="C76" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D76" t="s">
         <v>30</v>
@@ -4584,26 +4582,26 @@
         <v>12</v>
       </c>
       <c r="H76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>496</v>
+      </c>
+      <c r="B77" t="s">
+        <v>497</v>
+      </c>
+      <c r="C77" t="s">
         <v>498</v>
-      </c>
-      <c r="B77" t="s">
-        <v>499</v>
-      </c>
-      <c r="C77" t="s">
-        <v>500</v>
       </c>
       <c r="D77" t="s">
         <v>10</v>
@@ -4618,26 +4616,26 @@
         <v>12</v>
       </c>
       <c r="H77" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>500</v>
+      </c>
+      <c r="B78" t="s">
+        <v>501</v>
+      </c>
+      <c r="C78" t="s">
         <v>502</v>
-      </c>
-      <c r="B78" t="s">
-        <v>503</v>
-      </c>
-      <c r="C78" t="s">
-        <v>504</v>
       </c>
       <c r="D78" t="s">
         <v>10</v>
@@ -4652,26 +4650,26 @@
         <v>12</v>
       </c>
       <c r="H78" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B79" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C79" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D79" t="s">
         <v>30</v>
@@ -4686,26 +4684,26 @@
         <v>31</v>
       </c>
       <c r="H79" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>171</v>
+      </c>
+      <c r="B80" t="s">
         <v>172</v>
       </c>
-      <c r="B80" t="s">
-        <v>173</v>
-      </c>
       <c r="C80" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D80" t="s">
         <v>30</v>
@@ -4720,26 +4718,26 @@
         <v>21</v>
       </c>
       <c r="H80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>174</v>
+      </c>
+      <c r="B81" t="s">
         <v>175</v>
       </c>
-      <c r="B81" t="s">
-        <v>176</v>
-      </c>
       <c r="C81" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D81" t="s">
         <v>10</v>
@@ -4758,23 +4756,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>176</v>
+      </c>
+      <c r="B82" t="s">
         <v>177</v>
       </c>
-      <c r="B82" t="s">
-        <v>178</v>
-      </c>
       <c r="C82" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
@@ -4793,23 +4791,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>178</v>
+      </c>
+      <c r="B83" t="s">
         <v>179</v>
       </c>
-      <c r="B83" t="s">
-        <v>180</v>
-      </c>
       <c r="C83" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
@@ -4828,23 +4826,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J83" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" t="s">
         <v>181</v>
       </c>
-      <c r="B84" t="s">
-        <v>182</v>
-      </c>
       <c r="C84" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D84" t="s">
         <v>10</v>
@@ -4863,23 +4861,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" t="s">
         <v>183</v>
       </c>
-      <c r="B85" t="s">
-        <v>184</v>
-      </c>
       <c r="C85" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D85" t="s">
         <v>30</v>
@@ -4894,26 +4892,26 @@
         <v>12</v>
       </c>
       <c r="H85" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>siso_methods</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>185</v>
+      </c>
+      <c r="B86" t="s">
         <v>186</v>
       </c>
-      <c r="B86" t="s">
-        <v>187</v>
-      </c>
       <c r="C86" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D86" t="s">
         <v>30</v>
@@ -4928,26 +4926,26 @@
         <v>12</v>
       </c>
       <c r="H86" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, single-output</v>
       </c>
       <c r="J86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>siso_methods</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" t="s">
         <v>189</v>
       </c>
-      <c r="B87" t="s">
-        <v>190</v>
-      </c>
       <c r="C87" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D87" t="s">
         <v>57</v>
@@ -4962,26 +4960,26 @@
         <v>12</v>
       </c>
       <c r="H87" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" t="s">
         <v>191</v>
       </c>
-      <c r="B88" t="s">
-        <v>192</v>
-      </c>
       <c r="C88" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
@@ -5000,23 +4998,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J88" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>192</v>
+      </c>
+      <c r="B89" t="s">
         <v>193</v>
       </c>
-      <c r="B89" t="s">
-        <v>194</v>
-      </c>
       <c r="C89" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
@@ -5035,23 +5033,23 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>single-input, double-output</v>
       </c>
       <c r="J89" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>sido_methods</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>194</v>
+      </c>
+      <c r="B90" t="s">
         <v>195</v>
       </c>
-      <c r="B90" t="s">
-        <v>196</v>
-      </c>
       <c r="C90" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D90" t="s">
         <v>30</v>
@@ -5069,23 +5067,23 @@
         <v>65</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J90" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>196</v>
+      </c>
+      <c r="B91" t="s">
         <v>197</v>
       </c>
-      <c r="B91" t="s">
-        <v>198</v>
-      </c>
       <c r="C91" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D91" t="s">
         <v>30</v>
@@ -5100,14 +5098,14 @@
         <v>21</v>
       </c>
       <c r="H91" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
       <c r="J91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
@@ -5137,17 +5135,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE(A1,"_zo")</f>
         <v>aeration_basin_zo</v>
       </c>
       <c r="C1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" t="s">
         <v>201</v>
-      </c>
-      <c r="D1" t="s">
-        <v>202</v>
       </c>
       <c r="G1" t="str">
         <f>CONCATENATE(C1," ",D1)</f>
@@ -5156,17 +5154,17 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B65" si="0">CONCATENATE(A2,"_zo")</f>
         <v>air_flotation_zo</v>
       </c>
       <c r="C2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" t="s">
         <v>204</v>
-      </c>
-      <c r="D2" t="s">
-        <v>205</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G65" si="1">CONCATENATE(C2," ",D2)</f>
@@ -5175,20 +5173,20 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
         <v>anaerobic_digestion_oxidation_zo</v>
       </c>
       <c r="C3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" t="s">
         <v>207</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>208</v>
-      </c>
-      <c r="E3" t="s">
-        <v>209</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="1"/>
@@ -5197,20 +5195,20 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
         <v>anaerobic_mbr_mec_zo</v>
       </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" t="s">
         <v>211</v>
-      </c>
-      <c r="E4" t="s">
-        <v>212</v>
       </c>
       <c r="G4" t="str">
         <f>CONCATENATE(C4," ",D4," ",E4)</f>
@@ -5219,20 +5217,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>backwash_solids_handling_zo</v>
       </c>
       <c r="C5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
         <v>214</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>215</v>
-      </c>
-      <c r="E5" t="s">
-        <v>216</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ref="G5:G6" si="2">CONCATENATE(C5," ",D5," ",E5)</f>
@@ -5241,20 +5239,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>bio_active_filtration_zo</v>
       </c>
       <c r="C6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" t="s">
         <v>218</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>219</v>
-      </c>
-      <c r="E6" t="s">
-        <v>220</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="2"/>
@@ -5263,14 +5261,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>bioreactor_zo</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -5279,17 +5277,17 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>blending_resevoir_zo</v>
       </c>
       <c r="C8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" t="s">
         <v>223</v>
-      </c>
-      <c r="D8" t="s">
-        <v>224</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
@@ -5298,17 +5296,17 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>brine_concentrator_zo</v>
       </c>
       <c r="C9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" t="s">
         <v>226</v>
-      </c>
-      <c r="D9" t="s">
-        <v>227</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -5317,17 +5315,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>buffer_tank_zo</v>
       </c>
       <c r="C10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" t="s">
         <v>229</v>
-      </c>
-      <c r="D10" t="s">
-        <v>230</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -5336,14 +5334,14 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>CANDOP_zo</v>
       </c>
       <c r="C11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -5352,17 +5350,17 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>cartridge_filtration_zo</v>
       </c>
       <c r="C12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -5371,17 +5369,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>chemical_addition_zo</v>
       </c>
       <c r="C13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" t="s">
         <v>235</v>
-      </c>
-      <c r="D13" t="s">
-        <v>236</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -5390,14 +5388,14 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>chlorination_zo</v>
       </c>
       <c r="C14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -5406,14 +5404,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>clarifier_zo</v>
       </c>
       <c r="C15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -5422,17 +5420,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>co2_addition_zo</v>
       </c>
       <c r="C16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -5441,20 +5439,20 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v>coag_and_floc_zo</v>
       </c>
       <c r="C17" t="s">
+        <v>241</v>
+      </c>
+      <c r="D17" t="s">
         <v>242</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>243</v>
-      </c>
-      <c r="E17" t="s">
-        <v>244</v>
       </c>
       <c r="G17" t="str">
         <f>CONCATENATE(C17," ",D17," ",E17)</f>
@@ -5463,14 +5461,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>cofermentation_zo</v>
       </c>
       <c r="C18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ref="G18:G19" si="3">CONCATENATE(C18," ",D18," ",E18)</f>
@@ -5479,17 +5477,17 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>constructed_wetlands_zo</v>
       </c>
       <c r="C19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" t="s">
         <v>247</v>
-      </c>
-      <c r="D19" t="s">
-        <v>248</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="3"/>
@@ -5498,20 +5496,20 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>conventional_activated_sludge_zo</v>
       </c>
       <c r="C20" t="s">
+        <v>249</v>
+      </c>
+      <c r="D20" t="s">
         <v>250</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>251</v>
-      </c>
-      <c r="E20" t="s">
-        <v>252</v>
       </c>
       <c r="G20" t="str">
         <f>CONCATENATE(C20," ",D20," ",E20)</f>
@@ -5520,17 +5518,17 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>cooling_supply_zo</v>
       </c>
       <c r="C21" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" t="s">
         <v>254</v>
-      </c>
-      <c r="D21" t="s">
-        <v>255</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ref="G21:G22" si="4">CONCATENATE(C21," ",D21," ",E21)</f>
@@ -5539,17 +5537,17 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>cooling_tower_zo</v>
       </c>
       <c r="C22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="4"/>
@@ -5558,14 +5556,14 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>decarbonator_zo</v>
       </c>
       <c r="C23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -5574,20 +5572,20 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v>deep_well_injection_zo</v>
       </c>
       <c r="C24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" t="s">
         <v>260</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>261</v>
-      </c>
-      <c r="E24" t="s">
-        <v>262</v>
       </c>
       <c r="G24" t="str">
         <f>CONCATENATE(C24," ",D24," ",E24)</f>
@@ -5596,20 +5594,20 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>dissolved_air_flotation_zo</v>
       </c>
       <c r="C25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D25" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" t="s">
         <v>204</v>
-      </c>
-      <c r="E25" t="s">
-        <v>205</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ref="G25" si="5">CONCATENATE(C25," ",D25," ",E25)</f>
@@ -5618,14 +5616,14 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>dmbr_zo</v>
       </c>
       <c r="C26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G26" t="str">
         <f>CONCATENATE(C26," ",D26)</f>
@@ -5634,20 +5632,20 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
         <v>dual_media_filtration_zo</v>
       </c>
       <c r="C27" t="s">
+        <v>266</v>
+      </c>
+      <c r="D27" t="s">
         <v>267</v>
       </c>
-      <c r="D27" t="s">
-        <v>268</v>
-      </c>
       <c r="E27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G27" t="str">
         <f>CONCATENATE(C27," ",D27," ",E27)</f>
@@ -5656,20 +5654,20 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
         <v>electrochemical_nutrient_removal_zo</v>
       </c>
       <c r="C28" t="s">
+        <v>269</v>
+      </c>
+      <c r="D28" t="s">
         <v>270</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>271</v>
-      </c>
-      <c r="E28" t="s">
-        <v>272</v>
       </c>
       <c r="G28" t="str">
         <f>CONCATENATE(C28," ",D28," ",E28)</f>
@@ -5678,17 +5676,17 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
         <v>electrodialysis_reversal_zo</v>
       </c>
       <c r="C29" t="s">
+        <v>273</v>
+      </c>
+      <c r="D29" t="s">
         <v>274</v>
-      </c>
-      <c r="D29" t="s">
-        <v>275</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -5697,7 +5695,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -5707,7 +5705,7 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -5716,17 +5714,17 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
         <v>evaporation_pond_zo</v>
       </c>
       <c r="C31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D31" t="s">
         <v>279</v>
-      </c>
-      <c r="D31" t="s">
-        <v>280</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -5735,20 +5733,20 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
         <v>feed_water_tank_zo</v>
       </c>
       <c r="C32" t="s">
+        <v>281</v>
+      </c>
+      <c r="D32" t="s">
         <v>282</v>
       </c>
-      <c r="D32" t="s">
-        <v>283</v>
-      </c>
       <c r="E32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G32" t="str">
         <f>CONCATENATE(C32," ",D32," ",E32)</f>
@@ -5757,14 +5755,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>feed_zo</v>
       </c>
       <c r="C33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -5773,17 +5771,17 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
         <v>filter_press_zo</v>
       </c>
       <c r="C34" t="s">
+        <v>284</v>
+      </c>
+      <c r="D34" t="s">
         <v>285</v>
-      </c>
-      <c r="D34" t="s">
-        <v>286</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -5792,17 +5790,17 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>fixed_bed_zo</v>
       </c>
       <c r="C35" t="s">
+        <v>287</v>
+      </c>
+      <c r="D35" t="s">
         <v>288</v>
-      </c>
-      <c r="D35" t="s">
-        <v>289</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -5811,14 +5809,14 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>gac_zo</v>
       </c>
       <c r="C36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -5827,20 +5825,20 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>gas_sparged_membrane_zo</v>
       </c>
       <c r="C37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D37" t="s">
         <v>292</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>293</v>
-      </c>
-      <c r="E37" t="s">
-        <v>294</v>
       </c>
       <c r="G37" t="str">
         <f>CONCATENATE(C37," ",D37," ",E37)</f>
@@ -5849,20 +5847,20 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>injection_well_disposal_zo</v>
       </c>
       <c r="C38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G38" t="str">
         <f>CONCATENATE(C38," ",D38," ",E38)</f>
@@ -5871,17 +5869,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>intrusion_mitigation_zo</v>
       </c>
       <c r="C39" t="s">
+        <v>297</v>
+      </c>
+      <c r="D39" t="s">
         <v>298</v>
-      </c>
-      <c r="D39" t="s">
-        <v>299</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -5890,17 +5888,17 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>ion_exchange_zo</v>
       </c>
       <c r="C40" t="s">
+        <v>300</v>
+      </c>
+      <c r="D40" t="s">
         <v>301</v>
-      </c>
-      <c r="D40" t="s">
-        <v>302</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -5909,23 +5907,23 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>iron_and_manganese_removal_zo</v>
       </c>
       <c r="C41" t="s">
+        <v>303</v>
+      </c>
+      <c r="D41" t="s">
+        <v>242</v>
+      </c>
+      <c r="E41" t="s">
         <v>304</v>
       </c>
-      <c r="D41" t="s">
-        <v>243</v>
-      </c>
-      <c r="E41" t="s">
-        <v>305</v>
-      </c>
       <c r="F41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G41" t="str">
         <f>CONCATENATE(C41," ",D41," ",E41," ",F41)</f>
@@ -5934,14 +5932,14 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>landfill_zo</v>
       </c>
       <c r="C42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -5950,14 +5948,14 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>mabr_zo</v>
       </c>
       <c r="C43" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -5966,14 +5964,14 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>mbr_zo</v>
       </c>
       <c r="C44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -5982,17 +5980,17 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>media_filtration_zo</v>
       </c>
       <c r="C45" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -6001,14 +5999,14 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>metab_zo</v>
       </c>
       <c r="C46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -6017,14 +6015,14 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>microfiltration_zo</v>
       </c>
       <c r="C47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -6033,17 +6031,17 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
         <v>microscreen_filtration_zo</v>
       </c>
       <c r="C48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -6052,17 +6050,17 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
         <v>municipal_drinking_zo</v>
       </c>
       <c r="C49" t="s">
+        <v>313</v>
+      </c>
+      <c r="D49" t="s">
         <v>314</v>
-      </c>
-      <c r="D49" t="s">
-        <v>315</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -6071,17 +6069,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
         <v>municipal_wwtp_zo</v>
       </c>
       <c r="C50" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D50" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -6090,14 +6088,14 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>nanofiltration_zo</v>
       </c>
       <c r="C51" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -6106,17 +6104,17 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
         <v>ozone_aop _zo</v>
       </c>
       <c r="C52" t="s">
+        <v>319</v>
+      </c>
+      <c r="D52" t="s">
         <v>320</v>
-      </c>
-      <c r="D52" t="s">
-        <v>321</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -6125,14 +6123,14 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>ozone_zo</v>
       </c>
       <c r="C53" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -6141,17 +6139,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
         <v>photothermal_membrane_zo</v>
       </c>
       <c r="C54" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D54" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -6160,17 +6158,17 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
         <v>primary_separator_zo</v>
       </c>
       <c r="C55" t="s">
+        <v>324</v>
+      </c>
+      <c r="D55" t="s">
         <v>325</v>
-      </c>
-      <c r="D55" t="s">
-        <v>326</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -6186,10 +6184,10 @@
         <v>pump_electricity_zo</v>
       </c>
       <c r="C56" t="s">
+        <v>326</v>
+      </c>
+      <c r="D56" t="s">
         <v>327</v>
-      </c>
-      <c r="D56" t="s">
-        <v>328</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
@@ -6198,14 +6196,14 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
         <v>pump_zo</v>
       </c>
       <c r="C57" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -6214,14 +6212,14 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
         <v>screen_zo</v>
       </c>
       <c r="C58" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -6230,20 +6228,20 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="0"/>
         <v>secondary_treatment_wwtp_zo</v>
       </c>
       <c r="C59" t="s">
+        <v>330</v>
+      </c>
+      <c r="D59" t="s">
         <v>331</v>
       </c>
-      <c r="D59" t="s">
-        <v>332</v>
-      </c>
       <c r="E59" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G59" t="str">
         <f>CONCATENATE(C59," ",D59," ",E59)</f>
@@ -6252,14 +6250,14 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
         <v>sedimentation_zo</v>
       </c>
       <c r="C60" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -6268,17 +6266,17 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="0"/>
         <v>settling_pond_zo</v>
       </c>
       <c r="C61" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D61" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -6287,17 +6285,17 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
         <v>sludge_tank_zo</v>
       </c>
       <c r="C62" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -6306,14 +6304,14 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
         <v>smp_zo</v>
       </c>
       <c r="C63" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -6322,17 +6320,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="0"/>
         <v>static_mixer_zo</v>
       </c>
       <c r="C64" t="s">
+        <v>338</v>
+      </c>
+      <c r="D64" t="s">
         <v>339</v>
-      </c>
-      <c r="D64" t="s">
-        <v>340</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -6341,17 +6339,17 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="0"/>
         <v>storage_tank_zo</v>
       </c>
       <c r="C65" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D65" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -6360,17 +6358,17 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" ref="B66:B77" si="6">CONCATENATE(A66,"_zo")</f>
         <v>surface_discharge_zo</v>
       </c>
       <c r="C66" t="s">
+        <v>343</v>
+      </c>
+      <c r="D66" t="s">
         <v>344</v>
-      </c>
-      <c r="D66" t="s">
-        <v>345</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" ref="G66:G77" si="7">CONCATENATE(C66," ",D66)</f>
@@ -6379,20 +6377,20 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="6"/>
         <v>sw_onshore_intake_zo</v>
       </c>
       <c r="C67" t="s">
+        <v>346</v>
+      </c>
+      <c r="D67" t="s">
         <v>347</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>348</v>
-      </c>
-      <c r="E67" t="s">
-        <v>349</v>
       </c>
       <c r="G67" t="str">
         <f>CONCATENATE(C67," ",D67," ",E67)</f>
@@ -6401,20 +6399,20 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="6"/>
         <v>tramp_oil_tank_zo</v>
       </c>
       <c r="C68" t="s">
+        <v>350</v>
+      </c>
+      <c r="D68" t="s">
         <v>351</v>
       </c>
-      <c r="D68" t="s">
-        <v>352</v>
-      </c>
       <c r="E68" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" ref="G68:G69" si="8">CONCATENATE(C68," ",D68," ",E68)</f>
@@ -6423,20 +6421,20 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="6"/>
         <v>tri_media_filtration_zo</v>
       </c>
       <c r="C69" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D69" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="8"/>
@@ -6445,17 +6443,17 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="6"/>
         <v>ultra_filtration_zo</v>
       </c>
       <c r="C70" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D70" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="7"/>
@@ -6464,17 +6462,17 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="6"/>
         <v>uv_aop_zo</v>
       </c>
       <c r="C71" t="s">
+        <v>357</v>
+      </c>
+      <c r="D71" t="s">
         <v>358</v>
-      </c>
-      <c r="D71" t="s">
-        <v>359</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="7"/>
@@ -6483,14 +6481,14 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="6"/>
         <v>uv_zo</v>
       </c>
       <c r="C72" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="7"/>
@@ -6499,17 +6497,17 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="6"/>
         <v>vfa_recovery_zo</v>
       </c>
       <c r="C73" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D73" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="7"/>
@@ -6518,14 +6516,14 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="6"/>
         <v>waiv_zo</v>
       </c>
       <c r="C74" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="7"/>
@@ -6534,20 +6532,20 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="6"/>
         <v>walnut_shell_filter_zo</v>
       </c>
       <c r="C75" t="s">
+        <v>363</v>
+      </c>
+      <c r="D75" t="s">
         <v>364</v>
       </c>
-      <c r="D75" t="s">
-        <v>365</v>
-      </c>
       <c r="E75" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ref="G75:G76" si="9">CONCATENATE(C75," ",D75," ",E75)</f>
@@ -6556,20 +6554,20 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="6"/>
         <v>water_pumping_station_zo</v>
       </c>
       <c r="C76" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D76" t="s">
+        <v>366</v>
+      </c>
+      <c r="E76" t="s">
         <v>367</v>
-      </c>
-      <c r="E76" t="s">
-        <v>368</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="9"/>
@@ -6578,17 +6576,17 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="6"/>
         <v>well_field_zo</v>
       </c>
       <c r="C77" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D77" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="7"/>
@@ -6619,7 +6617,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
@@ -6627,7 +6625,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
@@ -6635,7 +6633,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -6643,15 +6641,15 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -6659,7 +6657,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
@@ -6667,7 +6665,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
@@ -6675,15 +6673,15 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
@@ -6691,7 +6689,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
@@ -6699,7 +6697,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
@@ -6707,7 +6705,7 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
@@ -6715,7 +6713,7 @@
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
@@ -6723,7 +6721,7 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
@@ -6731,7 +6729,7 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
@@ -6739,7 +6737,7 @@
         <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -6747,7 +6745,7 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
@@ -6755,7 +6753,7 @@
         <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
@@ -6763,7 +6761,7 @@
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -6771,7 +6769,7 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
@@ -6779,7 +6777,7 @@
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
@@ -6787,7 +6785,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
@@ -6795,7 +6793,7 @@
         <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
@@ -6803,7 +6801,7 @@
         <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
@@ -6811,7 +6809,7 @@
         <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
@@ -6819,7 +6817,7 @@
         <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
@@ -6827,7 +6825,7 @@
         <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
@@ -6835,7 +6833,7 @@
         <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
@@ -6843,7 +6841,7 @@
         <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
@@ -6851,7 +6849,7 @@
         <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
@@ -6859,7 +6857,7 @@
         <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
@@ -6867,7 +6865,7 @@
         <v>86</v>
       </c>
       <c r="C32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
@@ -6875,7 +6873,7 @@
         <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
@@ -6883,7 +6881,7 @@
         <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
@@ -6891,7 +6889,7 @@
         <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
@@ -6899,7 +6897,7 @@
         <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
@@ -6907,351 +6905,351 @@
         <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C39" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C46" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C49" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C52" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C54" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C55" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C56" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C58" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C61" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C62" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C63" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C65" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C66" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C67" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C68" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C69" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C70" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C71" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C73" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C74" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C76" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C77" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C78" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C79" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C80" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel updatted properly now
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592FA0B6-2293-4B38-A619-6793CEE2CE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDB7974-2905-4DB3-9B67-7B5EA810D191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="508">
   <si>
     <t>Name</t>
   </si>
@@ -1553,6 +1553,9 @@
   </si>
   <si>
     <t>anaerobic digestion</t>
+  </si>
+  <si>
+    <t>cost_gac</t>
   </si>
 </sst>
 </file>
@@ -1963,7 +1966,7 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3376,9 +3379,8 @@
       <c r="G41" t="s">
         <v>31</v>
       </c>
-      <c r="H41" t="b">
-        <f>IF(D38="basic","cost_power_law_flow")</f>
-        <v>0</v>
+      <c r="H41" t="s">
+        <v>507</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="3"/>
@@ -3411,8 +3413,8 @@
       <c r="G42" t="s">
         <v>21</v>
       </c>
-      <c r="H42" t="s">
-        <v>65</v>
+      <c r="H42" t="b">
+        <v>0</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
modify and run automate_rst_file_wt3 to generate more extensive document for electrocoagulation_zo
</commit_message>
<xml_diff>
--- a/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
+++ b/docs/technical_reference/unit_models/zero_order_unit_models/WT3_unit_classification_for_doc.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDB7974-2905-4DB3-9B67-7B5EA810D191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54105F9-699E-40C1-91E9-7B98EAFB177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$92</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="512">
   <si>
     <t>Name</t>
   </si>
@@ -1556,6 +1556,18 @@
   </si>
   <si>
     <t>cost_gac</t>
+  </si>
+  <si>
+    <t>electrocoagulation</t>
+  </si>
+  <si>
+    <t>electrocoagulation_zo</t>
+  </si>
+  <si>
+    <t>ElectrocoagulationZO</t>
+  </si>
+  <si>
+    <t>cost_electrocoagulation</t>
   </si>
 </sst>
 </file>
@@ -1963,26 +1975,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.46484375" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.53125" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="38.5546875" customWidth="1"/>
-    <col min="9" max="9" width="30.21875" customWidth="1"/>
-    <col min="10" max="10" width="25.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" customWidth="1"/>
+    <col min="8" max="8" width="38.53125" customWidth="1"/>
+    <col min="9" max="9" width="30.19921875" customWidth="1"/>
+    <col min="10" max="10" width="25.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2014,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2041,15 +2053,15 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I37" si="1">IF(E2="SIDO","single-input, double-output",IF(E2="SISO","single-input, single-output",IF(E2="PT","pass-through",IF(E2="DISO","double-input, single-output",IF(E2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <f t="shared" ref="I2:I38" si="1">IF(E2="SIDO","single-input, double-output",IF(E2="SISO","single-input, single-output",IF(E2="PT","pass-through",IF(E2="DISO","double-input, single-output",IF(E2="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
         <v>single-input, double-output</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J37" si="2">IF(E2="SIDO","sido_methods",IF(E2="SISO","siso_methods",IF(E2="PT","pt_methods",IF(E2="DISO","diso_methods",IF(E2="SIDO reactive","sidor_methods","")))))</f>
+        <f t="shared" ref="J2:J38" si="2">IF(E2="SIDO","sido_methods",IF(E2="SISO","siso_methods",IF(E2="PT","pt_methods",IF(E2="DISO","diso_methods",IF(E2="SIDO reactive","sidor_methods","")))))</f>
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2084,7 +2096,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>506</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>463</v>
       </c>
@@ -2153,7 +2165,7 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2187,7 +2199,7 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -2221,7 +2233,7 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2256,7 +2268,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2291,7 +2303,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2326,7 +2338,7 @@
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>372</v>
       </c>
@@ -2361,7 +2373,7 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2395,7 +2407,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -2430,7 +2442,7 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2499,7 +2511,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>467</v>
       </c>
@@ -2533,7 +2545,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2567,7 +2579,7 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2601,7 +2613,7 @@
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2636,7 +2648,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>471</v>
       </c>
@@ -2670,7 +2682,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2705,7 +2717,7 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2739,7 +2751,7 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2773,7 +2785,7 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2807,7 +2819,7 @@
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2877,7 +2889,7 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2911,7 +2923,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -2946,7 +2958,7 @@
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2980,7 +2992,7 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -3015,7 +3027,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -3049,7 +3061,7 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -3084,7 +3096,7 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -3118,15 +3130,15 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>508</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>509</v>
       </c>
       <c r="C34" t="s">
-        <v>382</v>
+        <v>510</v>
       </c>
       <c r="D34" t="s">
         <v>30</v>
@@ -3141,7 +3153,7 @@
         <v>31</v>
       </c>
       <c r="H34" t="s">
-        <v>65</v>
+        <v>511</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="1"/>
@@ -3152,56 +3164,55 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="str">
-        <f>IF(D35="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+        <v>31</v>
+      </c>
+      <c r="H35" t="s">
+        <v>65</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="1"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="2"/>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>437</v>
+        <v>396</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
@@ -3209,33 +3220,34 @@
       <c r="G36" t="s">
         <v>12</v>
       </c>
-      <c r="H36" t="s">
-        <v>87</v>
+      <c r="H36" t="str">
+        <f>IF(D36="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="1"/>
-        <v>single-input, double-output</v>
+        <v>pass-through</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="2"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>pt_methods</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>393</v>
+        <v>437</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
@@ -3243,163 +3255,163 @@
       <c r="G37" t="s">
         <v>12</v>
       </c>
-      <c r="H37" t="str">
-        <f>IF(D37="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+      <c r="H37" t="s">
+        <v>87</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="1"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="2"/>
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>393</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" t="str">
+        <f>IF(D38="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v>pass-through</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="2"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>90</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>91</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>394</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>92</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>58</v>
-      </c>
-      <c r="F38" t="b">
-        <v>0</v>
-      </c>
-      <c r="G38" t="s">
-        <v>58</v>
-      </c>
-      <c r="H38" t="b">
-        <f>IF(D38="basic","cost_power_law_flow")</f>
-        <v>0</v>
-      </c>
-      <c r="I38" t="s">
-        <v>93</v>
-      </c>
-      <c r="J38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" t="s">
-        <v>438</v>
-      </c>
-      <c r="D39" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" t="s">
-        <v>11</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>31</v>
-      </c>
-      <c r="H39" t="s">
-        <v>96</v>
-      </c>
-      <c r="I39" t="str">
-        <f t="shared" ref="I39:I44" si="3">IF(E39="SIDO","single-input, double-output",IF(E39="SISO","single-input, single-output",IF(E39="PT","pass-through",IF(E39="DISO","double-input, single-output",IF(E39="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
-        <v>single-input, double-output</v>
-      </c>
-      <c r="J39" t="str">
-        <f t="shared" ref="J39:J44" si="4">IF(E39="SIDO","sido_methods",IF(E39="SISO","siso_methods",IF(E39="PT","pt_methods",IF(E39="DISO","diso_methods",IF(E39="SIDO reactive","sidor_methods","")))))</f>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="H39" t="b">
+        <f>IF(D39="basic","cost_power_law_flow")</f>
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>93</v>
+      </c>
+      <c r="J39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>423</v>
+        <v>438</v>
       </c>
       <c r="D40" t="s">
         <v>30</v>
       </c>
       <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" ref="I40:I45" si="3">IF(E40="SIDO","single-input, double-output",IF(E40="SISO","single-input, single-output",IF(E40="PT","pass-through",IF(E40="DISO","double-input, single-output",IF(E40="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <v>single-input, double-output</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" ref="J40:J45" si="4">IF(E40="SIDO","sido_methods",IF(E40="SISO","siso_methods",IF(E40="PT","pt_methods",IF(E40="DISO","diso_methods",IF(E40="SIDO reactive","sidor_methods","")))))</f>
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>423</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
         <v>26</v>
       </c>
-      <c r="F40" t="b">
+      <c r="F41" t="b">
         <v>1</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G41" t="s">
         <v>12</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H41" t="s">
         <v>99</v>
       </c>
-      <c r="I40" t="str">
+      <c r="I41" t="str">
         <f t="shared" si="3"/>
         <v>single-input, single-output</v>
       </c>
-      <c r="J40" t="str">
+      <c r="J41" t="str">
         <f t="shared" si="4"/>
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>100</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>429</v>
-      </c>
-      <c r="D41" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" t="b">
-        <v>0</v>
-      </c>
-      <c r="G41" t="s">
-        <v>31</v>
-      </c>
-      <c r="H41" t="s">
-        <v>507</v>
-      </c>
-      <c r="I41" t="str">
-        <f t="shared" si="3"/>
-        <v>single-input, double-output</v>
-      </c>
-      <c r="J41" t="str">
-        <f t="shared" si="4"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" t="s">
-        <v>451</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
@@ -3408,13 +3420,13 @@
         <v>11</v>
       </c>
       <c r="F42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" t="b">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="H42" t="s">
+        <v>507</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="3"/>
@@ -3425,52 +3437,52 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>475</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>474</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" t="s">
-        <v>477</v>
+        <v>21</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="3"/>
-        <v>reactive single-inlet, double-outlet</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="4"/>
-        <v>sidor_methods</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B44" t="s">
-        <v>456</v>
+        <v>474</v>
       </c>
       <c r="C44" t="s">
-        <v>452</v>
+        <v>476</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E44" t="s">
         <v>18</v>
@@ -3479,10 +3491,10 @@
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="3"/>
@@ -3493,50 +3505,49 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>478</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>456</v>
       </c>
       <c r="C45" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" t="str">
-        <f>IF(D45="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+        <v>31</v>
+      </c>
+      <c r="H45" t="s">
+        <v>479</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" ref="I45:I91" si="5">IF(E45="SIDO","single-input, double-output",IF(E45="SISO","single-input, single-output",IF(E45="PT","pass-through",IF(E45="DISO","double-input, single-output",IF(E45="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
-        <v>pass-through</v>
+        <f t="shared" si="3"/>
+        <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" ref="J45:J91" si="6">IF(E45="SIDO","sido_methods",IF(E45="SISO","siso_methods",IF(E45="PT","pt_methods",IF(E45="DISO","diso_methods",IF(E45="SIDO reactive","sidor_methods","")))))</f>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>sidor_methods</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
@@ -3555,57 +3566,58 @@
         <v>cost_power_law_flow</v>
       </c>
       <c r="I46" t="str">
+        <f t="shared" ref="I46:I92" si="5">IF(E46="SIDO","single-input, double-output",IF(E46="SISO","single-input, single-output",IF(E46="PT","pass-through",IF(E46="DISO","double-input, single-output",IF(E46="SIDO reactive","reactive single-inlet, double-outlet","")))))</f>
+        <v>pass-through</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" ref="J46:J92" si="6">IF(E46="SIDO","sido_methods",IF(E46="SISO","siso_methods",IF(E46="PT","pt_methods",IF(E46="DISO","diso_methods",IF(E46="SIDO reactive","sidor_methods","")))))</f>
+        <v>pt_methods</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" t="s">
+        <v>441</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="str">
+        <f>IF(D47="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
+      </c>
+      <c r="I47" t="str">
         <f t="shared" si="5"/>
         <v>pass-through</v>
       </c>
-      <c r="J46" t="str">
+      <c r="J47" t="str">
         <f t="shared" si="6"/>
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>108</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>109</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>427</v>
-      </c>
-      <c r="D47" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" t="b">
-        <v>1</v>
-      </c>
-      <c r="G47" t="s">
-        <v>21</v>
-      </c>
-      <c r="H47" t="s">
-        <v>110</v>
-      </c>
-      <c r="I47" t="str">
-        <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
-      </c>
-      <c r="J47" t="str">
-        <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48" t="s">
-        <v>397</v>
       </c>
       <c r="D48" t="s">
         <v>30</v>
@@ -3614,13 +3626,13 @@
         <v>11</v>
       </c>
       <c r="F48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H48" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="5"/>
@@ -3631,55 +3643,55 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E49" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H49" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="5"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="6"/>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C50" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D50" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
@@ -3688,26 +3700,26 @@
         <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="5"/>
-        <v>reactive single-inlet, double-outlet</v>
+        <v>pass-through</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="6"/>
-        <v>sidor_methods</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+        <v>pt_methods</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>480</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>481</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>482</v>
+        <v>400</v>
       </c>
       <c r="D51" t="s">
         <v>30</v>
@@ -3722,7 +3734,7 @@
         <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>483</v>
+        <v>119</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="5"/>
@@ -3733,21 +3745,21 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>481</v>
       </c>
       <c r="C52" t="s">
-        <v>401</v>
+        <v>482</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
@@ -3755,28 +3767,27 @@
       <c r="G52" t="s">
         <v>12</v>
       </c>
-      <c r="H52" t="str">
-        <f>IF(D52="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+      <c r="H52" t="s">
+        <v>483</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sidor_methods</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C53" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D53" t="s">
         <v>10</v>
@@ -3803,18 +3814,18 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>484</v>
+        <v>122</v>
       </c>
       <c r="B54" t="s">
-        <v>485</v>
+        <v>123</v>
       </c>
       <c r="C54" t="s">
-        <v>486</v>
+        <v>402</v>
       </c>
       <c r="D54" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E54" t="s">
         <v>11</v>
@@ -3825,8 +3836,9 @@
       <c r="G54" t="s">
         <v>12</v>
       </c>
-      <c r="H54" t="s">
-        <v>487</v>
+      <c r="H54" t="str">
+        <f>IF(D54="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="5"/>
@@ -3837,49 +3849,49 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>484</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>485</v>
       </c>
       <c r="C55" t="s">
-        <v>386</v>
+        <v>486</v>
       </c>
       <c r="D55" t="s">
         <v>30</v>
       </c>
       <c r="E55" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>126</v>
+        <v>487</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="5"/>
-        <v>reactive single-inlet, double-outlet</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="6"/>
-        <v>sidor_methods</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>488</v>
+        <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>489</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>490</v>
+        <v>386</v>
       </c>
       <c r="D56" t="s">
         <v>30</v>
@@ -3888,13 +3900,13 @@
         <v>18</v>
       </c>
       <c r="F56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H56" t="s">
-        <v>491</v>
+        <v>126</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="5"/>
@@ -3905,21 +3917,21 @@
         <v>sidor_methods</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>488</v>
       </c>
       <c r="B57" t="s">
-        <v>128</v>
+        <v>489</v>
       </c>
       <c r="C57" t="s">
-        <v>403</v>
+        <v>490</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -3927,28 +3939,27 @@
       <c r="G57" t="s">
         <v>12</v>
       </c>
-      <c r="H57" t="str">
-        <f>IF(D57="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+      <c r="H57" t="s">
+        <v>491</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sidor_methods</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C58" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
@@ -3975,49 +3986,50 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
       </c>
       <c r="E59" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" t="s">
-        <v>65</v>
+        <v>12</v>
+      </c>
+      <c r="H59" t="str">
+        <f>IF(D59="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="5"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="6"/>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>405</v>
+        <v>424</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
@@ -4029,11 +4041,10 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" t="str">
-        <f>IF(D60="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+        <v>21</v>
+      </c>
+      <c r="H60" t="s">
+        <v>65</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="5"/>
@@ -4044,55 +4055,56 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C61" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D61" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>31</v>
-      </c>
-      <c r="H61" t="s">
-        <v>137</v>
+        <v>12</v>
+      </c>
+      <c r="H61" t="str">
+        <f>IF(D61="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>pass-through</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+        <v>pt_methods</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B62" t="s">
-        <v>370</v>
+        <v>136</v>
       </c>
       <c r="C62" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="D62" t="s">
         <v>30</v>
       </c>
       <c r="E62" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
@@ -4101,26 +4113,26 @@
         <v>31</v>
       </c>
       <c r="H62" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, single-output</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="6"/>
-        <v>siso_methods</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>370</v>
       </c>
       <c r="C63" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D63" t="s">
         <v>30</v>
@@ -4135,7 +4147,7 @@
         <v>31</v>
       </c>
       <c r="H63" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="5"/>
@@ -4146,99 +4158,98 @@
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>492</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
-        <v>493</v>
+        <v>141</v>
       </c>
       <c r="C64" t="s">
-        <v>494</v>
+        <v>425</v>
       </c>
       <c r="D64" t="s">
         <v>30</v>
       </c>
       <c r="E64" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H64" t="s">
-        <v>495</v>
+        <v>142</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" si="5"/>
-        <v>reactive single-inlet, double-outlet</v>
+        <v>single-input, single-output</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="6"/>
-        <v>sidor_methods</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+        <v>siso_methods</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>492</v>
       </c>
       <c r="B65" t="s">
-        <v>144</v>
+        <v>493</v>
       </c>
       <c r="C65" t="s">
-        <v>444</v>
+        <v>494</v>
       </c>
       <c r="D65" t="s">
         <v>30</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>145</v>
+        <v>495</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>reactive single-inlet, double-outlet</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sidor_methods</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B66" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s">
-        <v>408</v>
+        <v>444</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E66" t="s">
         <v>11</v>
       </c>
       <c r="F66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>12</v>
-      </c>
-      <c r="H66" t="str">
-        <f>IF(D66="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+        <v>31</v>
+      </c>
+      <c r="H66" t="s">
+        <v>145</v>
       </c>
       <c r="I66" t="str">
         <f t="shared" si="5"/>
@@ -4249,65 +4260,65 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C67" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="D67" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E67" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>31</v>
-      </c>
-      <c r="H67" t="s">
-        <v>150</v>
+        <v>12</v>
+      </c>
+      <c r="H67" t="str">
+        <f>IF(D67="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" si="5"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J67" t="str">
         <f t="shared" si="6"/>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B68" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C68" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E68" t="s">
         <v>27</v>
       </c>
       <c r="F68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>12</v>
-      </c>
-      <c r="H68" t="str">
-        <f>IF(D68="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+        <v>31</v>
+      </c>
+      <c r="H68" t="s">
+        <v>150</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" si="5"/>
@@ -4318,21 +4329,21 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B69" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C69" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F69" t="b">
         <v>1</v>
@@ -4346,25 +4357,25 @@
       </c>
       <c r="I69" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>pass-through</v>
       </c>
       <c r="J69" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+        <v>pt_methods</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B70" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C70" t="s">
-        <v>448</v>
+        <v>410</v>
       </c>
       <c r="D70" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="E70" t="s">
         <v>11</v>
@@ -4375,8 +4386,9 @@
       <c r="G70" t="s">
         <v>12</v>
       </c>
-      <c r="H70" t="s">
-        <v>65</v>
+      <c r="H70" t="str">
+        <f>IF(D70="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="5"/>
@@ -4387,18 +4399,18 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B71" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C71" t="s">
-        <v>411</v>
+        <v>448</v>
       </c>
       <c r="D71" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="E71" t="s">
         <v>11</v>
@@ -4410,7 +4422,7 @@
         <v>12</v>
       </c>
       <c r="H71" t="s">
-        <v>159</v>
+        <v>65</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="5"/>
@@ -4421,18 +4433,18 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B72" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E72" t="s">
         <v>11</v>
@@ -4443,9 +4455,8 @@
       <c r="G72" t="s">
         <v>12</v>
       </c>
-      <c r="H72" t="str">
-        <f>IF(D72="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+      <c r="H72" t="s">
+        <v>159</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="5"/>
@@ -4456,15 +4467,15 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B73" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C73" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="D73" t="s">
         <v>10</v>
@@ -4491,21 +4502,21 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B74" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C74" t="s">
-        <v>413</v>
+        <v>436</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
       </c>
       <c r="E74" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F74" t="b">
         <v>1</v>
@@ -4519,22 +4530,22 @@
       </c>
       <c r="I74" t="str">
         <f t="shared" si="5"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="6"/>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B75" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C75" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
@@ -4561,18 +4572,18 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B76" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C76" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="D76" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E76" t="s">
         <v>27</v>
@@ -4583,8 +4594,9 @@
       <c r="G76" t="s">
         <v>12</v>
       </c>
-      <c r="H76" t="s">
-        <v>170</v>
+      <c r="H76" t="str">
+        <f>IF(D76="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="5"/>
@@ -4595,18 +4607,18 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>496</v>
+        <v>168</v>
       </c>
       <c r="B77" t="s">
-        <v>497</v>
+        <v>169</v>
       </c>
       <c r="C77" t="s">
-        <v>498</v>
+        <v>431</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E77" t="s">
         <v>27</v>
@@ -4618,7 +4630,7 @@
         <v>12</v>
       </c>
       <c r="H77" t="s">
-        <v>499</v>
+        <v>170</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="5"/>
@@ -4629,21 +4641,21 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B78" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C78" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="D78" t="s">
         <v>10</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F78" t="b">
         <v>1</v>
@@ -4652,41 +4664,41 @@
         <v>12</v>
       </c>
       <c r="H78" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="I78" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>pass-through</v>
       </c>
       <c r="J78" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+        <v>pt_methods</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B79" t="s">
-        <v>457</v>
+        <v>501</v>
       </c>
       <c r="C79" t="s">
-        <v>453</v>
+        <v>502</v>
       </c>
       <c r="D79" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E79" t="s">
         <v>11</v>
       </c>
       <c r="F79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H79" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="5"/>
@@ -4697,52 +4709,52 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>171</v>
+        <v>504</v>
       </c>
       <c r="B80" t="s">
-        <v>172</v>
+        <v>457</v>
       </c>
       <c r="C80" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="D80" t="s">
         <v>30</v>
       </c>
       <c r="E80" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H80" t="s">
-        <v>173</v>
+        <v>505</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" si="5"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J80" t="str">
         <f t="shared" si="6"/>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B81" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C81" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E81" t="s">
         <v>27</v>
@@ -4753,9 +4765,8 @@
       <c r="G81" t="s">
         <v>21</v>
       </c>
-      <c r="H81" t="str">
-        <f>IF(D81="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+      <c r="H81" t="s">
+        <v>173</v>
       </c>
       <c r="I81" t="str">
         <f t="shared" si="5"/>
@@ -4766,15 +4777,15 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B82" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C82" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
@@ -4786,7 +4797,7 @@
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H82" t="str">
         <f>IF(D82="basic","cost_power_law_flow")</f>
@@ -4801,21 +4812,21 @@
         <v>pt_methods</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C83" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F83" t="b">
         <v>1</v>
@@ -4829,22 +4840,22 @@
       </c>
       <c r="I83" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>pass-through</v>
       </c>
       <c r="J83" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+        <v>pt_methods</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B84" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C84" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D84" t="s">
         <v>10</v>
@@ -4871,21 +4882,21 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B85" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C85" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D85" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E85" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F85" t="b">
         <v>1</v>
@@ -4893,27 +4904,28 @@
       <c r="G85" t="s">
         <v>12</v>
       </c>
-      <c r="H85" t="s">
-        <v>184</v>
+      <c r="H85" t="str">
+        <f>IF(D85="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I85" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, single-output</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J85" t="str">
         <f t="shared" si="6"/>
-        <v>siso_methods</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B86" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C86" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D86" t="s">
         <v>30</v>
@@ -4928,7 +4940,7 @@
         <v>12</v>
       </c>
       <c r="H86" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I86" t="str">
         <f t="shared" si="5"/>
@@ -4939,21 +4951,21 @@
         <v>siso_methods</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C87" t="s">
-        <v>454</v>
+        <v>418</v>
       </c>
       <c r="D87" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F87" t="b">
         <v>1</v>
@@ -4962,29 +4974,29 @@
         <v>12</v>
       </c>
       <c r="H87" t="s">
-        <v>461</v>
+        <v>187</v>
       </c>
       <c r="I87" t="str">
         <f t="shared" si="5"/>
-        <v>single-input, double-output</v>
+        <v>single-input, single-output</v>
       </c>
       <c r="J87" t="str">
         <f t="shared" si="6"/>
-        <v>sido_methods</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+        <v>siso_methods</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B88" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C88" t="s">
-        <v>421</v>
+        <v>454</v>
       </c>
       <c r="D88" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="E88" t="s">
         <v>11</v>
@@ -4995,9 +5007,8 @@
       <c r="G88" t="s">
         <v>12</v>
       </c>
-      <c r="H88" t="str">
-        <f>IF(D88="basic","cost_power_law_flow")</f>
-        <v>cost_power_law_flow</v>
+      <c r="H88" t="s">
+        <v>461</v>
       </c>
       <c r="I88" t="str">
         <f t="shared" si="5"/>
@@ -5008,15 +5019,15 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B89" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C89" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
@@ -5043,49 +5054,50 @@
         <v>sido_methods</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B90" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C90" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="D90" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E90" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>31</v>
-      </c>
-      <c r="H90" t="s">
-        <v>65</v>
+        <v>12</v>
+      </c>
+      <c r="H90" t="str">
+        <f>IF(D90="basic","cost_power_law_flow")</f>
+        <v>cost_power_law_flow</v>
       </c>
       <c r="I90" t="str">
         <f t="shared" si="5"/>
-        <v>pass-through</v>
+        <v>single-input, double-output</v>
       </c>
       <c r="J90" t="str">
         <f t="shared" si="6"/>
-        <v>pt_methods</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+        <v>sido_methods</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B91" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C91" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D91" t="s">
         <v>30</v>
@@ -5094,13 +5106,13 @@
         <v>27</v>
       </c>
       <c r="F91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H91" t="s">
-        <v>198</v>
+        <v>65</v>
       </c>
       <c r="I91" t="str">
         <f t="shared" si="5"/>
@@ -5111,9 +5123,43 @@
         <v>pt_methods</v>
       </c>
     </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>196</v>
+      </c>
+      <c r="B92" t="s">
+        <v>197</v>
+      </c>
+      <c r="C92" t="s">
+        <v>440</v>
+      </c>
+      <c r="D92" t="s">
+        <v>30</v>
+      </c>
+      <c r="E92" t="s">
+        <v>27</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+      <c r="G92" t="s">
+        <v>21</v>
+      </c>
+      <c r="H92" t="s">
+        <v>198</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="5"/>
+        <v>pass-through</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="6"/>
+        <v>pt_methods</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J91">
-    <sortCondition ref="B2:B91"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J92">
+    <sortCondition ref="B2:B92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5128,14 +5174,14 @@
       <selection activeCell="G77" sqref="G1:G77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.53125" customWidth="1"/>
+    <col min="3" max="3" width="31.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>199</v>
       </c>
@@ -5154,7 +5200,7 @@
         <v>aeration basin</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>202</v>
       </c>
@@ -5173,7 +5219,7 @@
         <v>air flotation</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>205</v>
       </c>
@@ -5195,7 +5241,7 @@
         <v>anaerobic digestion</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>209</v>
       </c>
@@ -5217,7 +5263,7 @@
         <v>anaerobic mbr mec</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>212</v>
       </c>
@@ -5239,7 +5285,7 @@
         <v>backwash solids handling</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>216</v>
       </c>
@@ -5261,7 +5307,7 @@
         <v>bio active filtration</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -5277,7 +5323,7 @@
         <v xml:space="preserve">bioreactor </v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>221</v>
       </c>
@@ -5296,7 +5342,7 @@
         <v>blending resevoir</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>224</v>
       </c>
@@ -5315,7 +5361,7 @@
         <v>brine concentrator</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>227</v>
       </c>
@@ -5334,7 +5380,7 @@
         <v>buffer tank</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>230</v>
       </c>
@@ -5350,7 +5396,7 @@
         <v xml:space="preserve">CANDOP </v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>231</v>
       </c>
@@ -5369,7 +5415,7 @@
         <v>cartridge filtration</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>233</v>
       </c>
@@ -5388,7 +5434,7 @@
         <v>chemical addition</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>236</v>
       </c>
@@ -5404,7 +5450,7 @@
         <v xml:space="preserve">chlorination </v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>237</v>
       </c>
@@ -5420,7 +5466,7 @@
         <v xml:space="preserve">clarifier </v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>238</v>
       </c>
@@ -5439,7 +5485,7 @@
         <v>co2 addition</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>240</v>
       </c>
@@ -5461,7 +5507,7 @@
         <v>coag and floc</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>244</v>
       </c>
@@ -5477,7 +5523,7 @@
         <v xml:space="preserve">cofermentation  </v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>245</v>
       </c>
@@ -5496,7 +5542,7 @@
         <v xml:space="preserve">constructed wetlands </v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>248</v>
       </c>
@@ -5518,7 +5564,7 @@
         <v>conventional activated sludge</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>252</v>
       </c>
@@ -5537,7 +5583,7 @@
         <v xml:space="preserve">cooling supply </v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>255</v>
       </c>
@@ -5556,7 +5602,7 @@
         <v xml:space="preserve">cooling tower </v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>257</v>
       </c>
@@ -5572,7 +5618,7 @@
         <v xml:space="preserve">decarbonator </v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>258</v>
       </c>
@@ -5594,7 +5640,7 @@
         <v>deep well injection</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>262</v>
       </c>
@@ -5616,7 +5662,7 @@
         <v>dissolved air flotation</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>264</v>
       </c>
@@ -5632,7 +5678,7 @@
         <v xml:space="preserve">dmbr </v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>265</v>
       </c>
@@ -5654,7 +5700,7 @@
         <v>dual media filtration</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>268</v>
       </c>
@@ -5676,7 +5722,7 @@
         <v>electrochemical nutrient removal</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>272</v>
       </c>
@@ -5695,7 +5741,7 @@
         <v>electrodialysis reversal</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>275</v>
       </c>
@@ -5714,7 +5760,7 @@
         <v>energy recovery</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>277</v>
       </c>
@@ -5733,7 +5779,7 @@
         <v>evaporation pond</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>280</v>
       </c>
@@ -5755,7 +5801,7 @@
         <v>feed water tank</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>281</v>
       </c>
@@ -5771,7 +5817,7 @@
         <v xml:space="preserve">feed </v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>283</v>
       </c>
@@ -5790,7 +5836,7 @@
         <v>filter press</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>286</v>
       </c>
@@ -5809,7 +5855,7 @@
         <v>fixed bed</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>289</v>
       </c>
@@ -5825,7 +5871,7 @@
         <v xml:space="preserve">gac </v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>290</v>
       </c>
@@ -5847,7 +5893,7 @@
         <v>gas sparged membrane</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>294</v>
       </c>
@@ -5869,7 +5915,7 @@
         <v>injection well disposal</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>296</v>
       </c>
@@ -5888,7 +5934,7 @@
         <v>intrusion mitigation</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>299</v>
       </c>
@@ -5907,7 +5953,7 @@
         <v>ion exchange</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>302</v>
       </c>
@@ -5932,7 +5978,7 @@
         <v>iron and manganese removal</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>305</v>
       </c>
@@ -5948,7 +5994,7 @@
         <v xml:space="preserve">landfill </v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>306</v>
       </c>
@@ -5964,7 +6010,7 @@
         <v xml:space="preserve">mabr </v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>210</v>
       </c>
@@ -5980,7 +6026,7 @@
         <v xml:space="preserve">mbr </v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>307</v>
       </c>
@@ -5999,7 +6045,7 @@
         <v>media filtration</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>308</v>
       </c>
@@ -6015,7 +6061,7 @@
         <v xml:space="preserve">metab </v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>309</v>
       </c>
@@ -6031,7 +6077,7 @@
         <v xml:space="preserve">microfiltration </v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>310</v>
       </c>
@@ -6050,7 +6096,7 @@
         <v>microscreen filtration</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>312</v>
       </c>
@@ -6069,7 +6115,7 @@
         <v>municipal drinking</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>315</v>
       </c>
@@ -6088,7 +6134,7 @@
         <v>municipal wwtp</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -6104,7 +6150,7 @@
         <v xml:space="preserve">nanofiltration </v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>318</v>
       </c>
@@ -6123,7 +6169,7 @@
         <v xml:space="preserve">ozone aop </v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>319</v>
       </c>
@@ -6139,7 +6185,7 @@
         <v xml:space="preserve">ozone </v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>321</v>
       </c>
@@ -6158,7 +6204,7 @@
         <v>photothermal membrane</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>323</v>
       </c>
@@ -6177,7 +6223,7 @@
         <v>primary separator</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>21</v>
       </c>
@@ -6196,7 +6242,7 @@
         <v>pump electricity</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>326</v>
       </c>
@@ -6212,7 +6258,7 @@
         <v xml:space="preserve">pump </v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>328</v>
       </c>
@@ -6228,7 +6274,7 @@
         <v xml:space="preserve">screen </v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>329</v>
       </c>
@@ -6250,7 +6296,7 @@
         <v>secondary treatment wwtp</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>332</v>
       </c>
@@ -6266,7 +6312,7 @@
         <v xml:space="preserve">sedimentation </v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>333</v>
       </c>
@@ -6285,7 +6331,7 @@
         <v>settling pond</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>335</v>
       </c>
@@ -6304,7 +6350,7 @@
         <v>sludge tank</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>336</v>
       </c>
@@ -6320,7 +6366,7 @@
         <v xml:space="preserve">smp </v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>337</v>
       </c>
@@ -6339,7 +6385,7 @@
         <v>static mixer</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>340</v>
       </c>
@@ -6358,7 +6404,7 @@
         <v>storage tank</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>342</v>
       </c>
@@ -6377,7 +6423,7 @@
         <v>surface discharge</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>345</v>
       </c>
@@ -6399,7 +6445,7 @@
         <v>sw onshore intake</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>349</v>
       </c>
@@ -6421,7 +6467,7 @@
         <v>tramp oil tank</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>352</v>
       </c>
@@ -6443,7 +6489,7 @@
         <v>tri media filtration</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>354</v>
       </c>
@@ -6462,7 +6508,7 @@
         <v>ultra filtration</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>356</v>
       </c>
@@ -6481,7 +6527,7 @@
         <v>uv aop</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>357</v>
       </c>
@@ -6497,7 +6543,7 @@
         <v xml:space="preserve">uv </v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>359</v>
       </c>
@@ -6516,7 +6562,7 @@
         <v>vfa recovery</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>361</v>
       </c>
@@ -6532,7 +6578,7 @@
         <v xml:space="preserve">waiv </v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>362</v>
       </c>
@@ -6554,7 +6600,7 @@
         <v>walnut shell filter</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>365</v>
       </c>
@@ -6576,7 +6622,7 @@
         <v>water pumping station</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>368</v>
       </c>
@@ -6609,12 +6655,12 @@
       <selection activeCell="C1" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="37.21875" customWidth="1"/>
+    <col min="2" max="2" width="37.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -6622,7 +6668,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -6630,7 +6676,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -6638,7 +6684,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -6646,7 +6692,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>455</v>
       </c>
@@ -6654,7 +6700,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -6662,7 +6708,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -6670,7 +6716,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -6678,7 +6724,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>371</v>
       </c>
@@ -6686,7 +6732,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -6694,7 +6740,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -6702,7 +6748,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -6710,7 +6756,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -6718,7 +6764,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>41</v>
       </c>
@@ -6726,7 +6772,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>44</v>
       </c>
@@ -6734,7 +6780,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>47</v>
       </c>
@@ -6742,7 +6788,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>49</v>
       </c>
@@ -6750,7 +6796,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>51</v>
       </c>
@@ -6758,7 +6804,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>54</v>
       </c>
@@ -6766,7 +6812,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>56</v>
       </c>
@@ -6774,7 +6820,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>60</v>
       </c>
@@ -6782,7 +6828,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>62</v>
       </c>
@@ -6790,7 +6836,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>64</v>
       </c>
@@ -6798,7 +6844,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>67</v>
       </c>
@@ -6806,7 +6852,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>69</v>
       </c>
@@ -6814,7 +6860,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>72</v>
       </c>
@@ -6822,7 +6868,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>74</v>
       </c>
@@ -6830,7 +6876,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>77</v>
       </c>
@@ -6838,7 +6884,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>79</v>
       </c>
@@ -6846,7 +6892,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>82</v>
       </c>
@@ -6854,7 +6900,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>84</v>
       </c>
@@ -6862,7 +6908,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>86</v>
       </c>
@@ -6870,7 +6916,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>89</v>
       </c>
@@ -6878,7 +6924,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>91</v>
       </c>
@@ -6886,7 +6932,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>95</v>
       </c>
@@ -6894,7 +6940,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>98</v>
       </c>
@@ -6902,7 +6948,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>101</v>
       </c>
@@ -6910,7 +6956,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>103</v>
       </c>
@@ -6918,7 +6964,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>456</v>
       </c>
@@ -6926,7 +6972,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>105</v>
       </c>
@@ -6934,7 +6980,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>107</v>
       </c>
@@ -6942,7 +6988,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>109</v>
       </c>
@@ -6950,7 +6996,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>112</v>
       </c>
@@ -6958,7 +7004,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>115</v>
       </c>
@@ -6966,7 +7012,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>118</v>
       </c>
@@ -6974,7 +7020,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>121</v>
       </c>
@@ -6982,7 +7028,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
         <v>123</v>
       </c>
@@ -6990,7 +7036,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
         <v>125</v>
       </c>
@@ -6998,7 +7044,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>128</v>
       </c>
@@ -7006,7 +7052,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>130</v>
       </c>
@@ -7014,7 +7060,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
         <v>132</v>
       </c>
@@ -7022,7 +7068,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>134</v>
       </c>
@@ -7030,7 +7076,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
         <v>136</v>
       </c>
@@ -7038,7 +7084,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
         <v>370</v>
       </c>
@@ -7046,7 +7092,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
         <v>141</v>
       </c>
@@ -7054,7 +7100,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>144</v>
       </c>
@@ -7062,7 +7108,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>147</v>
       </c>
@@ -7070,7 +7116,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
         <v>149</v>
       </c>
@@ -7078,7 +7124,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
         <v>152</v>
       </c>
@@ -7086,7 +7132,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
         <v>154</v>
       </c>
@@ -7094,7 +7140,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>156</v>
       </c>
@@ -7102,7 +7148,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
         <v>158</v>
       </c>
@@ -7110,7 +7156,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
         <v>161</v>
       </c>
@@ -7118,7 +7164,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -7126,7 +7172,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
         <v>165</v>
       </c>
@@ -7134,7 +7180,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>167</v>
       </c>
@@ -7142,7 +7188,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
         <v>169</v>
       </c>
@@ -7150,7 +7196,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
         <v>457</v>
       </c>
@@ -7158,7 +7204,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
         <v>172</v>
       </c>
@@ -7166,7 +7212,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
         <v>175</v>
       </c>
@@ -7174,7 +7220,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
         <v>177</v>
       </c>
@@ -7182,7 +7228,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
         <v>179</v>
       </c>
@@ -7190,7 +7236,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
         <v>181</v>
       </c>
@@ -7198,7 +7244,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
         <v>183</v>
       </c>
@@ -7206,7 +7252,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
         <v>186</v>
       </c>
@@ -7214,7 +7260,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
         <v>189</v>
       </c>
@@ -7222,7 +7268,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
         <v>191</v>
       </c>
@@ -7230,7 +7276,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
         <v>193</v>
       </c>
@@ -7238,7 +7284,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
         <v>195</v>
       </c>
@@ -7246,7 +7292,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
         <v>197</v>
       </c>

</xml_diff>